<commit_message>
add checkbox for set zero point manually
</commit_message>
<xml_diff>
--- a/applications/VBA/_3д_1_Ц.xlsx
+++ b/applications/VBA/_3д_1_Ц.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" codeName="ЭтаКнига" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="300" yWindow="4530" windowWidth="14805" windowHeight="5745"/>
@@ -12,12 +12,12 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$1:$X$32</definedName>
   </definedNames>
-  <calcPr calcId="124519" iterate="1" iterateCount="1"/>
+  <calcPr calcId="125725" iterate="1" iterateCount="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>О</t>
   </si>
@@ -26,9 +26,6 @@
   </si>
   <si>
     <t>У</t>
-  </si>
-  <si>
-    <t>Линейность</t>
   </si>
   <si>
     <t>Разница</t>
@@ -70,37 +67,13 @@
     <t>£</t>
   </si>
   <si>
-    <t>НГД</t>
-  </si>
-  <si>
     <t>№</t>
   </si>
   <si>
-    <t>Х</t>
+    <t>COM2</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>З/R1</t>
-  </si>
-  <si>
-    <t>К/R3</t>
-  </si>
-  <si>
-    <t>R5</t>
-  </si>
-  <si>
-    <t>R[2|5]</t>
-  </si>
-  <si>
-    <t>Ж/R[2|3]</t>
-  </si>
-  <si>
-    <t>И/R[1|2]</t>
-  </si>
-  <si>
-    <t>COM3</t>
+    <t>COM9</t>
   </si>
 </sst>
 </file>
@@ -111,7 +84,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -339,6 +312,14 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -656,7 +637,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="163">
+  <cellXfs count="165">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1032,6 +1013,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2256,9 +2243,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="9.5949478026902763E-2"/>
-          <c:y val="3.0407576263407971E-2"/>
+          <c:y val="3.0407576263407978E-2"/>
           <c:w val="0.83101021525844065"/>
-          <c:h val="0.92240676091667229"/>
+          <c:h val="0.92240676091667206"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2321,28 +2308,28 @@
                   <c:v>12.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>15.48</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>14.19</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>12.799999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>11.85</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>10.459999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>9.5100000000000016</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>8.66</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>8.18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2418,19 +2405,19 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>8.18</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>7.740000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>7.2199999999999989</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>6.82</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>6.2299999999999969</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2494,31 +2481,31 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>6.2299999999999969</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>5.3500000000000014</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>4.509999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>3.4400000000000048</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>-0.35000000000000853</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>-2.2900000000000063</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>-3.2400000000000091</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>-4.0900000000000034</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>-4.5299999999999869</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2574,7 +2561,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>А</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2638,7 +2625,7 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>8.18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2670,7 +2657,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Б</c:v>
+                  <c:v>-3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2693,8 +2680,8 @@
               <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-7.7082901385847526E-3"/>
-                  <c:y val="-3.7230948225716771E-2"/>
+                  <c:x val="-7.7082901385847561E-3"/>
+                  <c:y val="-3.7230948225716799E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -2742,7 +2729,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>6.2299999999999969</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2774,7 +2761,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>В</c:v>
+                  <c:v>-4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2845,7 +2832,7 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>-4.5299999999999869</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3174,11 +3161,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:axId val="69835392"/>
-        <c:axId val="69853952"/>
+        <c:axId val="158775936"/>
+        <c:axId val="158786304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="69835392"/>
+        <c:axId val="158775936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3204,19 +3191,19 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.38193271256707251"/>
+              <c:x val="0.38193271256707262"/>
               <c:y val="0.95763807011034663"/>
             </c:manualLayout>
           </c:layout>
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69853952"/>
+        <c:tickLblPos val="none"/>
+        <c:crossAx val="158786304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="69853952"/>
+        <c:axId val="158786304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="240"/>
@@ -3254,7 +3241,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69835392"/>
+        <c:crossAx val="158775936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="12"/>
@@ -3779,7 +3766,7 @@
   <dimension ref="A1:AD49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScaleSheetLayoutView="110" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3805,34 +3792,34 @@
   <sheetData>
     <row r="1" spans="1:30" ht="14.25" customHeight="1" thickBot="1">
       <c r="A1" s="143" t="str">
-        <f>IF(B30=" ",IF((C8&gt;3)*(C8&lt;15),C8,IF(C8&gt;2000," ",A1)),IF(ABS(560-((B28-B30)*A4/(B28-B30+A4)+B30+(B29-B31)*A21/(B29-B31+A21)+B31)*3300/(((B28-B30)*A4/(B28-B30+A4)+B30+(B29-B31)*A21/(B29-B31+A21)+B31)+3300))&lt;ABS(560-((B28-B30)*A4/(B28-B30+A4)+B30+(B29-B31)*A21/(B29-B31+A21)+B31)*6800/(((B28-B30)*A4/(B28-B30+A4)+B30+(B29-B31)*A21/(B29-B31+A21)+B31)+6800)),3.3,IF(ABS(((B28-B30)*A4/(B28-B30+A4)+B30+(B29-B31)*A21/(B29-B31+A21)+B31)*6800/(((B28-B30)*A4/(B28-B30+A4)+B30+(B29-B31)*A21/(B29-B31+A21)+B31)+6800)-560)&lt;ABS(((B28-B30)*A4/(B28-B30+A4)+B30+(B29-B31)*A21/(B29-B31+A21)+B31)*12000/(((B28-B30)*A4/(B28-B30+A4)+B30+(B29-B31)*A21/(B29-B31+A21)+B31)+12000)-560),6.8,12)))</f>
+        <f ca="1">IF(B30=" ",IF((C8&gt;3)*(C8&lt;15),C8,IF(C8&gt;2000," ",A1)),IF(ABS(560-((B28-B30)*A4/(B28-B30+A4)+B30+(B29-B31)*A21/(B29-B31+A21)+B31)*3300/(((B28-B30)*A4/(B28-B30+A4)+B30+(B29-B31)*A21/(B29-B31+A21)+B31)+3300))&lt;ABS(560-((B28-B30)*A4/(B28-B30+A4)+B30+(B29-B31)*A21/(B29-B31+A21)+B31)*6800/(((B28-B30)*A4/(B28-B30+A4)+B30+(B29-B31)*A21/(B29-B31+A21)+B31)+6800)),3.3,IF(ABS(((B28-B30)*A4/(B28-B30+A4)+B30+(B29-B31)*A21/(B29-B31+A21)+B31)*6800/(((B28-B30)*A4/(B28-B30+A4)+B30+(B29-B31)*A21/(B29-B31+A21)+B31)+6800)-560)&lt;ABS(((B28-B30)*A4/(B28-B30+A4)+B30+(B29-B31)*A21/(B29-B31+A21)+B31)*12000/(((B28-B30)*A4/(B28-B30+A4)+B30+(B29-B31)*A21/(B29-B31+A21)+B31)+12000)-560),6.8,12)))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="B1" s="41" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C1" s="83"/>
       <c r="D1" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="82" t="s">
         <v>15</v>
-      </c>
-      <c r="E1" s="82" t="s">
-        <v>16</v>
       </c>
       <c r="F1" s="70" t="str">
         <f>IFERROR(IF(K12&lt;0.5,"Расчёт","Расчет"),"Расчёт")</f>
-        <v>Расчет</v>
+        <v>Расчёт</v>
       </c>
       <c r="G1" s="69" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="145" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="153"/>
-      <c r="J1" s="145" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="146"/>
+        <v>13</v>
+      </c>
+      <c r="H1" s="147" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="155"/>
+      <c r="J1" s="147">
+        <v>0</v>
+      </c>
+      <c r="K1" s="148"/>
       <c r="L1" s="8"/>
       <c r="M1" s="9"/>
       <c r="N1" s="8"/>
@@ -3849,7 +3836,7 @@
       <c r="Y1" s="8"/>
       <c r="Z1" s="8"/>
       <c r="AA1" s="144" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:30" ht="15.75" customHeight="1" thickBot="1">
@@ -3859,8 +3846,8 @@
       <c r="B2" s="20">
         <v>0</v>
       </c>
-      <c r="C2" s="53" t="s">
-        <v>7</v>
+      <c r="C2" s="53">
+        <v>4.05</v>
       </c>
       <c r="D2" s="89" t="str">
         <f ca="1">IFERROR(E27/D27,IF(B1="R",E27/C27," "))</f>
@@ -3870,12 +3857,12 @@
         <f>K3</f>
         <v>0</v>
       </c>
-      <c r="F2" s="58" t="str">
+      <c r="F2" s="58">
         <f>IF((C2&gt;2000)," ",C2*0)</f>
-        <v xml:space="preserve"> </v>
+        <v>0</v>
       </c>
       <c r="G2" s="106" t="str">
-        <f>IFERROR(100/C27," ")</f>
+        <f ca="1">IFERROR(100/C27," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H2" s="31">
@@ -3885,10 +3872,10 @@
         <v>0</v>
       </c>
       <c r="J2" s="57" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K2" s="81" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L2" s="8"/>
       <c r="M2" s="10">
@@ -3908,6 +3895,9 @@
       <c r="X2" s="8"/>
       <c r="Y2" s="8"/>
       <c r="Z2" s="8"/>
+      <c r="AA2" s="144" t="s">
+        <v>18</v>
+      </c>
       <c r="AC2" s="2">
         <v>0</v>
       </c>
@@ -3917,45 +3907,45 @@
     </row>
     <row r="3" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A3" s="78" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="32">
         <f t="shared" ref="B3:B8" si="0">B2+12</f>
         <v>12</v>
       </c>
-      <c r="C3" s="86" t="s">
-        <v>25</v>
+      <c r="C3" s="86">
+        <v>7.88</v>
       </c>
       <c r="D3" s="90" t="e">
         <f t="shared" ref="D3:D9" ca="1" si="1">((B3-$E$26*($E$2*94/($B$28-$B$30)))/(9.4-((9.4/($B$28-$B$30))*($E$2+$E$10)*$E$26)))*($B$28-$B$30+($E$26*E2))*(($D$2-($E$27/($A$1*1000)))-((((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))*($D$2-($E$27/($A$1*1000))))/$A$4))</f>
         <v>#VALUE!</v>
       </c>
       <c r="E3" s="71"/>
-      <c r="F3" s="59" t="e">
+      <c r="F3" s="59">
         <f t="shared" ref="F3:F9" si="2">(B3-$B$2)/($B$11-$B$2)*$C$11</f>
-        <v>#VALUE!</v>
+        <v>4.4399999999999995</v>
       </c>
       <c r="G3" s="93" t="e">
         <f ca="1">C3-D3</f>
         <v>#VALUE!</v>
       </c>
-      <c r="H3" s="36" t="e">
+      <c r="H3" s="36">
         <f>J3/F3</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I3" s="150" t="e">
+        <v>0.77477477477477497</v>
+      </c>
+      <c r="I3" s="152">
         <f>SUM(H3:H9)/9</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="J3" s="40" t="e">
+        <v>0.14950009533342867</v>
+      </c>
+      <c r="J3" s="40">
         <f t="shared" ref="J3:J9" si="3">ABS(C3-F3)</f>
-        <v>#VALUE!</v>
+        <v>3.4400000000000004</v>
       </c>
       <c r="K3" s="43"/>
       <c r="L3" s="8"/>
-      <c r="M3" s="12" t="e">
-        <f ca="1">IF((C3&gt;100)*((B1="№")+(B1="R"))+(B1="Т"),D3+AD3,C3+AD3)</f>
-        <v>#VALUE!</v>
+      <c r="M3" s="12">
+        <f>IF((C3&gt;100)*((B1="№")+(B1="R"))+(B1="Т"),D3+AD3,C3+AD3)</f>
+        <v>15.48</v>
       </c>
       <c r="N3" s="8"/>
       <c r="O3" s="13"/>
@@ -3970,6 +3960,9 @@
       <c r="X3" s="8"/>
       <c r="Y3" s="8"/>
       <c r="Z3" s="8"/>
+      <c r="AA3" s="144">
+        <v>50.53</v>
+      </c>
       <c r="AC3" s="1">
         <f t="shared" ref="AC3:AC8" si="4">AC2+12</f>
         <v>12</v>
@@ -3980,44 +3973,44 @@
       </c>
     </row>
     <row r="4" spans="1:30" ht="15" customHeight="1">
-      <c r="A4" s="159" t="str">
-        <f>IF(B30=" ",IF(C7&gt;2000," ",IF((C7&gt;200)*(C7&lt;400),C7,A4)),326.8)</f>
+      <c r="A4" s="161" t="str">
+        <f ca="1">IF(B30=" ",IF(C7&gt;2000," ",IF((C7&gt;200)*(C7&lt;400),C7,A4)),326.8)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="B4" s="33">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="C4" s="87" t="s">
-        <v>26</v>
+      <c r="C4" s="87">
+        <v>11.59</v>
       </c>
       <c r="D4" s="91" t="e">
         <f t="shared" ca="1" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="E4" s="72"/>
-      <c r="F4" s="60" t="e">
+      <c r="F4" s="60">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+        <v>8.879999999999999</v>
       </c>
       <c r="G4" s="91" t="e">
         <f t="shared" ref="G4:G24" ca="1" si="5">C4-D4</f>
         <v>#VALUE!</v>
       </c>
-      <c r="H4" s="37" t="e">
+      <c r="H4" s="37">
         <f t="shared" ref="H4:H25" si="6">J4/F4</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I4" s="150"/>
-      <c r="J4" s="77" t="e">
+        <v>0.30518018018018028</v>
+      </c>
+      <c r="I4" s="152"/>
+      <c r="J4" s="77">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v>2.7100000000000009</v>
       </c>
       <c r="K4" s="44"/>
       <c r="L4" s="8"/>
-      <c r="M4" s="12" t="e">
-        <f ca="1">IF((C4&gt;100)*((B1="№")+(B1="R"))+(B1="Т"),D4+AD4,C4+AD4)</f>
-        <v>#VALUE!</v>
+      <c r="M4" s="12">
+        <f>IF((C4&gt;100)*((B1="№")+(B1="R"))+(B1="Т"),D4+AD4,C4+AD4)</f>
+        <v>14.19</v>
       </c>
       <c r="N4" s="8"/>
       <c r="O4" s="13"/>
@@ -4032,6 +4025,9 @@
       <c r="X4" s="8"/>
       <c r="Y4" s="8"/>
       <c r="Z4" s="8"/>
+      <c r="AA4" s="144">
+        <v>126.37</v>
+      </c>
       <c r="AC4" s="1">
         <f t="shared" si="4"/>
         <v>24</v>
@@ -4042,44 +4038,44 @@
       </c>
     </row>
     <row r="5" spans="1:30" ht="15" customHeight="1">
-      <c r="A5" s="160"/>
+      <c r="A5" s="162"/>
       <c r="B5" s="34">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="C5" s="86" t="s">
-        <v>21</v>
+      <c r="C5" s="86">
+        <v>15.2</v>
       </c>
       <c r="D5" s="90" t="e">
         <f t="shared" ca="1" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="E5" s="71"/>
-      <c r="F5" s="59" t="e">
+      <c r="F5" s="59">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+        <v>13.32</v>
       </c>
       <c r="G5" s="93" t="e">
         <f t="shared" ca="1" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H5" s="36" t="e">
+      <c r="H5" s="36">
         <f t="shared" si="6"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I5" s="150"/>
-      <c r="J5" s="40" t="e">
+        <v>0.14114114114114107</v>
+      </c>
+      <c r="I5" s="152"/>
+      <c r="J5" s="40">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K5" s="151" t="str">
+        <v>1.879999999999999</v>
+      </c>
+      <c r="K5" s="153">
         <f>IFERROR(IF(MAX(J3:J9)&gt;10,"FAIL",MAX(J3:J9)),"∆ОА=")</f>
-        <v>∆ОА=</v>
+        <v>3.4400000000000004</v>
       </c>
       <c r="L5" s="8"/>
-      <c r="M5" s="12" t="e">
-        <f ca="1">IF((C5&gt;100)*((B1="№")+(B1="R"))+(B1="Т"),D5+AD5,C5+AD5)</f>
-        <v>#VALUE!</v>
+      <c r="M5" s="12">
+        <f>IF((C5&gt;100)*((B1="№")+(B1="R"))+(B1="Т"),D5+AD5,C5+AD5)</f>
+        <v>12.799999999999999</v>
       </c>
       <c r="N5" s="8"/>
       <c r="O5" s="13"/>
@@ -4094,6 +4090,7 @@
       <c r="X5" s="8"/>
       <c r="Y5" s="8"/>
       <c r="Z5" s="8"/>
+      <c r="AA5" s="144"/>
       <c r="AC5" s="1">
         <f t="shared" si="4"/>
         <v>36</v>
@@ -4104,41 +4101,41 @@
       </c>
     </row>
     <row r="6" spans="1:30" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A6" s="161"/>
+      <c r="A6" s="163"/>
       <c r="B6" s="33">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="C6" s="87" t="s">
-        <v>22</v>
+      <c r="C6" s="87">
+        <v>19.25</v>
       </c>
       <c r="D6" s="91" t="e">
         <f t="shared" ca="1" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="E6" s="72"/>
-      <c r="F6" s="60" t="e">
+      <c r="F6" s="60">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+        <v>17.759999999999998</v>
       </c>
       <c r="G6" s="91" t="e">
         <f t="shared" ca="1" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H6" s="37" t="e">
+      <c r="H6" s="37">
         <f t="shared" si="6"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I6" s="150"/>
-      <c r="J6" s="77" t="e">
+        <v>8.3896396396396511E-2</v>
+      </c>
+      <c r="I6" s="152"/>
+      <c r="J6" s="77">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K6" s="151"/>
+        <v>1.490000000000002</v>
+      </c>
+      <c r="K6" s="153"/>
       <c r="L6" s="14"/>
-      <c r="M6" s="12" t="e">
-        <f ca="1">IF(((C6&gt;100)+(C6&lt;5))*((B1="№")+(B1="R"))+(B1="Т"),D6+AD6,C6+AD6)</f>
-        <v>#VALUE!</v>
+      <c r="M6" s="12">
+        <f>IF(((C6&gt;100)+(C6&lt;5))*((B1="№")+(B1="R"))+(B1="Т"),D6+AD6,C6+AD6)</f>
+        <v>11.85</v>
       </c>
       <c r="N6" s="8"/>
       <c r="O6" s="13"/>
@@ -4153,6 +4150,7 @@
       <c r="X6" s="8"/>
       <c r="Y6" s="8"/>
       <c r="Z6" s="8"/>
+      <c r="AA6" s="144"/>
       <c r="AC6" s="1">
         <f t="shared" si="4"/>
         <v>48</v>
@@ -4163,44 +4161,44 @@
       </c>
     </row>
     <row r="7" spans="1:30" ht="15" customHeight="1">
-      <c r="A7" s="162" t="str">
-        <f>IF((C27=" ")+(B30=" "),IF((C3&gt;200)*(C3&lt;400),C3,IF(C3&gt;2000," ",A7)),((((B28-B30)*A4/(B28-B30+A4))+B30)*(A1*1000+((B29-B31)*A21/((B29-B31)+A21))+B31))/((((B28-B30)*A4/((B28-B30)+A4))+B30)+A1*1000+((B29-B31)*A21/((B29-B31)+A21))+B31))</f>
+      <c r="A7" s="164" t="str">
+        <f ca="1">IF((C27=" ")+(B30=" "),IF((C3&gt;200)*(C3&lt;400),C3,IF(C3&gt;2000," ",A7)),((((B28-B30)*A4/(B28-B30+A4))+B30)*(A1*1000+((B29-B31)*A21/((B29-B31)+A21))+B31))/((((B28-B30)*A4/((B28-B30)+A4))+B30)+A1*1000+((B29-B31)*A21/((B29-B31)+A21))+B31))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="B7" s="34">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="C7" s="86" t="s">
-        <v>12</v>
+      <c r="C7" s="86">
+        <v>22.86</v>
       </c>
       <c r="D7" s="90" t="e">
         <f t="shared" ca="1" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="E7" s="71"/>
-      <c r="F7" s="59" t="e">
+      <c r="F7" s="59">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+        <v>22.200000000000003</v>
       </c>
       <c r="G7" s="93" t="e">
         <f t="shared" ca="1" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H7" s="36" t="e">
+      <c r="H7" s="36">
         <f t="shared" si="6"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I7" s="150"/>
-      <c r="J7" s="40" t="e">
+        <v>2.9729729729729572E-2</v>
+      </c>
+      <c r="I7" s="152"/>
+      <c r="J7" s="40">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K7" s="151"/>
+        <v>0.65999999999999659</v>
+      </c>
+      <c r="K7" s="153"/>
       <c r="L7" s="8"/>
-      <c r="M7" s="12" t="e">
-        <f ca="1">IF((C7&gt;100)*((B1="№")+(B1="R"))+(B1="Т"),D7+AD7,C7+AD7)</f>
-        <v>#VALUE!</v>
+      <c r="M7" s="12">
+        <f>IF((C7&gt;100)*((B1="№")+(B1="R"))+(B1="Т"),D7+AD7,C7+AD7)</f>
+        <v>10.459999999999999</v>
       </c>
       <c r="N7" s="8"/>
       <c r="O7" s="13"/>
@@ -4225,41 +4223,41 @@
       </c>
     </row>
     <row r="8" spans="1:30" ht="15" customHeight="1">
-      <c r="A8" s="162"/>
+      <c r="A8" s="164"/>
       <c r="B8" s="33">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
-      <c r="C8" s="87" t="s">
-        <v>23</v>
+      <c r="C8" s="87">
+        <v>26.91</v>
       </c>
       <c r="D8" s="91" t="e">
         <f t="shared" ca="1" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="E8" s="72"/>
-      <c r="F8" s="60" t="e">
+      <c r="F8" s="60">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+        <v>26.64</v>
       </c>
       <c r="G8" s="91" t="e">
         <f t="shared" ca="1" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H8" s="37" t="e">
+      <c r="H8" s="37">
         <f t="shared" si="6"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I8" s="150"/>
-      <c r="J8" s="77" t="e">
+        <v>1.0135135135135118E-2</v>
+      </c>
+      <c r="I8" s="152"/>
+      <c r="J8" s="77">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v>0.26999999999999957</v>
       </c>
       <c r="K8" s="44"/>
       <c r="L8" s="8"/>
-      <c r="M8" s="12" t="e">
-        <f ca="1">IF(((C8&gt;100)+(C8&lt;15))*((B1="№")+(B1="R"))+(B1="Т"),D8+AD8,C8+AD8)</f>
-        <v>#VALUE!</v>
+      <c r="M8" s="12">
+        <f>IF(((C8&gt;100)+(C8&lt;15))*((B1="№")+(B1="R"))+(B1="Т"),D8+AD8,C8+AD8)</f>
+        <v>9.5100000000000016</v>
       </c>
       <c r="N8" s="8"/>
       <c r="O8" s="13"/>
@@ -4284,41 +4282,41 @@
       </c>
     </row>
     <row r="9" spans="1:30" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A9" s="162"/>
+      <c r="A9" s="164"/>
       <c r="B9" s="35">
         <f>B8+12</f>
         <v>84</v>
       </c>
-      <c r="C9" s="88" t="s">
-        <v>24</v>
+      <c r="C9" s="88">
+        <v>31.06</v>
       </c>
       <c r="D9" s="90" t="e">
         <f t="shared" ca="1" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="E9" s="71"/>
-      <c r="F9" s="59" t="e">
+      <c r="F9" s="59">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+        <v>31.08</v>
       </c>
       <c r="G9" s="93" t="e">
         <f t="shared" ca="1" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H9" s="36" t="e">
+      <c r="H9" s="36">
         <f t="shared" si="6"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I9" s="150"/>
-      <c r="J9" s="40" t="e">
+        <v>6.4350064350062982E-4</v>
+      </c>
+      <c r="I9" s="152"/>
+      <c r="J9" s="40">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v>1.9999999999999574E-2</v>
       </c>
       <c r="K9" s="44"/>
       <c r="L9" s="8"/>
-      <c r="M9" s="12" t="e">
-        <f ca="1">IF(((C9&gt;100)+(C9&lt;5))*((B1="№")+(B1="R"))+(B1="Т"),D9+AD9,C9+AD9)</f>
-        <v>#VALUE!</v>
+      <c r="M9" s="12">
+        <f>IF(((C9&gt;100)+(C9&lt;5))*((B1="№")+(B1="R"))+(B1="Т"),D9+AD9,C9+AD9)</f>
+        <v>8.66</v>
       </c>
       <c r="N9" s="8"/>
       <c r="O9" s="13"/>
@@ -4345,9 +4343,9 @@
     <row r="10" spans="1:30" ht="15.75" hidden="1" customHeight="1" thickBot="1">
       <c r="A10" s="50"/>
       <c r="B10" s="61"/>
-      <c r="C10" s="62" t="str">
+      <c r="C10" s="62">
         <f>IF($B$11=94,$C$11,$C$10)</f>
-        <v xml:space="preserve"> </v>
+        <v>34.78</v>
       </c>
       <c r="D10" s="131" t="e">
         <f ca="1">(((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))*($D$2-($E$27/($A$1*1000))))*10</f>
@@ -4384,50 +4382,50 @@
       <c r="AC10" s="1"/>
     </row>
     <row r="11" spans="1:30" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A11" s="47" t="str">
+      <c r="A11" s="47">
         <f>IFERROR(IF((K5&gt;K11)+(K12&gt;K17),IF((K5-K11)&gt;(K12-K17),IF(SUM(F3:F9)&lt;SUM(C3:C9),IF((K5-K11)*5&lt;1,1,IF((K5-K11)*5&gt;3,3,(K5-K11)*5)),IF((K5-K11)*5&lt;1,-1,IF((K5-K11)*5&gt;3,-3,-(K5-K11)*5))),IF(SUM(F12:F15)&lt;SUM(C12:C15),IF((K12-K17)*5&lt;1,-1,IF((K12-K17)*5&gt;3,-3,-(K12-K17)*5)),IF((K12-K17)*5&lt;1,1,IF((K12-K17)*5&gt;3,3,(K12-K17)*5)))),"А"),"А")</f>
-        <v>А</v>
+        <v>3</v>
       </c>
       <c r="B11" s="20">
         <v>94</v>
       </c>
-      <c r="C11" s="53" t="s">
-        <v>20</v>
+      <c r="C11" s="53">
+        <v>34.78</v>
       </c>
       <c r="D11" s="123" t="str">
-        <f>IFERROR(IF((B11-$E$26*($E$2*94/($B$28-$B$30)))&gt;94,((B11-$E$26*($E$2*94/($B$28-$B$30)))-94)/(2.4-(2.4*$E$26*($E$11+$E$13)/$B$30))*($B$30+$E$11*$E$26)*($D$2-($E$27/($A$1*1000)))+(((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))*($D$2-($E$27/($A$1*1000))))*10,(((B11-$E$26*($E$2*94/($B$28-$B$30)))/(9.4-((9.4/($B$28-$B$30))*($E$2+$E$10)*$E$26)))*($B$28-$B$30+($E$26*E9))*(($D$2-($E$27/($A$1*1000)))-((((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))*($D$2-($E$27/($A$1*1000))))/$A$4))))," ")</f>
+        <f ca="1">IFERROR(IF((B11-$E$26*($E$2*94/($B$28-$B$30)))&gt;94,((B11-$E$26*($E$2*94/($B$28-$B$30)))-94)/(2.4-(2.4*$E$26*($E$11+$E$13)/$B$30))*($B$30+$E$11*$E$26)*($D$2-($E$27/($A$1*1000)))+(((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))*($D$2-($E$27/($A$1*1000))))*10,(((B11-$E$26*($E$2*94/($B$28-$B$30)))/(9.4-((9.4/($B$28-$B$30))*($E$2+$E$10)*$E$26)))*($B$28-$B$30+($E$26*E9))*(($D$2-($E$27/($A$1*1000)))-((((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))*($D$2-($E$27/($A$1*1000))))/$A$4))))," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E11" s="116">
         <f>K9</f>
         <v>0</v>
       </c>
-      <c r="F11" s="58" t="str">
+      <c r="F11" s="58">
         <f>IF(C11=" "," ",C11)</f>
+        <v>34.78</v>
+      </c>
+      <c r="G11" s="92" t="str">
+        <f ca="1">IFERROR(C11-D11," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="G11" s="92" t="str">
-        <f>IFERROR(C11-D11," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H11" s="38" t="e">
+      <c r="H11" s="38">
         <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+        <v>0</v>
       </c>
       <c r="I11" s="30">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="J11" s="39" t="str">
+      <c r="J11" s="39">
         <f>IF(F11=" "," ",IF(B1=7,(IF(($C$10&gt;(((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))*($D$2-($E$27/($A$1*1000))))*10),(94-((2.4*($C$10-((((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))*($D$2-($E$27/($A$1*1000))))*10)))/($D$30*($D$2-($E$27/($A$1*1000)))))),(94-(9.4*($C$10-((((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))*($D$2-($E$27/($A$1*1000))))*10)))/(($D$28-$D$30)*(($D$2-($E$27/($A$1*1000)))-((((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))*($D$2-($E$27/($A$1*1000))))/$A$4)))))),0))</f>
-        <v xml:space="preserve"> </v>
+        <v>0</v>
       </c>
       <c r="K11" s="80">
         <v>0.4</v>
       </c>
       <c r="L11" s="8"/>
-      <c r="M11" s="10" t="e">
+      <c r="M11" s="10">
         <f>IF((C11&gt;100)*(B1="№")+(B1="Т"),D11+AD15,IF(B11=AC11,C11+AD11,IF(B11=AC12,C11+AD12,IF(B11=AC14,C11+AD14,IF(B11=AC15,C11+AD15,IF(B11=AC17,C11+AD17,IF(B11=AC18,C11+AD18,IF(B11=AC19,C11+AD19,"ошибка"))))))))</f>
-        <v>#VALUE!</v>
+        <v>8.18</v>
       </c>
       <c r="N11" s="8"/>
       <c r="O11" s="11"/>
@@ -4451,49 +4449,49 @@
       </c>
     </row>
     <row r="12" spans="1:30" ht="15" customHeight="1">
-      <c r="A12" s="158" t="str">
-        <f>IF((A7=" ")+(A18=" ")," ",ABS(A7-A18))</f>
+      <c r="A12" s="160" t="str">
+        <f ca="1">IF((A7=" ")+(A18=" ")," ",ABS(A7-A18))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="B12" s="18">
         <v>108</v>
       </c>
-      <c r="C12" s="55" t="s">
-        <v>20</v>
+      <c r="C12" s="55">
+        <v>40.14</v>
       </c>
       <c r="D12" s="124" t="e">
         <f ca="1">((B12-$E$26*($E$2*94/($B$28-$B$30)))-94)/(2.4-(2.4*$E$26*($E$11+$E$13)/$B$30))*($B$30+$E$11*$E$26)*($D$2-($E$27/($A$1*1000)))+(((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))*($D$2-($E$27/($A$1*1000))))*10</f>
         <v>#VALUE!</v>
       </c>
       <c r="E12" s="74"/>
-      <c r="F12" s="59" t="e">
+      <c r="F12" s="59">
         <f t="shared" ref="F12:F15" si="8">(B12-$B$11)/($B$17-$B$11)*($C$17-$C$11)+$C$11</f>
-        <v>#VALUE!</v>
+        <v>40.044583333333335</v>
       </c>
       <c r="G12" s="93" t="e">
         <f t="shared" ca="1" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H12" s="36" t="e">
+      <c r="H12" s="36">
         <f t="shared" si="6"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I12" s="150" t="e">
+        <v>2.3827608811012348E-3</v>
+      </c>
+      <c r="I12" s="152">
         <f>SUM(H12,H14,H15)/5</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="J12" s="40" t="e">
+        <v>1.3720364152971093E-3</v>
+      </c>
+      <c r="J12" s="40">
         <f>ABS(C12-F12)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K12" s="152" t="str">
+        <v>9.5416666666665151E-2</v>
+      </c>
+      <c r="K12" s="154">
         <f>IFERROR(IF(MAX(J12:J15)&gt;10,"FAIL",MAX(J12:J15)),"∆АБ=")</f>
-        <v>∆АБ=</v>
+        <v>0.15041666666666487</v>
       </c>
       <c r="L12" s="8"/>
-      <c r="M12" s="12" t="e">
-        <f ca="1">IF((C12&gt;100)*(B1="№")+(B1="Т"),D12+AD20,C12+AD20)</f>
-        <v>#VALUE!</v>
+      <c r="M12" s="12">
+        <f>IF((C12&gt;100)*(B1="№")+(B1="Т"),D12+AD20,C12+AD20)</f>
+        <v>7.740000000000002</v>
       </c>
       <c r="N12" s="8"/>
       <c r="O12" s="13"/>
@@ -4517,7 +4515,7 @@
       </c>
     </row>
     <row r="13" spans="1:30" ht="15" hidden="1" customHeight="1">
-      <c r="A13" s="158"/>
+      <c r="A13" s="160"/>
       <c r="B13" s="67"/>
       <c r="C13" s="62"/>
       <c r="D13" s="94" t="e">
@@ -4534,12 +4532,12 @@
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I13" s="150"/>
+      <c r="I13" s="152"/>
       <c r="J13" s="68">
         <f>ABS(C13-F13)</f>
         <v>0</v>
       </c>
-      <c r="K13" s="151"/>
+      <c r="K13" s="153"/>
       <c r="L13" s="8"/>
       <c r="M13" s="12"/>
       <c r="N13" s="8"/>
@@ -4559,43 +4557,43 @@
       <c r="AD13" s="4"/>
     </row>
     <row r="14" spans="1:30" ht="15" customHeight="1">
-      <c r="A14" s="158"/>
+      <c r="A14" s="160"/>
       <c r="B14" s="19">
         <v>120</v>
       </c>
-      <c r="C14" s="56" t="s">
-        <v>20</v>
+      <c r="C14" s="56">
+        <v>44.62</v>
       </c>
       <c r="D14" s="91" t="e">
-        <f>IF((B14-$E$26*($E$2*94/($B$28-$B$30)))&gt;118,((B14-$E$26*($E$2*94/($B$28-$B$30)))-118)/(2.4-(2.4*$E$26*($E$14+$E$16)/$B$31))*($B$31+E14*$E$26)*($D$2-($E$27/($A$1*1000)))+((((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))*($D$2-($E$27/($A$1*1000))))+$D$30*($D$2-($E$27/($A$1*1000))))*10,((B14-$E$26*($E$2*94/($B$28-$B$30)))-94)/(2.4-(2.4*$E$26*($E$11+$E$13)/$B$30))*($B$30+$E$12*$E$26)*($D$2-($E$27/($A$1*1000)))+(((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))*($D$2-($E$27/($A$1*1000))))*10)</f>
+        <f ca="1">IF((B14-$E$26*($E$2*94/($B$28-$B$30)))&gt;118,((B14-$E$26*($E$2*94/($B$28-$B$30)))-118)/(2.4-(2.4*$E$26*($E$14+$E$16)/$B$31))*($B$31+E14*$E$26)*($D$2-($E$27/($A$1*1000)))+((((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))*($D$2-($E$27/($A$1*1000))))+$D$30*($D$2-($E$27/($A$1*1000))))*10,((B14-$E$26*($E$2*94/($B$28-$B$30)))-94)/(2.4-(2.4*$E$26*($E$11+$E$13)/$B$30))*($B$30+$E$12*$E$26)*($D$2-($E$27/($A$1*1000)))+(((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))*($D$2-($E$27/($A$1*1000))))*10)</f>
         <v>#VALUE!</v>
       </c>
       <c r="E14" s="118">
         <f>K19</f>
         <v>0</v>
       </c>
-      <c r="F14" s="60" t="e">
+      <c r="F14" s="60">
         <f t="shared" si="8"/>
+        <v>44.557083333333331</v>
+      </c>
+      <c r="G14" s="91" t="e">
+        <f t="shared" ca="1" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G14" s="91" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H14" s="37" t="e">
+      <c r="H14" s="37">
         <f t="shared" si="6"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I14" s="150"/>
-      <c r="J14" s="77" t="e">
+        <v>1.41204634504427E-3</v>
+      </c>
+      <c r="I14" s="152"/>
+      <c r="J14" s="77">
         <f>IF(B14=118,IF(C14&gt;D14,(118-2.4*(($C$14-$D$14)/($D$2-($E$27/($A$1*1000))))/$D$31),(118-2.4*(($C$14-$D$14)/($D$2-($E$27/($A$1*1000))))/$D$31)),ABS(C14-F14))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K14" s="151"/>
+        <v>6.2916666666666288E-2</v>
+      </c>
+      <c r="K14" s="153"/>
       <c r="L14" s="14"/>
-      <c r="M14" s="12" t="e">
+      <c r="M14" s="12">
         <f>IF((C14&gt;100)*(B1="№")+(B1="Т"),D14+AD21,C14+AD21)</f>
-        <v>#VALUE!</v>
+        <v>7.2199999999999989</v>
       </c>
       <c r="N14" s="8"/>
       <c r="O14" s="13"/>
@@ -4619,40 +4617,40 @@
       </c>
     </row>
     <row r="15" spans="1:30" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A15" s="158"/>
+      <c r="A15" s="160"/>
       <c r="B15" s="18">
         <v>132</v>
       </c>
-      <c r="C15" s="55" t="s">
-        <v>20</v>
+      <c r="C15" s="55">
+        <v>49.22</v>
       </c>
       <c r="D15" s="125" t="e">
         <f ca="1">((B15-$E$26*($E$2*94/($B$28-$B$30)))-118)/(2.4-(2.4*$E$26*($E$14+$E$16)/$B$31))*($B$31+E14*$E$26)*($D$2-($E$27/($A$1*1000)))+((((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))*($D$2-($E$27/($A$1*1000))))+$D$30*($D$2-($E$27/($A$1*1000))))*10</f>
         <v>#VALUE!</v>
       </c>
       <c r="E15" s="71"/>
-      <c r="F15" s="59" t="e">
+      <c r="F15" s="59">
         <f t="shared" si="8"/>
-        <v>#VALUE!</v>
+        <v>49.069583333333334</v>
       </c>
       <c r="G15" s="93" t="e">
         <f t="shared" ca="1" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H15" s="36" t="e">
+      <c r="H15" s="36">
         <f t="shared" si="6"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I15" s="150"/>
-      <c r="J15" s="40" t="e">
+        <v>3.0653748503400415E-3</v>
+      </c>
+      <c r="I15" s="152"/>
+      <c r="J15" s="40">
         <f>ABS(C15-F15)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K15" s="151"/>
+        <v>0.15041666666666487</v>
+      </c>
+      <c r="K15" s="153"/>
       <c r="L15" s="8"/>
-      <c r="M15" s="12" t="e">
-        <f ca="1">IF((C15&gt;100)*(B1="№")+(B1="Т"),D15+AD22,C15+AD22)</f>
-        <v>#VALUE!</v>
+      <c r="M15" s="12">
+        <f>IF((C15&gt;100)*(B1="№")+(B1="Т"),D15+AD22,C15+AD22)</f>
+        <v>6.82</v>
       </c>
       <c r="N15" s="8"/>
       <c r="O15" s="13"/>
@@ -4678,9 +4676,9 @@
     <row r="16" spans="1:30" ht="15.75" hidden="1" customHeight="1" thickBot="1">
       <c r="A16" s="49"/>
       <c r="B16" s="67"/>
-      <c r="C16" s="62" t="str">
+      <c r="C16" s="62">
         <f>IF($B$17=142,$C$17,$C$16)</f>
-        <v xml:space="preserve"> </v>
+        <v>52.83</v>
       </c>
       <c r="D16" s="131" t="e">
         <f ca="1">((((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))+$D$30+$D$31)*($D$2-($E$27/($A$1*1000))))*10</f>
@@ -4718,50 +4716,50 @@
       <c r="AD16" s="4"/>
     </row>
     <row r="17" spans="1:30" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A17" s="47" t="str">
+      <c r="A17" s="47">
         <f>IFERROR(IF((K12&gt;K17)+(K20&gt;K25),IF((K12-K17)&gt;(K20-K25),IF(SUM(F12:F15)&lt;SUM(C12:C15),IF((K12-K17)*5&lt;1,-1,IF((K12-K17)*5&gt;3,-3,-(K12-K17)*5)),IF((K12-K17)*5&lt;1,1,IF((K12-K17)*5&gt;3,3,(K12-K17)*5))),IF(SUM(F18:F24)&lt;SUM(C18:C24),IF((K20-K25)*5&lt;1,1,IF((K20-K25)*5+1&gt;3,3,(K20-K25)*5+1)),IF((K20-K25)*5&lt;1,-1,IF((K20-K25)*5+1&gt;3,-3,-(K20-K25)*5-1)))),"Б"),"Б")</f>
-        <v>Б</v>
+        <v>-3</v>
       </c>
       <c r="B17" s="29">
         <v>142</v>
       </c>
-      <c r="C17" s="53" t="s">
-        <v>20</v>
+      <c r="C17" s="53">
+        <v>52.83</v>
       </c>
       <c r="D17" s="123" t="str">
-        <f>IFERROR(IF((B17-$E$26*($E$2*94/($B$28-$B$30)))&gt;142,((B17-$E$26*($E$2*94/($B$28-$B$30)))-142)/(9.4-(9.4*$E$26*($E$17+$E$25)/($B$29-$B$31)))*($B$29-$B$31+E17*$E$26)*(($D$2-($E$27/($A$1*1000)))-((((($D$29-$D$31)*$A$21)/($D$29-$D$31+$A$21))*($D$2-($E$27/($A$1*1000))))/$A$21))+((((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))+$D$30+$D$31)*($D$2-($E$27/($A$1*1000))))*10,((B17-$E$26*($E$2*94/($B$28-$B$30)))-118)/(2.4-(2.4*$E$26*($E$14+$E$16)/$B$31))*($B$31+E15*$E$26)*($D$2-($E$27/($A$1*1000)))+((((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))*($D$2-($E$27/($A$1*1000))))+$D$30*($D$2-($E$27/($A$1*1000))))*10)," ")</f>
+        <f ca="1">IFERROR(IF((B17-$E$26*($E$2*94/($B$28-$B$30)))&gt;142,((B17-$E$26*($E$2*94/($B$28-$B$30)))-142)/(9.4-(9.4*$E$26*($E$17+$E$25)/($B$29-$B$31)))*($B$29-$B$31+E17*$E$26)*(($D$2-($E$27/($A$1*1000)))-((((($D$29-$D$31)*$A$21)/($D$29-$D$31+$A$21))*($D$2-($E$27/($A$1*1000))))/$A$21))+((((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))+$D$30+$D$31)*($D$2-($E$27/($A$1*1000))))*10,((B17-$E$26*($E$2*94/($B$28-$B$30)))-118)/(2.4-(2.4*$E$26*($E$14+$E$16)/$B$31))*($B$31+E15*$E$26)*($D$2-($E$27/($A$1*1000)))+((((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))*($D$2-($E$27/($A$1*1000))))+$D$30*($D$2-($E$27/($A$1*1000))))*10)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E17" s="116">
         <f>K24</f>
         <v>0</v>
       </c>
-      <c r="F17" s="58" t="str">
+      <c r="F17" s="58">
         <f>IF(C17=" "," ",C17)</f>
+        <v>52.83</v>
+      </c>
+      <c r="G17" s="92" t="str">
+        <f ca="1">IFERROR(C17-D17," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="G17" s="92" t="str">
-        <f>IFERROR(C17-D17," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H17" s="38" t="e">
+      <c r="H17" s="38">
         <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+        <v>0</v>
       </c>
       <c r="I17" s="30">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="J17" s="39" t="str">
+      <c r="J17" s="39">
         <f>IF(F17=" "," ",IF(B1=7,IF(($C$16&gt;(((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))+$D$30+$D$31)*($D$2-($E$27/($A$1*1000)))*10),(142-(9.4*($C$16-(((((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))+$D$30+$D$31)*($D$2-($E$27/($A$1*1000))))*10))/(($D$29-$D$31)*(($D$2-($E$27/($A$1*1000)))-((((($D$29-$D$31)*$A$21)/($D$29-$D$31+$A$21))*($D$2-($E$27/($A$1*1000))))/$A$21))))),(142-(2.4*($C$16-(((((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))+$D$30+$D$31)*($D$2-($E$27/($A$1*1000))))*10))/($D$31*($D$2-($E$27/($A$1*1000))))))),0))</f>
-        <v xml:space="preserve"> </v>
+        <v>0</v>
       </c>
       <c r="K17" s="80">
         <v>0.5</v>
       </c>
       <c r="L17" s="8"/>
-      <c r="M17" s="16" t="e">
+      <c r="M17" s="16">
         <f>IF((C17&gt;100)*(B1="№")+(B1="Т"),D17+AD26,IF(B17=AC23,C17+AD23,IF(B17=AC24,C17+AD24,IF(B17=AC25,C17+AD25,IF(B17=AC26,C17+AD26,IF(B17=AC27,C17+AD27,IF(B17=AC32,C17+AD32,IF(B17=AC33,C17+AD33,"ошибка"))))))))</f>
-        <v>#VALUE!</v>
+        <v>6.2299999999999969</v>
       </c>
       <c r="N17" s="8"/>
       <c r="O17" s="11"/>
@@ -4785,46 +4783,46 @@
       </c>
     </row>
     <row r="18" spans="1:30" ht="15" customHeight="1">
-      <c r="A18" s="157" t="str">
-        <f>IF((C27=" ")+(B30=" "),IF((C4&gt;200)*(C4&lt;400),C4,IF(C4&gt;2000," ",A18)),(((B29-B31)*A21/(B29-B31+A21)+B31)*(A1*1000+(B28-B30)*A4/(B28-B30+A4)+B30))/(((B29-B31)*A21/((B29-B31)+A21)+B31)+A1*1000+(B28-B30)*A4/(B28-B30+A4)+B30))</f>
+      <c r="A18" s="159" t="str">
+        <f ca="1">IF((C27=" ")+(B30=" "),IF((C4&gt;200)*(C4&lt;400),C4,IF(C4&gt;2000," ",A18)),(((B29-B31)*A21/(B29-B31+A21)+B31)*(A1*1000+(B28-B30)*A4/(B28-B30+A4)+B30))/(((B29-B31)*A21/((B29-B31)+A21)+B31)+A1*1000+(B28-B30)*A4/(B28-B30+A4)+B30))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="B18" s="32">
         <v>156</v>
       </c>
-      <c r="C18" s="55" t="s">
-        <v>20</v>
+      <c r="C18" s="55">
+        <v>57.75</v>
       </c>
       <c r="D18" s="95" t="e">
         <f t="shared" ref="D18:D24" ca="1" si="9">((B18-$E$26*($E$2*94/($B$28-$B$30)))-142)/(9.4-(9.4*$E$26*($E$17+$E$25)/($B$29-$B$31)))*($B$29-$B$31+E17*$E$26)*(($D$2-($E$27/($A$1*1000)))-((((($D$29-$D$31)*$A$21)/($D$29-$D$31+$A$21))*($D$2-($E$27/($A$1*1000))))/$A$21))+((((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))+$D$30+$D$31)*($D$2-($E$27/($A$1*1000))))*10</f>
         <v>#VALUE!</v>
       </c>
       <c r="E18" s="75"/>
-      <c r="F18" s="59" t="e">
+      <c r="F18" s="59">
         <f t="shared" ref="F18:F24" si="10">(B18-$B$17)/($B$25-$B$17)*($C$25-$C$17)+$C$17</f>
-        <v>#VALUE!</v>
+        <v>57.065744680851061</v>
       </c>
       <c r="G18" s="93" t="e">
         <f t="shared" ca="1" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H18" s="36" t="e">
+      <c r="H18" s="36">
         <f t="shared" si="6"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I18" s="150" t="e">
+        <v>1.1990649083364138E-2</v>
+      </c>
+      <c r="I18" s="152">
         <f>SUM(H17:H25)/9</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="J18" s="40" t="e">
+        <v>1.2270336334577112E-2</v>
+      </c>
+      <c r="J18" s="40">
         <f t="shared" ref="J18:J24" si="11">ABS(C18-F18)</f>
-        <v>#VALUE!</v>
+        <v>0.68425531914893867</v>
       </c>
       <c r="K18" s="44"/>
       <c r="L18" s="8"/>
-      <c r="M18" s="12" t="e">
-        <f ca="1">IF((C18&gt;100)*(B1="№")+(B1="Т"),D18+AD34,C18+AD34)</f>
-        <v>#VALUE!</v>
+      <c r="M18" s="12">
+        <f>IF((C18&gt;100)*(B1="№")+(B1="Т"),D18+AD34,C18+AD34)</f>
+        <v>5.3500000000000014</v>
       </c>
       <c r="N18" s="8"/>
       <c r="O18" s="13"/>
@@ -4848,40 +4846,40 @@
       </c>
     </row>
     <row r="19" spans="1:30" ht="15" customHeight="1">
-      <c r="A19" s="157"/>
+      <c r="A19" s="159"/>
       <c r="B19" s="33">
         <v>168</v>
       </c>
-      <c r="C19" s="56" t="s">
-        <v>20</v>
+      <c r="C19" s="56">
+        <v>61.91</v>
       </c>
       <c r="D19" s="133" t="e">
         <f t="shared" ca="1" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="E19" s="76"/>
-      <c r="F19" s="60" t="e">
+      <c r="F19" s="60">
         <f t="shared" si="10"/>
-        <v>#VALUE!</v>
+        <v>60.696382978723406</v>
       </c>
       <c r="G19" s="91" t="e">
         <f t="shared" ca="1" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H19" s="37" t="e">
+      <c r="H19" s="37">
         <f t="shared" si="6"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I19" s="150"/>
-      <c r="J19" s="77" t="e">
+        <v>1.9994882095396252E-2</v>
+      </c>
+      <c r="I19" s="152"/>
+      <c r="J19" s="77">
         <f t="shared" si="11"/>
-        <v>#VALUE!</v>
+        <v>1.2136170212765904</v>
       </c>
       <c r="K19" s="44"/>
       <c r="L19" s="8"/>
-      <c r="M19" s="12" t="e">
-        <f ca="1">IF((C19&gt;100)*(B1="№")+(B1="Т"),D19+AD35,C19+AD35)</f>
-        <v>#VALUE!</v>
+      <c r="M19" s="12">
+        <f>IF((C19&gt;100)*(B1="№")+(B1="Т"),D19+AD35,C19+AD35)</f>
+        <v>4.509999999999998</v>
       </c>
       <c r="N19" s="8"/>
       <c r="O19" s="13"/>
@@ -4905,43 +4903,43 @@
       </c>
     </row>
     <row r="20" spans="1:30" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A20" s="157"/>
+      <c r="A20" s="159"/>
       <c r="B20" s="34">
         <v>180</v>
       </c>
-      <c r="C20" s="55" t="s">
-        <v>20</v>
+      <c r="C20" s="55">
+        <v>65.84</v>
       </c>
       <c r="D20" s="95" t="e">
         <f t="shared" ca="1" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="E20" s="75"/>
-      <c r="F20" s="59" t="e">
+      <c r="F20" s="59">
         <f t="shared" si="10"/>
-        <v>#VALUE!</v>
+        <v>64.327021276595744</v>
       </c>
       <c r="G20" s="93" t="e">
         <f t="shared" ca="1" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H20" s="36" t="e">
+      <c r="H20" s="36">
         <f t="shared" si="6"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I20" s="150"/>
-      <c r="J20" s="40" t="e">
+        <v>2.3520111663474931E-2</v>
+      </c>
+      <c r="I20" s="152"/>
+      <c r="J20" s="40">
         <f t="shared" si="11"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K20" s="151" t="str">
+        <v>1.5129787234042595</v>
+      </c>
+      <c r="K20" s="153">
         <f>IFERROR(IF(MAX(J18:J24)&gt;10,"FAIL",MAX(J18:J24)),"∆БВ=")</f>
-        <v>∆БВ=</v>
+        <v>1.5129787234042595</v>
       </c>
       <c r="L20" s="8"/>
-      <c r="M20" s="12" t="e">
-        <f ca="1">IF((C20&gt;100)*(B1="№")+(B1="Т"),D20+AD36,C20+AD36)</f>
-        <v>#VALUE!</v>
+      <c r="M20" s="12">
+        <f>IF((C20&gt;100)*(B1="№")+(B1="Т"),D20+AD36,C20+AD36)</f>
+        <v>3.4400000000000048</v>
       </c>
       <c r="N20" s="8"/>
       <c r="O20" s="13"/>
@@ -4965,43 +4963,43 @@
       </c>
     </row>
     <row r="21" spans="1:30" ht="15" customHeight="1">
-      <c r="A21" s="154" t="str">
-        <f>IF(B30=" ",IF(C6&gt;2000," ",IF((C6&gt;200)*(C6&lt;400),C6,A21)),326.8)</f>
+      <c r="A21" s="156" t="str">
+        <f ca="1">IF(B30=" ",IF(C6&gt;2000," ",IF((C6&gt;200)*(C6&lt;400),C6,A21)),326.8)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="B21" s="33">
         <v>192</v>
       </c>
-      <c r="C21" s="56" t="s">
-        <v>20</v>
+      <c r="C21" s="56">
+        <v>67.05</v>
       </c>
       <c r="D21" s="133" t="e">
         <f t="shared" ca="1" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="E21" s="76"/>
-      <c r="F21" s="60" t="e">
+      <c r="F21" s="60">
         <f t="shared" si="10"/>
-        <v>#VALUE!</v>
+        <v>67.957659574468082</v>
       </c>
       <c r="G21" s="91" t="e">
         <f t="shared" ca="1" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H21" s="37" t="e">
+      <c r="H21" s="37">
         <f t="shared" si="6"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I21" s="150"/>
-      <c r="J21" s="77" t="e">
+        <v>1.3356251232776345E-2</v>
+      </c>
+      <c r="I21" s="152"/>
+      <c r="J21" s="77">
         <f t="shared" si="11"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K21" s="151"/>
+        <v>0.90765957446808443</v>
+      </c>
+      <c r="K21" s="153"/>
       <c r="L21" s="14"/>
-      <c r="M21" s="12" t="e">
-        <f ca="1">IF((C21&gt;100)*(B1="№")+(B1="Т"),D21+AD37,C21+AD37)</f>
-        <v>#VALUE!</v>
+      <c r="M21" s="12">
+        <f>IF((C21&gt;100)*(B1="№")+(B1="Т"),D21+AD37,C21+AD37)</f>
+        <v>-0.35000000000000853</v>
       </c>
       <c r="N21" s="8"/>
       <c r="O21" s="13"/>
@@ -5025,40 +5023,40 @@
       </c>
     </row>
     <row r="22" spans="1:30" ht="15" customHeight="1">
-      <c r="A22" s="155"/>
+      <c r="A22" s="157"/>
       <c r="B22" s="34">
         <v>204</v>
       </c>
-      <c r="C22" s="55" t="s">
-        <v>20</v>
+      <c r="C22" s="55">
+        <v>70.11</v>
       </c>
       <c r="D22" s="95" t="e">
         <f t="shared" ca="1" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="E22" s="75"/>
-      <c r="F22" s="59" t="e">
+      <c r="F22" s="59">
         <f t="shared" si="10"/>
-        <v>#VALUE!</v>
+        <v>71.588297872340419</v>
       </c>
       <c r="G22" s="93" t="e">
         <f t="shared" ca="1" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H22" s="36" t="e">
+      <c r="H22" s="36">
         <f t="shared" si="6"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I22" s="150"/>
-      <c r="J22" s="40" t="e">
+        <v>2.0649993312825923E-2</v>
+      </c>
+      <c r="I22" s="152"/>
+      <c r="J22" s="40">
         <f t="shared" si="11"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K22" s="151"/>
+        <v>1.4782978723404199</v>
+      </c>
+      <c r="K22" s="153"/>
       <c r="L22" s="8"/>
-      <c r="M22" s="12" t="e">
-        <f ca="1">IF((C22&gt;100)*(B1="№")+(B1="Т"),D22+AD38,C22+AD38)</f>
-        <v>#VALUE!</v>
+      <c r="M22" s="12">
+        <f>IF((C22&gt;100)*(B1="№")+(B1="Т"),D22+AD38,C22+AD38)</f>
+        <v>-2.2900000000000063</v>
       </c>
       <c r="N22" s="8"/>
       <c r="O22" s="13"/>
@@ -5082,40 +5080,40 @@
       </c>
     </row>
     <row r="23" spans="1:30" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A23" s="156"/>
+      <c r="A23" s="158"/>
       <c r="B23" s="33">
         <v>216</v>
       </c>
-      <c r="C23" s="56" t="s">
-        <v>20</v>
+      <c r="C23" s="56">
+        <v>74.16</v>
       </c>
       <c r="D23" s="133" t="e">
         <f t="shared" ca="1" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="E23" s="76"/>
-      <c r="F23" s="60" t="e">
+      <c r="F23" s="60">
         <f t="shared" si="10"/>
-        <v>#VALUE!</v>
+        <v>75.218936170212771</v>
       </c>
       <c r="G23" s="91" t="e">
         <f t="shared" ca="1" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H23" s="37" t="e">
+      <c r="H23" s="37">
         <f t="shared" si="6"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I23" s="150"/>
-      <c r="J23" s="77" t="e">
+        <v>1.4078053002724078E-2</v>
+      </c>
+      <c r="I23" s="152"/>
+      <c r="J23" s="77">
         <f t="shared" si="11"/>
-        <v>#VALUE!</v>
+        <v>1.0589361702127746</v>
       </c>
       <c r="K23" s="44"/>
       <c r="L23" s="8"/>
-      <c r="M23" s="12" t="e">
-        <f ca="1">IF((C23&gt;100)*(B1="№")+(B1="Т"),D23+AD39,C23+AD39)</f>
-        <v>#VALUE!</v>
+      <c r="M23" s="12">
+        <f>IF((C23&gt;100)*(B1="№")+(B1="Т"),D23+AD39,C23+AD39)</f>
+        <v>-3.2400000000000091</v>
       </c>
       <c r="N23" s="8"/>
       <c r="O23" s="13"/>
@@ -5140,41 +5138,41 @@
     </row>
     <row r="24" spans="1:30" ht="15.75" customHeight="1" thickBot="1">
       <c r="A24" s="28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B24" s="35">
         <v>228</v>
       </c>
-      <c r="C24" s="55" t="s">
-        <v>20</v>
+      <c r="C24" s="55">
+        <v>78.31</v>
       </c>
       <c r="D24" s="95" t="e">
         <f t="shared" ca="1" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="E24" s="75"/>
-      <c r="F24" s="59" t="e">
+      <c r="F24" s="59">
         <f t="shared" si="10"/>
-        <v>#VALUE!</v>
+        <v>78.849574468085109</v>
       </c>
       <c r="G24" s="93" t="e">
         <f t="shared" ca="1" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H24" s="36" t="e">
+      <c r="H24" s="36">
         <f t="shared" si="6"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I24" s="150"/>
-      <c r="J24" s="40" t="e">
+        <v>6.8430866206323415E-3</v>
+      </c>
+      <c r="I24" s="152"/>
+      <c r="J24" s="40">
         <f t="shared" si="11"/>
-        <v>#VALUE!</v>
+        <v>0.53957446808510667</v>
       </c>
       <c r="K24" s="45"/>
       <c r="L24" s="8"/>
-      <c r="M24" s="12" t="e">
-        <f ca="1">IF((C24&gt;100)*(B1="№")+(B1="Т"),D24+AD40,C24+AD40)</f>
-        <v>#VALUE!</v>
+      <c r="M24" s="12">
+        <f>IF((C24&gt;100)*(B1="№")+(B1="Т"),D24+AD40,C24+AD40)</f>
+        <v>-4.0900000000000034</v>
       </c>
       <c r="N24" s="8"/>
       <c r="O24" s="13"/>
@@ -5198,15 +5196,15 @@
       </c>
     </row>
     <row r="25" spans="1:30" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A25" s="47" t="str">
+      <c r="A25" s="47">
         <f>IFERROR(IF(K20&gt;K25,IF(SUM(F18:F24)&lt;SUM(C18:C24),IF(C25&gt;99.5,IF((K20-K25)*5&lt;1,-1,IF((K20-K25)*5&gt;4,-4,-(K20-K25)*5)),IF((K20-K25)*5&lt;1,1,IF((K20-K25)*5&gt;4,4,(K20-K25)*5))),IF(C25&gt;99.5,IF((K20-K25)*5&lt;1,1,IF((K20-K25)*5&gt;4,4,(K20-K25)*5)),IF((K20-K25)*5&lt;1,-1,IF((K20-K25)*5&gt;4,-4,-(K20-K25)*5)))),"В"),"В")</f>
-        <v>В</v>
+        <v>-4</v>
       </c>
       <c r="B25" s="29">
         <v>236</v>
       </c>
-      <c r="C25" s="53" t="s">
-        <v>20</v>
+      <c r="C25" s="53">
+        <v>81.27</v>
       </c>
       <c r="D25" s="132" t="str">
         <f ca="1">IFERROR(((B25-$E$26*($E$2*94/($B$28-$B$30)))-142)/(9.4-(9.4*$E$26*($E$17+$E$25)/($B$29-$B$31)))*($B$29-$B$31+E24*$E$26)*(($D$2-($E$27/($A$1*1000)))-((((($D$29-$D$31)*$A$21)/($D$29-$D$31+$A$21))*($D$2-($E$27/($A$1*1000))))/$A$21))+((((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))+$D$30+$D$31)*($D$2-($E$27/($A$1*1000))))*10," ")</f>
@@ -5216,32 +5214,32 @@
         <f>K4</f>
         <v>0</v>
       </c>
-      <c r="F25" s="58" t="str">
+      <c r="F25" s="58">
         <f>IF(C25=" "," ",C25)</f>
-        <v xml:space="preserve"> </v>
+        <v>81.27</v>
       </c>
       <c r="G25" s="92" t="str">
         <f ca="1">IFERROR(C25-D25," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H25" s="38" t="e">
+      <c r="H25" s="38">
         <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+        <v>0</v>
       </c>
       <c r="I25" s="30">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="J25" s="142" t="str">
+      <c r="J25" s="142">
         <f>IF(F25=" "," ",IF(B1=7,236-(9.4*(($C$24-$D$24)/(($D$2-($E$27/($A$1*1000)))-((((($D$29-$D$31)*$A$21)/($D$29-$D$31+$A$21))*($D$2-($E$27/($A$1*1000))))/$A$21)))/($D$29-$D$31)),0))</f>
-        <v xml:space="preserve"> </v>
+        <v>0</v>
       </c>
       <c r="K25" s="80">
         <v>0.4</v>
       </c>
       <c r="L25" s="8"/>
-      <c r="M25" s="10" t="e">
-        <f ca="1">IF((C25&gt;110)*(B1="№")+(B1="Т"),D25+AD45,IF(B25=AC41,C25+AD41,IF(B25=AC42,C25+AD42,IF(B25=AC43,C25+AD43,IF(B25=AC44,C25+AD44,IF(B25=AC45,C25+AD45,IF(B25=AC46,C25+AD46,IF(B25=AC47,C25+AD47,IF(B25=AC48,C25+AD48,IF(B25=AC49,C25+AD49,"ошибка"))))))))))</f>
-        <v>#VALUE!</v>
+      <c r="M25" s="10">
+        <f>IF((C25&gt;110)*(B1="№")+(B1="Т"),D25+AD45,IF(B25=AC41,C25+AD41,IF(B25=AC42,C25+AD42,IF(B25=AC43,C25+AD43,IF(B25=AC44,C25+AD44,IF(B25=AC45,C25+AD45,IF(B25=AC46,C25+AD46,IF(B25=AC47,C25+AD47,IF(B25=AC48,C25+AD48,IF(B25=AC49,C25+AD49,"ошибка"))))))))))</f>
+        <v>-4.5299999999999869</v>
       </c>
       <c r="N25" s="8"/>
       <c r="O25" s="11"/>
@@ -5266,19 +5264,19 @@
     </row>
     <row r="26" spans="1:30" ht="15.75" thickBot="1">
       <c r="A26" s="122" t="str">
-        <f>IF(C9&gt;5000," ",IF((C9&lt;5),C9,A26))</f>
+        <f ca="1">IF(C9&gt;5000," ",IF((C9&lt;5),C9,A26))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="B26" s="52" t="e">
-        <f>IF(B27&lt;600,"Ползун",B28/B30)</f>
+        <f ca="1">IF(B27&lt;600,"Ползун",B28/B30)</f>
         <v>#VALUE!</v>
       </c>
       <c r="C26" s="51" t="e">
-        <f>IF(B27&lt;600,"Общее",B29/B31)</f>
+        <f ca="1">IF(B27&lt;600,"Общее",B29/B31)</f>
         <v>#VALUE!</v>
       </c>
       <c r="D26" s="96" t="str">
-        <f>IFERROR(D28+D29," ")</f>
+        <f ca="1">IFERROR(D28+D29," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E26" s="84">
@@ -5315,14 +5313,14 @@
     </row>
     <row r="27" spans="1:30" ht="15.75" thickBot="1">
       <c r="A27" s="21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B27" s="79" t="str">
-        <f>IF(B28=" ",IF((C5&gt;200)*(C5&lt;2000),C5,IF(C5&gt;2000," ",B27)),B28+B29)</f>
+        <f ca="1">IF(B28=" ",IF((C5&gt;200)*(C5&lt;2000),C5,IF(C5&gt;2000," ",B27)),B28+B29)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="C27" s="85" t="str">
-        <f>(IF(B30=" ",IF((C2&gt;400)*(C2&lt;2000),C2,IF(C2&gt;2000," ",C27)),((B28-B30)*A4/((B28-B30)+A4)+B30+B31+(B29-B31)*A21/((B29-B31)+A21))*A1*1000/(((B28-B30)*A4/((B28-B30)+A4)+B30+B31+(B29-B31)*A21/((B29-B31)+A21))+A1*1000)))</f>
+        <f ca="1">(IF(B30=" ",IF((C2&gt;400)*(C2&lt;2000),C2,IF(C2&gt;2000," ",C27)),((B28-B30)*A4/((B28-B30)+A4)+B30+B31+(B29-B31)*A21/((B29-B31)+A21))*A1*1000/(((B28-B30)*A4/((B28-B30)+A4)+B30+B31+(B29-B31)*A21/((B29-B31)+A21))+A1*1000)))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D27" s="105" t="str">
@@ -5363,22 +5361,22 @@
     </row>
     <row r="28" spans="1:30">
       <c r="A28" s="42" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B28" s="97" t="str">
-        <f>IF(C3&gt;2000," ",IF((C3&gt;400)*(C3&lt;1500),C3,B28))</f>
+        <f ca="1">IF(C3&gt;2000," ",IF((C3&gt;400)*(C3&lt;1500),C3,B28))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C28" s="147" t="str">
-        <f>IF(NOT(B1="R"),IF(B28=" "," ",ABS(B28-B29)),ABS(D28-D29))</f>
+      <c r="C28" s="149" t="str">
+        <f ca="1">IF(NOT(B1="R"),IF(B28=" "," ",ABS(B28-B29)),ABS(D28-D29))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D28" s="98" t="str">
-        <f>IFERROR(IF(A7=" ",(SQRT(POWER(2*A4-(C27*A1*1000*0.8)/(A1*1000-C27),2)+(1.28*C27*A1*1000*A4)/(A1*1000-C27))+(C27*A1*1000*0.8)/(A1*1000-C27)-2*A4)/0.64,IFERROR(B28+E26*SUM(E2:E13),(-(A4-(1-1/E30)*((-(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-SQRT(((-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))*(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-4*(((A1*1000)*C27/((A1*1000)-C27))+(A1*1000))*A7)))/2))+SQRT(((A4-(1-1/E30)*((-(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-SQRT(((-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))*(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-4*(((A1*1000)*C27/((A1*1000)-C27))+(A1*1000))*A7)))/2))*(A4-(1-1/E30)*((-(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-SQRT(((-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))*(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-4*(((A1*1000)*C27/((A1*1000)-C27))+(A1*1000))*A7)))/2))+4*((E30-1)/(E30*E30))*A4*((-(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-SQRT(((-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))*(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-4*(((A1*1000)*C27/((A1*1000)-C27))+(A1*1000))*A7)))/2))))/(2*((E30-1)/(E30*E30)))))," ")</f>
+        <f ca="1">IFERROR(IF(A7=" ",(SQRT(POWER(2*A4-(C27*A1*1000*0.8)/(A1*1000-C27),2)+(1.28*C27*A1*1000*A4)/(A1*1000-C27))+(C27*A1*1000*0.8)/(A1*1000-C27)-2*A4)/0.64,IFERROR(B28+E26*SUM(E2:E13),(-(A4-(1-1/E30)*((-(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-SQRT(((-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))*(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-4*(((A1*1000)*C27/((A1*1000)-C27))+(A1*1000))*A7)))/2))+SQRT(((A4-(1-1/E30)*((-(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-SQRT(((-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))*(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-4*(((A1*1000)*C27/((A1*1000)-C27))+(A1*1000))*A7)))/2))*(A4-(1-1/E30)*((-(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-SQRT(((-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))*(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-4*(((A1*1000)*C27/((A1*1000)-C27))+(A1*1000))*A7)))/2))+4*((E30-1)/(E30*E30))*A4*((-(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-SQRT(((-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))*(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-4*(((A1*1000)*C27/((A1*1000)-C27))+(A1*1000))*A7)))/2))))/(2*((E30-1)/(E30*E30)))))," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E28" s="98" t="str">
-        <f>IFERROR(ABS(D28-D29)," ")</f>
+        <f ca="1">IFERROR(ABS(D28-D29)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F28" s="110"/>
@@ -5406,15 +5404,15 @@
     </row>
     <row r="29" spans="1:30" ht="15.75" thickBot="1">
       <c r="A29" s="99" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B29" s="100" t="str">
-        <f>IF(C4&gt;2000," ",IF((C4&gt;400)*(C4&lt;1500),C4,B29))</f>
+        <f ca="1">IF(C4&gt;2000," ",IF((C4&gt;400)*(C4&lt;1500),C4,B29))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C29" s="148"/>
+      <c r="C29" s="150"/>
       <c r="D29" s="101" t="str">
-        <f>IFERROR(IF(A18=" ",(SQRT(POWER(2*A4-(C27*A1*1000*0.8)/(A1*1000-C27),2)+(1.28*C27*A1*1000*A4)/(A1*1000-C27))+(C27*A1*1000*0.8)/(A1*1000-C27)-2*A4)/0.64,IFERROR(B29+E26*SUM(E14:E25),(-(A21-(1-1/E31)*((-(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-SQRT(((-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))*(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-4*(((A1*1000)*C27/((A1*1000)-C27))+(A1*1000))*A18)))/2))+SQRT(((A21-(1-1/E31)*((-(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-SQRT(((-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))*(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-4*(((A1*1000)*C27/((A1*1000)-C27))+(A1*1000))*A18)))/2))*(A21-(1-1/E31)*((-(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-SQRT(((-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))*(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-4*(((A1*1000)*C27/((A1*1000)-C27))+(A1*1000))*A18)))/2))+4*((E31-1)/(E31*E31))*A21*((-(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-SQRT(((-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))*(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-4*(((A1*1000)*C27/((A1*1000)-C27))+(A1*1000))*A18)))/2))))/(2*((E31-1)/(E31*E31)))))," ")</f>
+        <f ca="1">IFERROR(IF(A18=" ",(SQRT(POWER(2*A4-(C27*A1*1000*0.8)/(A1*1000-C27),2)+(1.28*C27*A1*1000*A4)/(A1*1000-C27))+(C27*A1*1000*0.8)/(A1*1000-C27)-2*A4)/0.64,IFERROR(B29+E26*SUM(E14:E25),(-(A21-(1-1/E31)*((-(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-SQRT(((-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))*(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-4*(((A1*1000)*C27/((A1*1000)-C27))+(A1*1000))*A18)))/2))+SQRT(((A21-(1-1/E31)*((-(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-SQRT(((-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))*(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-4*(((A1*1000)*C27/((A1*1000)-C27))+(A1*1000))*A18)))/2))*(A21-(1-1/E31)*((-(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-SQRT(((-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))*(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-4*(((A1*1000)*C27/((A1*1000)-C27))+(A1*1000))*A18)))/2))+4*((E31-1)/(E31*E31))*A21*((-(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-SQRT(((-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))*(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-4*(((A1*1000)*C27/((A1*1000)-C27))+(A1*1000))*A18)))/2))))/(2*((E31-1)/(E31*E31)))))," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E29" s="101" t="str">
@@ -5446,14 +5444,14 @@
     </row>
     <row r="30" spans="1:30">
       <c r="A30" s="102" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B30" s="103" t="str">
-        <f>IF(C5&gt;400," ",IF((C5&gt;100)*(C5&lt;250),C5,B30))</f>
+        <f ca="1">IF(C5&gt;400," ",IF((C5&gt;100)*(C5&lt;250),C5,B30))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C30" s="149" t="str">
-        <f>IF(NOT(B1="R"),IF(B30=" "," ",ABS(B30-B31)),ABS(D30-D31))</f>
+      <c r="C30" s="151" t="str">
+        <f ca="1">IF(NOT(B1="R"),IF(B30=" "," ",ABS(B30-B31)),ABS(D30-D31))</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D30" s="140" t="str">
@@ -5489,13 +5487,13 @@
     </row>
     <row r="31" spans="1:30" ht="15.75" thickBot="1">
       <c r="A31" s="99" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B31" s="104" t="str">
-        <f>IF(C6&gt;400," ",IF((C6&gt;100)*(C6&lt;250),C6,B31))</f>
+        <f ca="1">IF(C6&gt;400," ",IF((C6&gt;100)*(C6&lt;250),C6,B31))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C31" s="148"/>
+      <c r="C31" s="150"/>
       <c r="D31" s="120" t="str">
         <f ca="1">IFERROR(IFERROR(IF(NOT(B1="R"),B31+E26*SUM(E14:E16),IF(A18=" ",D29/5,D29/E31)),D29/E31)," ")</f>
         <v xml:space="preserve"> </v>
@@ -5564,15 +5562,11 @@
     </row>
     <row r="33" spans="1:30">
       <c r="A33" s="126"/>
-      <c r="B33" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="C33" s="22" t="s">
-        <v>17</v>
-      </c>
+      <c r="B33" s="145"/>
+      <c r="C33" s="145"/>
       <c r="D33" s="22"/>
       <c r="E33" s="22"/>
-      <c r="F33" s="136"/>
+      <c r="F33" s="146"/>
       <c r="G33" s="136"/>
       <c r="H33" s="136"/>
       <c r="I33" s="136"/>
@@ -5914,9 +5908,9 @@
     </row>
     <row r="43" spans="1:30">
       <c r="B43" s="130"/>
-      <c r="C43" s="7" t="e">
+      <c r="C43" s="7">
         <f>M11</f>
-        <v>#VALUE!</v>
+        <v>8.18</v>
       </c>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>

</xml_diff>

<commit_message>
check box set zero point is implemented
</commit_message>
<xml_diff>
--- a/applications/VBA/_3д_1_Ц.xlsx
+++ b/applications/VBA/_3д_1_Ц.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>О</t>
   </si>
@@ -68,12 +68,6 @@
   </si>
   <si>
     <t>№</t>
-  </si>
-  <si>
-    <t>COM2</t>
-  </si>
-  <si>
-    <t>COM9</t>
   </si>
 </sst>
 </file>
@@ -1019,31 +1013,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="20" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1071,6 +1040,31 @@
     <xf numFmtId="2" fontId="2" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="20" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -2243,9 +2237,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="9.5949478026902763E-2"/>
-          <c:y val="3.0407576263407978E-2"/>
+          <c:y val="3.0407576263407985E-2"/>
           <c:w val="0.83101021525844065"/>
-          <c:h val="0.92240676091667206"/>
+          <c:h val="0.92240676091667195"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2680,8 +2674,8 @@
               <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-7.7082901385847561E-3"/>
-                  <c:y val="-3.7230948225716799E-2"/>
+                  <c:x val="-7.7082901385847578E-3"/>
+                  <c:y val="-3.7230948225716813E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -3161,11 +3155,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:axId val="158775936"/>
-        <c:axId val="158786304"/>
+        <c:axId val="176237568"/>
+        <c:axId val="177069056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="158775936"/>
+        <c:axId val="176237568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3191,19 +3185,19 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.38193271256707262"/>
+              <c:x val="0.38193271256707267"/>
               <c:y val="0.95763807011034663"/>
             </c:manualLayout>
           </c:layout>
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="158786304"/>
+        <c:crossAx val="177069056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="158786304"/>
+        <c:axId val="177069056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="240"/>
@@ -3241,7 +3235,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="158775936"/>
+        <c:crossAx val="176237568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="12"/>
@@ -3766,7 +3760,7 @@
   <dimension ref="A1:AD49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScaleSheetLayoutView="110" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="AA14" sqref="AA14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3812,14 +3806,14 @@
       <c r="G1" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="147" t="s">
+      <c r="H1" s="156" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="155"/>
-      <c r="J1" s="147">
+      <c r="I1" s="164"/>
+      <c r="J1" s="156">
         <v>0</v>
       </c>
-      <c r="K1" s="148"/>
+      <c r="K1" s="157"/>
       <c r="L1" s="8"/>
       <c r="M1" s="9"/>
       <c r="N1" s="8"/>
@@ -3835,9 +3829,7 @@
       <c r="X1" s="8"/>
       <c r="Y1" s="8"/>
       <c r="Z1" s="8"/>
-      <c r="AA1" s="144" t="s">
-        <v>17</v>
-      </c>
+      <c r="AA1" s="144"/>
     </row>
     <row r="2" spans="1:30" ht="15.75" customHeight="1" thickBot="1">
       <c r="A2" s="46" t="s">
@@ -3895,9 +3887,7 @@
       <c r="X2" s="8"/>
       <c r="Y2" s="8"/>
       <c r="Z2" s="8"/>
-      <c r="AA2" s="144" t="s">
-        <v>18</v>
-      </c>
+      <c r="AA2" s="144"/>
       <c r="AC2" s="2">
         <v>0</v>
       </c>
@@ -3933,7 +3923,7 @@
         <f>J3/F3</f>
         <v>0.77477477477477497</v>
       </c>
-      <c r="I3" s="152">
+      <c r="I3" s="161">
         <f>SUM(H3:H9)/9</f>
         <v>0.14950009533342867</v>
       </c>
@@ -3960,9 +3950,7 @@
       <c r="X3" s="8"/>
       <c r="Y3" s="8"/>
       <c r="Z3" s="8"/>
-      <c r="AA3" s="144">
-        <v>50.53</v>
-      </c>
+      <c r="AA3" s="144"/>
       <c r="AC3" s="1">
         <f t="shared" ref="AC3:AC8" si="4">AC2+12</f>
         <v>12</v>
@@ -3973,7 +3961,7 @@
       </c>
     </row>
     <row r="4" spans="1:30" ht="15" customHeight="1">
-      <c r="A4" s="161" t="str">
+      <c r="A4" s="152" t="str">
         <f ca="1">IF(B30=" ",IF(C7&gt;2000," ",IF((C7&gt;200)*(C7&lt;400),C7,A4)),326.8)</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -4001,7 +3989,7 @@
         <f t="shared" ref="H4:H25" si="6">J4/F4</f>
         <v>0.30518018018018028</v>
       </c>
-      <c r="I4" s="152"/>
+      <c r="I4" s="161"/>
       <c r="J4" s="77">
         <f t="shared" si="3"/>
         <v>2.7100000000000009</v>
@@ -4025,9 +4013,7 @@
       <c r="X4" s="8"/>
       <c r="Y4" s="8"/>
       <c r="Z4" s="8"/>
-      <c r="AA4" s="144">
-        <v>126.37</v>
-      </c>
+      <c r="AA4" s="144"/>
       <c r="AC4" s="1">
         <f t="shared" si="4"/>
         <v>24</v>
@@ -4038,7 +4024,7 @@
       </c>
     </row>
     <row r="5" spans="1:30" ht="15" customHeight="1">
-      <c r="A5" s="162"/>
+      <c r="A5" s="153"/>
       <c r="B5" s="34">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -4063,12 +4049,12 @@
         <f t="shared" si="6"/>
         <v>0.14114114114114107</v>
       </c>
-      <c r="I5" s="152"/>
+      <c r="I5" s="161"/>
       <c r="J5" s="40">
         <f t="shared" si="3"/>
         <v>1.879999999999999</v>
       </c>
-      <c r="K5" s="153">
+      <c r="K5" s="162">
         <f>IFERROR(IF(MAX(J3:J9)&gt;10,"FAIL",MAX(J3:J9)),"∆ОА=")</f>
         <v>3.4400000000000004</v>
       </c>
@@ -4101,7 +4087,7 @@
       </c>
     </row>
     <row r="6" spans="1:30" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A6" s="163"/>
+      <c r="A6" s="154"/>
       <c r="B6" s="33">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -4126,12 +4112,12 @@
         <f t="shared" si="6"/>
         <v>8.3896396396396511E-2</v>
       </c>
-      <c r="I6" s="152"/>
+      <c r="I6" s="161"/>
       <c r="J6" s="77">
         <f t="shared" si="3"/>
         <v>1.490000000000002</v>
       </c>
-      <c r="K6" s="153"/>
+      <c r="K6" s="162"/>
       <c r="L6" s="14"/>
       <c r="M6" s="12">
         <f>IF(((C6&gt;100)+(C6&lt;5))*((B1="№")+(B1="R"))+(B1="Т"),D6+AD6,C6+AD6)</f>
@@ -4161,7 +4147,7 @@
       </c>
     </row>
     <row r="7" spans="1:30" ht="15" customHeight="1">
-      <c r="A7" s="164" t="str">
+      <c r="A7" s="155" t="str">
         <f ca="1">IF((C27=" ")+(B30=" "),IF((C3&gt;200)*(C3&lt;400),C3,IF(C3&gt;2000," ",A7)),((((B28-B30)*A4/(B28-B30+A4))+B30)*(A1*1000+((B29-B31)*A21/((B29-B31)+A21))+B31))/((((B28-B30)*A4/((B28-B30)+A4))+B30)+A1*1000+((B29-B31)*A21/((B29-B31)+A21))+B31))</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -4189,12 +4175,12 @@
         <f t="shared" si="6"/>
         <v>2.9729729729729572E-2</v>
       </c>
-      <c r="I7" s="152"/>
+      <c r="I7" s="161"/>
       <c r="J7" s="40">
         <f t="shared" si="3"/>
         <v>0.65999999999999659</v>
       </c>
-      <c r="K7" s="153"/>
+      <c r="K7" s="162"/>
       <c r="L7" s="8"/>
       <c r="M7" s="12">
         <f>IF((C7&gt;100)*((B1="№")+(B1="R"))+(B1="Т"),D7+AD7,C7+AD7)</f>
@@ -4223,7 +4209,7 @@
       </c>
     </row>
     <row r="8" spans="1:30" ht="15" customHeight="1">
-      <c r="A8" s="164"/>
+      <c r="A8" s="155"/>
       <c r="B8" s="33">
         <f t="shared" si="0"/>
         <v>72</v>
@@ -4248,7 +4234,7 @@
         <f t="shared" si="6"/>
         <v>1.0135135135135118E-2</v>
       </c>
-      <c r="I8" s="152"/>
+      <c r="I8" s="161"/>
       <c r="J8" s="77">
         <f t="shared" si="3"/>
         <v>0.26999999999999957</v>
@@ -4282,7 +4268,7 @@
       </c>
     </row>
     <row r="9" spans="1:30" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A9" s="164"/>
+      <c r="A9" s="155"/>
       <c r="B9" s="35">
         <f>B8+12</f>
         <v>84</v>
@@ -4307,7 +4293,7 @@
         <f t="shared" si="6"/>
         <v>6.4350064350062982E-4</v>
       </c>
-      <c r="I9" s="152"/>
+      <c r="I9" s="161"/>
       <c r="J9" s="40">
         <f t="shared" si="3"/>
         <v>1.9999999999999574E-2</v>
@@ -4449,7 +4435,7 @@
       </c>
     </row>
     <row r="12" spans="1:30" ht="15" customHeight="1">
-      <c r="A12" s="160" t="str">
+      <c r="A12" s="151" t="str">
         <f ca="1">IF((A7=" ")+(A18=" ")," ",ABS(A7-A18))</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -4476,7 +4462,7 @@
         <f t="shared" si="6"/>
         <v>2.3827608811012348E-3</v>
       </c>
-      <c r="I12" s="152">
+      <c r="I12" s="161">
         <f>SUM(H12,H14,H15)/5</f>
         <v>1.3720364152971093E-3</v>
       </c>
@@ -4484,7 +4470,7 @@
         <f>ABS(C12-F12)</f>
         <v>9.5416666666665151E-2</v>
       </c>
-      <c r="K12" s="154">
+      <c r="K12" s="163">
         <f>IFERROR(IF(MAX(J12:J15)&gt;10,"FAIL",MAX(J12:J15)),"∆АБ=")</f>
         <v>0.15041666666666487</v>
       </c>
@@ -4515,7 +4501,7 @@
       </c>
     </row>
     <row r="13" spans="1:30" ht="15" hidden="1" customHeight="1">
-      <c r="A13" s="160"/>
+      <c r="A13" s="151"/>
       <c r="B13" s="67"/>
       <c r="C13" s="62"/>
       <c r="D13" s="94" t="e">
@@ -4532,12 +4518,12 @@
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I13" s="152"/>
+      <c r="I13" s="161"/>
       <c r="J13" s="68">
         <f>ABS(C13-F13)</f>
         <v>0</v>
       </c>
-      <c r="K13" s="153"/>
+      <c r="K13" s="162"/>
       <c r="L13" s="8"/>
       <c r="M13" s="12"/>
       <c r="N13" s="8"/>
@@ -4557,7 +4543,7 @@
       <c r="AD13" s="4"/>
     </row>
     <row r="14" spans="1:30" ht="15" customHeight="1">
-      <c r="A14" s="160"/>
+      <c r="A14" s="151"/>
       <c r="B14" s="19">
         <v>120</v>
       </c>
@@ -4584,12 +4570,12 @@
         <f t="shared" si="6"/>
         <v>1.41204634504427E-3</v>
       </c>
-      <c r="I14" s="152"/>
+      <c r="I14" s="161"/>
       <c r="J14" s="77">
         <f>IF(B14=118,IF(C14&gt;D14,(118-2.4*(($C$14-$D$14)/($D$2-($E$27/($A$1*1000))))/$D$31),(118-2.4*(($C$14-$D$14)/($D$2-($E$27/($A$1*1000))))/$D$31)),ABS(C14-F14))</f>
         <v>6.2916666666666288E-2</v>
       </c>
-      <c r="K14" s="153"/>
+      <c r="K14" s="162"/>
       <c r="L14" s="14"/>
       <c r="M14" s="12">
         <f>IF((C14&gt;100)*(B1="№")+(B1="Т"),D14+AD21,C14+AD21)</f>
@@ -4617,7 +4603,7 @@
       </c>
     </row>
     <row r="15" spans="1:30" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A15" s="160"/>
+      <c r="A15" s="151"/>
       <c r="B15" s="18">
         <v>132</v>
       </c>
@@ -4641,12 +4627,12 @@
         <f t="shared" si="6"/>
         <v>3.0653748503400415E-3</v>
       </c>
-      <c r="I15" s="152"/>
+      <c r="I15" s="161"/>
       <c r="J15" s="40">
         <f>ABS(C15-F15)</f>
         <v>0.15041666666666487</v>
       </c>
-      <c r="K15" s="153"/>
+      <c r="K15" s="162"/>
       <c r="L15" s="8"/>
       <c r="M15" s="12">
         <f>IF((C15&gt;100)*(B1="№")+(B1="Т"),D15+AD22,C15+AD22)</f>
@@ -4783,7 +4769,7 @@
       </c>
     </row>
     <row r="18" spans="1:30" ht="15" customHeight="1">
-      <c r="A18" s="159" t="str">
+      <c r="A18" s="150" t="str">
         <f ca="1">IF((C27=" ")+(B30=" "),IF((C4&gt;200)*(C4&lt;400),C4,IF(C4&gt;2000," ",A18)),(((B29-B31)*A21/(B29-B31+A21)+B31)*(A1*1000+(B28-B30)*A4/(B28-B30+A4)+B30))/(((B29-B31)*A21/((B29-B31)+A21)+B31)+A1*1000+(B28-B30)*A4/(B28-B30+A4)+B30))</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -4810,7 +4796,7 @@
         <f t="shared" si="6"/>
         <v>1.1990649083364138E-2</v>
       </c>
-      <c r="I18" s="152">
+      <c r="I18" s="161">
         <f>SUM(H17:H25)/9</f>
         <v>1.2270336334577112E-2</v>
       </c>
@@ -4846,7 +4832,7 @@
       </c>
     </row>
     <row r="19" spans="1:30" ht="15" customHeight="1">
-      <c r="A19" s="159"/>
+      <c r="A19" s="150"/>
       <c r="B19" s="33">
         <v>168</v>
       </c>
@@ -4870,7 +4856,7 @@
         <f t="shared" si="6"/>
         <v>1.9994882095396252E-2</v>
       </c>
-      <c r="I19" s="152"/>
+      <c r="I19" s="161"/>
       <c r="J19" s="77">
         <f t="shared" si="11"/>
         <v>1.2136170212765904</v>
@@ -4903,7 +4889,7 @@
       </c>
     </row>
     <row r="20" spans="1:30" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A20" s="159"/>
+      <c r="A20" s="150"/>
       <c r="B20" s="34">
         <v>180</v>
       </c>
@@ -4927,12 +4913,12 @@
         <f t="shared" si="6"/>
         <v>2.3520111663474931E-2</v>
       </c>
-      <c r="I20" s="152"/>
+      <c r="I20" s="161"/>
       <c r="J20" s="40">
         <f t="shared" si="11"/>
         <v>1.5129787234042595</v>
       </c>
-      <c r="K20" s="153">
+      <c r="K20" s="162">
         <f>IFERROR(IF(MAX(J18:J24)&gt;10,"FAIL",MAX(J18:J24)),"∆БВ=")</f>
         <v>1.5129787234042595</v>
       </c>
@@ -4963,7 +4949,7 @@
       </c>
     </row>
     <row r="21" spans="1:30" ht="15" customHeight="1">
-      <c r="A21" s="156" t="str">
+      <c r="A21" s="147" t="str">
         <f ca="1">IF(B30=" ",IF(C6&gt;2000," ",IF((C6&gt;200)*(C6&lt;400),C6,A21)),326.8)</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -4990,12 +4976,12 @@
         <f t="shared" si="6"/>
         <v>1.3356251232776345E-2</v>
       </c>
-      <c r="I21" s="152"/>
+      <c r="I21" s="161"/>
       <c r="J21" s="77">
         <f t="shared" si="11"/>
         <v>0.90765957446808443</v>
       </c>
-      <c r="K21" s="153"/>
+      <c r="K21" s="162"/>
       <c r="L21" s="14"/>
       <c r="M21" s="12">
         <f>IF((C21&gt;100)*(B1="№")+(B1="Т"),D21+AD37,C21+AD37)</f>
@@ -5023,7 +5009,7 @@
       </c>
     </row>
     <row r="22" spans="1:30" ht="15" customHeight="1">
-      <c r="A22" s="157"/>
+      <c r="A22" s="148"/>
       <c r="B22" s="34">
         <v>204</v>
       </c>
@@ -5047,12 +5033,12 @@
         <f t="shared" si="6"/>
         <v>2.0649993312825923E-2</v>
       </c>
-      <c r="I22" s="152"/>
+      <c r="I22" s="161"/>
       <c r="J22" s="40">
         <f t="shared" si="11"/>
         <v>1.4782978723404199</v>
       </c>
-      <c r="K22" s="153"/>
+      <c r="K22" s="162"/>
       <c r="L22" s="8"/>
       <c r="M22" s="12">
         <f>IF((C22&gt;100)*(B1="№")+(B1="Т"),D22+AD38,C22+AD38)</f>
@@ -5080,7 +5066,7 @@
       </c>
     </row>
     <row r="23" spans="1:30" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A23" s="158"/>
+      <c r="A23" s="149"/>
       <c r="B23" s="33">
         <v>216</v>
       </c>
@@ -5104,7 +5090,7 @@
         <f t="shared" si="6"/>
         <v>1.4078053002724078E-2</v>
       </c>
-      <c r="I23" s="152"/>
+      <c r="I23" s="161"/>
       <c r="J23" s="77">
         <f t="shared" si="11"/>
         <v>1.0589361702127746</v>
@@ -5163,7 +5149,7 @@
         <f t="shared" si="6"/>
         <v>6.8430866206323415E-3</v>
       </c>
-      <c r="I24" s="152"/>
+      <c r="I24" s="161"/>
       <c r="J24" s="40">
         <f t="shared" si="11"/>
         <v>0.53957446808510667</v>
@@ -5367,7 +5353,7 @@
         <f ca="1">IF(C3&gt;2000," ",IF((C3&gt;400)*(C3&lt;1500),C3,B28))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C28" s="149" t="str">
+      <c r="C28" s="158" t="str">
         <f ca="1">IF(NOT(B1="R"),IF(B28=" "," ",ABS(B28-B29)),ABS(D28-D29))</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -5410,7 +5396,7 @@
         <f ca="1">IF(C4&gt;2000," ",IF((C4&gt;400)*(C4&lt;1500),C4,B29))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C29" s="150"/>
+      <c r="C29" s="159"/>
       <c r="D29" s="101" t="str">
         <f ca="1">IFERROR(IF(A18=" ",(SQRT(POWER(2*A4-(C27*A1*1000*0.8)/(A1*1000-C27),2)+(1.28*C27*A1*1000*A4)/(A1*1000-C27))+(C27*A1*1000*0.8)/(A1*1000-C27)-2*A4)/0.64,IFERROR(B29+E26*SUM(E14:E25),(-(A21-(1-1/E31)*((-(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-SQRT(((-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))*(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-4*(((A1*1000)*C27/((A1*1000)-C27))+(A1*1000))*A18)))/2))+SQRT(((A21-(1-1/E31)*((-(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-SQRT(((-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))*(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-4*(((A1*1000)*C27/((A1*1000)-C27))+(A1*1000))*A18)))/2))*(A21-(1-1/E31)*((-(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-SQRT(((-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))*(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-4*(((A1*1000)*C27/((A1*1000)-C27))+(A1*1000))*A18)))/2))+4*((E31-1)/(E31*E31))*A21*((-(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-SQRT(((-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))*(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-4*(((A1*1000)*C27/((A1*1000)-C27))+(A1*1000))*A18)))/2))))/(2*((E31-1)/(E31*E31)))))," ")</f>
         <v xml:space="preserve"> </v>
@@ -5450,7 +5436,7 @@
         <f ca="1">IF(C5&gt;400," ",IF((C5&gt;100)*(C5&lt;250),C5,B30))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C30" s="151" t="str">
+      <c r="C30" s="160" t="str">
         <f ca="1">IF(NOT(B1="R"),IF(B30=" "," ",ABS(B30-B31)),ABS(D30-D31))</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -5493,7 +5479,7 @@
         <f ca="1">IF(C6&gt;400," ",IF((C6&gt;100)*(C6&lt;250),C6,B31))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C31" s="150"/>
+      <c r="C31" s="159"/>
       <c r="D31" s="120" t="str">
         <f ca="1">IFERROR(IFERROR(IF(NOT(B1="R"),B31+E26*SUM(E14:E16),IF(A18=" ",D29/5,D29/E31)),D29/E31)," ")</f>
         <v xml:space="preserve"> </v>
@@ -6024,11 +6010,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A7:A9"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="C28:C29"/>
     <mergeCell ref="C30:C31"/>
@@ -6039,6 +6020,11 @@
     <mergeCell ref="K12:K15"/>
     <mergeCell ref="K20:K22"/>
     <mergeCell ref="H1:I1"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A9"/>
   </mergeCells>
   <conditionalFormatting sqref="I3:I10">
     <cfRule type="cellIs" dxfId="117" priority="460" operator="lessThan">

</xml_diff>

<commit_message>
rename addin  to V2
</commit_message>
<xml_diff>
--- a/applications/VBA/_3д_1_Ц.xlsx
+++ b/applications/VBA/_3д_1_Ц.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" codeName="ЭтаКнига" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="300" yWindow="4530" windowWidth="14805" windowHeight="5745"/>
@@ -12,12 +12,12 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$1:$X$32</definedName>
   </definedNames>
-  <calcPr calcId="125725" iterate="1" iterateCount="1"/>
+  <calcPr calcId="124519" iterate="1" iterateCount="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
   <si>
     <t>О</t>
   </si>
@@ -26,6 +26,9 @@
   </si>
   <si>
     <t>У</t>
+  </si>
+  <si>
+    <t>Линейность</t>
   </si>
   <si>
     <t>Разница</t>
@@ -67,7 +70,37 @@
     <t>£</t>
   </si>
   <si>
+    <t>НГД</t>
+  </si>
+  <si>
     <t>№</t>
+  </si>
+  <si>
+    <t>Х</t>
+  </si>
+  <si>
+    <t>COM3</t>
+  </si>
+  <si>
+    <t>Ж/R[1|2]</t>
+  </si>
+  <si>
+    <t>И/R[2|3]</t>
+  </si>
+  <si>
+    <t>З/R1</t>
+  </si>
+  <si>
+    <t>К/R3</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>R[2|5]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -78,7 +111,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -306,14 +339,6 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -631,7 +656,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="165">
+  <cellXfs count="173">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -652,20 +677,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -741,9 +752,6 @@
     <xf numFmtId="164" fontId="18" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -753,16 +761,7 @@
     <xf numFmtId="2" fontId="10" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="15" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="15" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -772,9 +771,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="11" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="11" fillId="8" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -836,15 +832,6 @@
     <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="21" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -978,10 +965,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="23" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1007,12 +990,66 @@
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="20" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1040,37 +1077,160 @@
     <xf numFmtId="2" fontId="2" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="20" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Процентный" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="118">
+  <dxfs count="134">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2236,10 +2396,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="9.5949478026902763E-2"/>
-          <c:y val="3.0407576263407985E-2"/>
+          <c:x val="7.7352263359077134E-2"/>
+          <c:y val="2.3520986174312187E-2"/>
           <c:w val="0.83101021525844065"/>
-          <c:h val="0.92240676091667195"/>
+          <c:h val="0.92240676091667173"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2302,28 +2462,28 @@
                   <c:v>12.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.48</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.19</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.799999999999999</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.85</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.459999999999999</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.5100000000000016</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.66</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.18</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2399,19 +2559,19 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>8.18</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.740000000000002</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.2199999999999989</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.82</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
-                  <c:v>6.2299999999999969</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2475,31 +2635,31 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>6.2299999999999969</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.3500000000000014</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.509999999999998</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.4400000000000048</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.35000000000000853</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-2.2900000000000063</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-3.2400000000000091</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-4.0900000000000034</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-4.5299999999999869</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2555,7 +2715,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>А</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2619,7 +2779,7 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>8.18</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2651,7 +2811,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>-3</c:v>
+                  <c:v>Б</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2674,8 +2834,8 @@
               <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-7.7082901385847578E-3"/>
-                  <c:y val="-3.7230948225716813E-2"/>
+                  <c:x val="-7.7082901385847596E-3"/>
+                  <c:y val="-3.7230948225716827E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -2723,7 +2883,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>6.2299999999999969</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2755,7 +2915,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>-4</c:v>
+                  <c:v>В</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2826,7 +2986,7 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>-4.5299999999999869</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3155,11 +3315,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:axId val="176237568"/>
-        <c:axId val="177069056"/>
+        <c:axId val="77497088"/>
+        <c:axId val="77499008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="176237568"/>
+        <c:axId val="77497088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3185,19 +3345,19 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.38193271256707267"/>
+              <c:x val="0.38193271256707273"/>
               <c:y val="0.95763807011034663"/>
             </c:manualLayout>
           </c:layout>
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
-        <c:tickLblPos val="none"/>
-        <c:crossAx val="177069056"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="77499008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="177069056"/>
+        <c:axId val="77499008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="240"/>
@@ -3235,7 +3395,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="176237568"/>
+        <c:crossAx val="77497088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="12"/>
@@ -3760,7 +3920,7 @@
   <dimension ref="A1:AD49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScaleSheetLayoutView="110" workbookViewId="0">
-      <selection activeCell="AA14" sqref="AA14"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3775,7 +3935,7 @@
     <col min="8" max="8" width="8.28515625" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="7.5703125" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="8.7109375" customWidth="1"/>
-    <col min="11" max="11" width="7.7109375" style="27" customWidth="1"/>
+    <col min="11" max="11" width="7.7109375" style="19" customWidth="1"/>
     <col min="13" max="13" width="9.140625" style="6"/>
     <col min="14" max="14" width="5.28515625" customWidth="1"/>
     <col min="15" max="15" width="11.28515625" customWidth="1"/>
@@ -3785,109 +3945,110 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A1" s="143" t="str">
-        <f ca="1">IF(B30=" ",IF((C8&gt;3)*(C8&lt;15),C8,IF(C8&gt;2000," ",A1)),IF(ABS(560-((B28-B30)*A4/(B28-B30+A4)+B30+(B29-B31)*A21/(B29-B31+A21)+B31)*3300/(((B28-B30)*A4/(B28-B30+A4)+B30+(B29-B31)*A21/(B29-B31+A21)+B31)+3300))&lt;ABS(560-((B28-B30)*A4/(B28-B30+A4)+B30+(B29-B31)*A21/(B29-B31+A21)+B31)*6800/(((B28-B30)*A4/(B28-B30+A4)+B30+(B29-B31)*A21/(B29-B31+A21)+B31)+6800)),3.3,IF(ABS(((B28-B30)*A4/(B28-B30+A4)+B30+(B29-B31)*A21/(B29-B31+A21)+B31)*6800/(((B28-B30)*A4/(B28-B30+A4)+B30+(B29-B31)*A21/(B29-B31+A21)+B31)+6800)-560)&lt;ABS(((B28-B30)*A4/(B28-B30+A4)+B30+(B29-B31)*A21/(B29-B31+A21)+B31)*12000/(((B28-B30)*A4/(B28-B30+A4)+B30+(B29-B31)*A21/(B29-B31+A21)+B31)+12000)-560),6.8,12)))</f>
+      <c r="A1" s="125" t="str">
+        <f>IF(B30=" ",IF((C8&gt;3)*(C8&lt;15),C8,IF(C8&gt;2000," ",A1)),IF(ABS(560-((B28-B30)*A4/(B28-B30+A4)+B30+(B29-B31)*A21/(B29-B31+A21)+B31)*3300/(((B28-B30)*A4/(B28-B30+A4)+B30+(B29-B31)*A21/(B29-B31+A21)+B31)+3300))&lt;ABS(560-((B28-B30)*A4/(B28-B30+A4)+B30+(B29-B31)*A21/(B29-B31+A21)+B31)*6800/(((B28-B30)*A4/(B28-B30+A4)+B30+(B29-B31)*A21/(B29-B31+A21)+B31)+6800)),3.3,IF(ABS(((B28-B30)*A4/(B28-B30+A4)+B30+(B29-B31)*A21/(B29-B31+A21)+B31)*6800/(((B28-B30)*A4/(B28-B30+A4)+B30+(B29-B31)*A21/(B29-B31+A21)+B31)+6800)-560)&lt;ABS(((B28-B30)*A4/(B28-B30+A4)+B30+(B29-B31)*A21/(B29-B31+A21)+B31)*12000/(((B28-B30)*A4/(B28-B30+A4)+B30+(B29-B31)*A21/(B29-B31+A21)+B31)+12000)-560),6.8,12)))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="70"/>
+      <c r="D1" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="83"/>
-      <c r="D1" s="54" t="s">
+      <c r="F1" s="57" t="str">
+        <f>IFERROR(IF(K12&lt;0.5,"Расчёт","Расчет"),"Расчёт")</f>
+        <v>Расчет</v>
+      </c>
+      <c r="G1" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="82" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="70" t="str">
-        <f>IFERROR(IF(K12&lt;0.5,"Расчёт","Расчет"),"Расчёт")</f>
-        <v>Расчёт</v>
-      </c>
-      <c r="G1" s="69" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="156" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="164"/>
-      <c r="J1" s="156">
-        <v>0</v>
-      </c>
-      <c r="K1" s="157"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
-      <c r="W1" s="8"/>
-      <c r="X1" s="8"/>
-      <c r="Y1" s="8"/>
+      <c r="H1" s="148" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="156"/>
+      <c r="J1" s="148" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="149"/>
+      <c r="L1" s="128"/>
+      <c r="M1" s="129"/>
+      <c r="N1" s="128"/>
+      <c r="O1" s="128"/>
+      <c r="P1" s="128"/>
+      <c r="Q1" s="128"/>
+      <c r="R1" s="128"/>
+      <c r="S1" s="128"/>
+      <c r="T1" s="128"/>
+      <c r="U1" s="128"/>
+      <c r="V1" s="128"/>
+      <c r="W1" s="128"/>
+      <c r="X1" s="128"/>
+      <c r="Y1" s="130"/>
       <c r="Z1" s="8"/>
-      <c r="AA1" s="144"/>
+      <c r="AA1" s="126" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="2" spans="1:30" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="20">
+      <c r="B2" s="12">
         <v>0</v>
       </c>
-      <c r="C2" s="53">
-        <v>4.05</v>
-      </c>
-      <c r="D2" s="89" t="str">
+      <c r="C2" s="166" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="73" t="str">
         <f ca="1">IFERROR(E27/D27,IF(B1="R",E27/C27," "))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E2" s="116">
+      <c r="E2" s="100">
         <f>K3</f>
         <v>0</v>
       </c>
-      <c r="F2" s="58">
+      <c r="F2" s="46" t="str">
         <f>IF((C2&gt;2000)," ",C2*0)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G2" s="90" t="str">
+        <f>IFERROR(100/C27," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="H2" s="23">
         <v>0</v>
       </c>
-      <c r="G2" s="106" t="str">
-        <f ca="1">IFERROR(100/C27," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H2" s="31">
+      <c r="I2" s="22">
         <v>0</v>
       </c>
-      <c r="I2" s="30">
-        <v>0</v>
-      </c>
-      <c r="J2" s="57" t="s">
-        <v>3</v>
-      </c>
-      <c r="K2" s="81" t="s">
-        <v>5</v>
-      </c>
-      <c r="L2" s="8"/>
-      <c r="M2" s="10">
+      <c r="J2" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="68" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="131"/>
+      <c r="M2" s="132">
         <f>AD2</f>
         <v>12.6</v>
       </c>
-      <c r="N2" s="8"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
-      <c r="W2" s="8"/>
-      <c r="X2" s="8"/>
-      <c r="Y2" s="8"/>
+      <c r="N2" s="131"/>
+      <c r="O2" s="133"/>
+      <c r="P2" s="133"/>
+      <c r="Q2" s="131"/>
+      <c r="R2" s="131"/>
+      <c r="S2" s="131"/>
+      <c r="T2" s="131"/>
+      <c r="U2" s="131"/>
+      <c r="V2" s="131"/>
+      <c r="W2" s="131"/>
+      <c r="X2" s="131"/>
+      <c r="Y2" s="134"/>
       <c r="Z2" s="8"/>
-      <c r="AA2" s="144"/>
       <c r="AC2" s="2">
         <v>0</v>
       </c>
@@ -3896,61 +4057,60 @@
       </c>
     </row>
     <row r="3" spans="1:30" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="78" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="32">
+      <c r="A3" s="65" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="24">
         <f t="shared" ref="B3:B8" si="0">B2+12</f>
         <v>12</v>
       </c>
-      <c r="C3" s="86">
-        <v>7.88</v>
-      </c>
-      <c r="D3" s="90" t="e">
+      <c r="C3" s="167" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="74" t="e">
         <f t="shared" ref="D3:D9" ca="1" si="1">((B3-$E$26*($E$2*94/($B$28-$B$30)))/(9.4-((9.4/($B$28-$B$30))*($E$2+$E$10)*$E$26)))*($B$28-$B$30+($E$26*E2))*(($D$2-($E$27/($A$1*1000)))-((((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))*($D$2-($E$27/($A$1*1000))))/$A$4))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E3" s="71"/>
-      <c r="F3" s="59">
+      <c r="E3" s="58"/>
+      <c r="F3" s="47" t="e">
         <f t="shared" ref="F3:F9" si="2">(B3-$B$2)/($B$11-$B$2)*$C$11</f>
-        <v>4.4399999999999995</v>
-      </c>
-      <c r="G3" s="93" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G3" s="77" t="e">
         <f ca="1">C3-D3</f>
         <v>#VALUE!</v>
       </c>
-      <c r="H3" s="36">
+      <c r="H3" s="28" t="e">
         <f>J3/F3</f>
-        <v>0.77477477477477497</v>
-      </c>
-      <c r="I3" s="161">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I3" s="153" t="e">
         <f>SUM(H3:H9)/9</f>
-        <v>0.14950009533342867</v>
-      </c>
-      <c r="J3" s="40">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J3" s="32" t="e">
         <f t="shared" ref="J3:J9" si="3">ABS(C3-F3)</f>
-        <v>3.4400000000000004</v>
-      </c>
-      <c r="K3" s="43"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="12">
-        <f>IF((C3&gt;100)*((B1="№")+(B1="R"))+(B1="Т"),D3+AD3,C3+AD3)</f>
-        <v>15.48</v>
-      </c>
-      <c r="N3" s="8"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="8"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K3" s="35"/>
+      <c r="L3" s="131"/>
+      <c r="M3" s="135" t="e">
+        <f ca="1">IF((C3&gt;100)*((B1="№")+(B1="R"))+(B1="Т"),D3+AD3,C3+AD3)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N3" s="131"/>
+      <c r="O3" s="136"/>
+      <c r="P3" s="136"/>
+      <c r="Q3" s="131"/>
+      <c r="R3" s="131"/>
+      <c r="S3" s="131"/>
+      <c r="T3" s="131"/>
+      <c r="U3" s="131"/>
+      <c r="V3" s="131"/>
+      <c r="W3" s="131"/>
+      <c r="X3" s="131"/>
+      <c r="Y3" s="134"/>
       <c r="Z3" s="8"/>
-      <c r="AA3" s="144"/>
       <c r="AC3" s="1">
         <f t="shared" ref="AC3:AC8" si="4">AC2+12</f>
         <v>12</v>
@@ -3961,59 +4121,58 @@
       </c>
     </row>
     <row r="4" spans="1:30" ht="15" customHeight="1">
-      <c r="A4" s="152" t="str">
-        <f ca="1">IF(B30=" ",IF(C7&gt;2000," ",IF((C7&gt;200)*(C7&lt;400),C7,A4)),326.8)</f>
+      <c r="A4" s="162" t="str">
+        <f>IF(B30=" ",IF(C7&gt;2000," ",IF((C7&gt;200)*(C7&lt;400),C7,A4)),326.8)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="B4" s="33">
+      <c r="B4" s="25">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="C4" s="87">
-        <v>11.59</v>
-      </c>
-      <c r="D4" s="91" t="e">
+      <c r="C4" s="168" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="75" t="e">
         <f t="shared" ca="1" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="E4" s="72"/>
-      <c r="F4" s="60">
+      <c r="E4" s="59"/>
+      <c r="F4" s="48" t="e">
         <f t="shared" si="2"/>
-        <v>8.879999999999999</v>
-      </c>
-      <c r="G4" s="91" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G4" s="75" t="e">
         <f t="shared" ref="G4:G24" ca="1" si="5">C4-D4</f>
         <v>#VALUE!</v>
       </c>
-      <c r="H4" s="37">
+      <c r="H4" s="29" t="e">
         <f t="shared" ref="H4:H25" si="6">J4/F4</f>
-        <v>0.30518018018018028</v>
-      </c>
-      <c r="I4" s="161"/>
-      <c r="J4" s="77">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I4" s="153"/>
+      <c r="J4" s="64" t="e">
         <f t="shared" si="3"/>
-        <v>2.7100000000000009</v>
-      </c>
-      <c r="K4" s="44"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="12">
-        <f>IF((C4&gt;100)*((B1="№")+(B1="R"))+(B1="Т"),D4+AD4,C4+AD4)</f>
-        <v>14.19</v>
-      </c>
-      <c r="N4" s="8"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
-      <c r="U4" s="8"/>
-      <c r="V4" s="8"/>
-      <c r="W4" s="8"/>
-      <c r="X4" s="8"/>
-      <c r="Y4" s="8"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K4" s="36"/>
+      <c r="L4" s="131"/>
+      <c r="M4" s="135" t="e">
+        <f ca="1">IF((C4&gt;100)*((B1="№")+(B1="R"))+(B1="Т"),D4+AD4,C4+AD4)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N4" s="131"/>
+      <c r="O4" s="136"/>
+      <c r="P4" s="136"/>
+      <c r="Q4" s="131"/>
+      <c r="R4" s="131"/>
+      <c r="S4" s="131"/>
+      <c r="T4" s="131"/>
+      <c r="U4" s="131"/>
+      <c r="V4" s="131"/>
+      <c r="W4" s="131"/>
+      <c r="X4" s="131"/>
+      <c r="Y4" s="134"/>
       <c r="Z4" s="8"/>
-      <c r="AA4" s="144"/>
       <c r="AC4" s="1">
         <f t="shared" si="4"/>
         <v>24</v>
@@ -4024,59 +4183,58 @@
       </c>
     </row>
     <row r="5" spans="1:30" ht="15" customHeight="1">
-      <c r="A5" s="153"/>
-      <c r="B5" s="34">
+      <c r="A5" s="163"/>
+      <c r="B5" s="26">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="C5" s="86">
-        <v>15.2</v>
-      </c>
-      <c r="D5" s="90" t="e">
+      <c r="C5" s="167" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="74" t="e">
         <f t="shared" ca="1" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="E5" s="71"/>
-      <c r="F5" s="59">
+      <c r="E5" s="58"/>
+      <c r="F5" s="47" t="e">
         <f t="shared" si="2"/>
-        <v>13.32</v>
-      </c>
-      <c r="G5" s="93" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G5" s="77" t="e">
         <f t="shared" ca="1" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H5" s="36">
+      <c r="H5" s="28" t="e">
         <f t="shared" si="6"/>
-        <v>0.14114114114114107</v>
-      </c>
-      <c r="I5" s="161"/>
-      <c r="J5" s="40">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I5" s="153"/>
+      <c r="J5" s="32" t="e">
         <f t="shared" si="3"/>
-        <v>1.879999999999999</v>
-      </c>
-      <c r="K5" s="162">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K5" s="154" t="str">
         <f>IFERROR(IF(MAX(J3:J9)&gt;10,"FAIL",MAX(J3:J9)),"∆ОА=")</f>
-        <v>3.4400000000000004</v>
-      </c>
-      <c r="L5" s="8"/>
-      <c r="M5" s="12">
-        <f>IF((C5&gt;100)*((B1="№")+(B1="R"))+(B1="Т"),D5+AD5,C5+AD5)</f>
-        <v>12.799999999999999</v>
-      </c>
-      <c r="N5" s="8"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
-      <c r="U5" s="8"/>
-      <c r="V5" s="8"/>
-      <c r="W5" s="8"/>
-      <c r="X5" s="8"/>
-      <c r="Y5" s="8"/>
+        <v>∆ОА=</v>
+      </c>
+      <c r="L5" s="131"/>
+      <c r="M5" s="135" t="e">
+        <f ca="1">IF((C5&gt;100)*((B1="№")+(B1="R"))+(B1="Т"),D5+AD5,C5+AD5)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N5" s="131"/>
+      <c r="O5" s="136"/>
+      <c r="P5" s="136"/>
+      <c r="Q5" s="131"/>
+      <c r="R5" s="131"/>
+      <c r="S5" s="131"/>
+      <c r="T5" s="131"/>
+      <c r="U5" s="131"/>
+      <c r="V5" s="131"/>
+      <c r="W5" s="131"/>
+      <c r="X5" s="131"/>
+      <c r="Y5" s="134"/>
       <c r="Z5" s="8"/>
-      <c r="AA5" s="144"/>
       <c r="AC5" s="1">
         <f t="shared" si="4"/>
         <v>36</v>
@@ -4087,56 +4245,55 @@
       </c>
     </row>
     <row r="6" spans="1:30" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A6" s="154"/>
-      <c r="B6" s="33">
+      <c r="A6" s="164"/>
+      <c r="B6" s="25">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="C6" s="87">
-        <v>19.25</v>
-      </c>
-      <c r="D6" s="91" t="e">
+      <c r="C6" s="168" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="75" t="e">
         <f t="shared" ca="1" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="E6" s="72"/>
-      <c r="F6" s="60">
+      <c r="E6" s="59"/>
+      <c r="F6" s="48" t="e">
         <f t="shared" si="2"/>
-        <v>17.759999999999998</v>
-      </c>
-      <c r="G6" s="91" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G6" s="75" t="e">
         <f t="shared" ca="1" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H6" s="37">
+      <c r="H6" s="29" t="e">
         <f t="shared" si="6"/>
-        <v>8.3896396396396511E-2</v>
-      </c>
-      <c r="I6" s="161"/>
-      <c r="J6" s="77">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I6" s="153"/>
+      <c r="J6" s="64" t="e">
         <f t="shared" si="3"/>
-        <v>1.490000000000002</v>
-      </c>
-      <c r="K6" s="162"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="12">
-        <f>IF(((C6&gt;100)+(C6&lt;5))*((B1="№")+(B1="R"))+(B1="Т"),D6+AD6,C6+AD6)</f>
-        <v>11.85</v>
-      </c>
-      <c r="N6" s="8"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="14"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="8"/>
-      <c r="U6" s="8"/>
-      <c r="V6" s="8"/>
-      <c r="W6" s="8"/>
-      <c r="X6" s="8"/>
-      <c r="Y6" s="8"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K6" s="154"/>
+      <c r="L6" s="137"/>
+      <c r="M6" s="135" t="e">
+        <f ca="1">IF(((C6&gt;100)+(C6&lt;5))*((B1="№")+(B1="R"))+(B1="Т"),D6+AD6,C6+AD6)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N6" s="131"/>
+      <c r="O6" s="136"/>
+      <c r="P6" s="136"/>
+      <c r="Q6" s="138"/>
+      <c r="R6" s="137"/>
+      <c r="S6" s="131"/>
+      <c r="T6" s="131"/>
+      <c r="U6" s="131"/>
+      <c r="V6" s="131"/>
+      <c r="W6" s="131"/>
+      <c r="X6" s="131"/>
+      <c r="Y6" s="134"/>
       <c r="Z6" s="8"/>
-      <c r="AA6" s="144"/>
       <c r="AC6" s="1">
         <f t="shared" si="4"/>
         <v>48</v>
@@ -4147,57 +4304,57 @@
       </c>
     </row>
     <row r="7" spans="1:30" ht="15" customHeight="1">
-      <c r="A7" s="155" t="str">
-        <f ca="1">IF((C27=" ")+(B30=" "),IF((C3&gt;200)*(C3&lt;400),C3,IF(C3&gt;2000," ",A7)),((((B28-B30)*A4/(B28-B30+A4))+B30)*(A1*1000+((B29-B31)*A21/((B29-B31)+A21))+B31))/((((B28-B30)*A4/((B28-B30)+A4))+B30)+A1*1000+((B29-B31)*A21/((B29-B31)+A21))+B31))</f>
+      <c r="A7" s="165" t="str">
+        <f>IF((C27=" ")+(B30=" "),IF((C3&gt;200)*(C3&lt;400),C3,IF(C3&gt;2000," ",A7)),((((B28-B30)*A4/(B28-B30+A4))+B30)*(A1*1000+((B29-B31)*A21/((B29-B31)+A21))+B31))/((((B28-B30)*A4/((B28-B30)+A4))+B30)+A1*1000+((B29-B31)*A21/((B29-B31)+A21))+B31))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="B7" s="34">
+      <c r="B7" s="26">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="C7" s="86">
-        <v>22.86</v>
-      </c>
-      <c r="D7" s="90" t="e">
+      <c r="C7" s="167" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="74" t="e">
         <f t="shared" ca="1" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="E7" s="71"/>
-      <c r="F7" s="59">
+      <c r="E7" s="58"/>
+      <c r="F7" s="47" t="e">
         <f t="shared" si="2"/>
-        <v>22.200000000000003</v>
-      </c>
-      <c r="G7" s="93" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G7" s="77" t="e">
         <f t="shared" ca="1" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H7" s="36">
+      <c r="H7" s="28" t="e">
         <f t="shared" si="6"/>
-        <v>2.9729729729729572E-2</v>
-      </c>
-      <c r="I7" s="161"/>
-      <c r="J7" s="40">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I7" s="153"/>
+      <c r="J7" s="32" t="e">
         <f t="shared" si="3"/>
-        <v>0.65999999999999659</v>
-      </c>
-      <c r="K7" s="162"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="12">
-        <f>IF((C7&gt;100)*((B1="№")+(B1="R"))+(B1="Т"),D7+AD7,C7+AD7)</f>
-        <v>10.459999999999999</v>
-      </c>
-      <c r="N7" s="8"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="8"/>
-      <c r="R7" s="8"/>
-      <c r="S7" s="8"/>
-      <c r="T7" s="8"/>
-      <c r="U7" s="8"/>
-      <c r="V7" s="8"/>
-      <c r="W7" s="8"/>
-      <c r="X7" s="8"/>
-      <c r="Y7" s="8"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K7" s="154"/>
+      <c r="L7" s="131"/>
+      <c r="M7" s="135" t="e">
+        <f ca="1">IF((C7&gt;100)*((B1="№")+(B1="R"))+(B1="Т"),D7+AD7,C7+AD7)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N7" s="131"/>
+      <c r="O7" s="136"/>
+      <c r="P7" s="136"/>
+      <c r="Q7" s="131"/>
+      <c r="R7" s="131"/>
+      <c r="S7" s="131"/>
+      <c r="T7" s="131"/>
+      <c r="U7" s="131"/>
+      <c r="V7" s="131"/>
+      <c r="W7" s="131"/>
+      <c r="X7" s="131"/>
+      <c r="Y7" s="134"/>
       <c r="Z7" s="8"/>
       <c r="AC7" s="1">
         <f t="shared" si="4"/>
@@ -4209,54 +4366,54 @@
       </c>
     </row>
     <row r="8" spans="1:30" ht="15" customHeight="1">
-      <c r="A8" s="155"/>
-      <c r="B8" s="33">
+      <c r="A8" s="165"/>
+      <c r="B8" s="25">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
-      <c r="C8" s="87">
-        <v>26.91</v>
-      </c>
-      <c r="D8" s="91" t="e">
+      <c r="C8" s="168" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="75" t="e">
         <f t="shared" ca="1" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="E8" s="72"/>
-      <c r="F8" s="60">
+      <c r="E8" s="59"/>
+      <c r="F8" s="48" t="e">
         <f t="shared" si="2"/>
-        <v>26.64</v>
-      </c>
-      <c r="G8" s="91" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G8" s="75" t="e">
         <f t="shared" ca="1" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H8" s="37">
+      <c r="H8" s="29" t="e">
         <f t="shared" si="6"/>
-        <v>1.0135135135135118E-2</v>
-      </c>
-      <c r="I8" s="161"/>
-      <c r="J8" s="77">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I8" s="153"/>
+      <c r="J8" s="64" t="e">
         <f t="shared" si="3"/>
-        <v>0.26999999999999957</v>
-      </c>
-      <c r="K8" s="44"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="12">
-        <f>IF(((C8&gt;100)+(C8&lt;15))*((B1="№")+(B1="R"))+(B1="Т"),D8+AD8,C8+AD8)</f>
-        <v>9.5100000000000016</v>
-      </c>
-      <c r="N8" s="8"/>
-      <c r="O8" s="13"/>
-      <c r="P8" s="13"/>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="8"/>
-      <c r="T8" s="8"/>
-      <c r="U8" s="8"/>
-      <c r="V8" s="8"/>
-      <c r="W8" s="8"/>
-      <c r="X8" s="8"/>
-      <c r="Y8" s="8"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K8" s="36"/>
+      <c r="L8" s="131"/>
+      <c r="M8" s="135" t="e">
+        <f ca="1">IF(((C8&gt;100)+(C8&lt;15))*((B1="№")+(B1="R"))+(B1="Т"),D8+AD8,C8+AD8)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N8" s="131"/>
+      <c r="O8" s="136"/>
+      <c r="P8" s="136"/>
+      <c r="Q8" s="131"/>
+      <c r="R8" s="131"/>
+      <c r="S8" s="131"/>
+      <c r="T8" s="131"/>
+      <c r="U8" s="131"/>
+      <c r="V8" s="131"/>
+      <c r="W8" s="131"/>
+      <c r="X8" s="131"/>
+      <c r="Y8" s="134"/>
       <c r="Z8" s="8"/>
       <c r="AC8" s="1">
         <f t="shared" si="4"/>
@@ -4268,54 +4425,54 @@
       </c>
     </row>
     <row r="9" spans="1:30" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A9" s="155"/>
-      <c r="B9" s="35">
+      <c r="A9" s="165"/>
+      <c r="B9" s="27">
         <f>B8+12</f>
         <v>84</v>
       </c>
-      <c r="C9" s="88">
-        <v>31.06</v>
-      </c>
-      <c r="D9" s="90" t="e">
+      <c r="C9" s="169" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="74" t="e">
         <f t="shared" ca="1" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="E9" s="71"/>
-      <c r="F9" s="59">
+      <c r="E9" s="58"/>
+      <c r="F9" s="47" t="e">
         <f t="shared" si="2"/>
-        <v>31.08</v>
-      </c>
-      <c r="G9" s="93" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G9" s="77" t="e">
         <f t="shared" ca="1" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H9" s="36">
+      <c r="H9" s="28" t="e">
         <f t="shared" si="6"/>
-        <v>6.4350064350062982E-4</v>
-      </c>
-      <c r="I9" s="161"/>
-      <c r="J9" s="40">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I9" s="153"/>
+      <c r="J9" s="32" t="e">
         <f t="shared" si="3"/>
-        <v>1.9999999999999574E-2</v>
-      </c>
-      <c r="K9" s="44"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="12">
-        <f>IF(((C9&gt;100)+(C9&lt;5))*((B1="№")+(B1="R"))+(B1="Т"),D9+AD9,C9+AD9)</f>
-        <v>8.66</v>
-      </c>
-      <c r="N9" s="8"/>
-      <c r="O9" s="13"/>
-      <c r="P9" s="13"/>
-      <c r="Q9" s="8"/>
-      <c r="R9" s="8"/>
-      <c r="S9" s="8"/>
-      <c r="T9" s="8"/>
-      <c r="U9" s="8"/>
-      <c r="V9" s="8"/>
-      <c r="W9" s="8"/>
-      <c r="X9" s="8"/>
-      <c r="Y9" s="8"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K9" s="36"/>
+      <c r="L9" s="131"/>
+      <c r="M9" s="135" t="e">
+        <f ca="1">IF(((C9&gt;100)+(C9&lt;5))*((B1="№")+(B1="R"))+(B1="Т"),D9+AD9,C9+AD9)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N9" s="131"/>
+      <c r="O9" s="136"/>
+      <c r="P9" s="136"/>
+      <c r="Q9" s="131"/>
+      <c r="R9" s="131"/>
+      <c r="S9" s="131"/>
+      <c r="T9" s="131"/>
+      <c r="U9" s="131"/>
+      <c r="V9" s="131"/>
+      <c r="W9" s="131"/>
+      <c r="X9" s="131"/>
+      <c r="Y9" s="134"/>
       <c r="Z9" s="8"/>
       <c r="AC9" s="1">
         <f>AC8+12</f>
@@ -4327,104 +4484,104 @@
       </c>
     </row>
     <row r="10" spans="1:30" ht="15.75" hidden="1" customHeight="1" thickBot="1">
-      <c r="A10" s="50"/>
-      <c r="B10" s="61"/>
-      <c r="C10" s="62">
+      <c r="A10" s="41"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="170" t="str">
         <f>IF($B$11=94,$C$11,$C$10)</f>
-        <v>34.78</v>
-      </c>
-      <c r="D10" s="131" t="e">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D10" s="115" t="e">
         <f ca="1">(((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))*($D$2-($E$27/($A$1*1000))))*10</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E10" s="73">
+      <c r="E10" s="60">
         <f>K8</f>
         <v>0</v>
       </c>
-      <c r="F10" s="63"/>
-      <c r="G10" s="94"/>
-      <c r="H10" s="36" t="e">
+      <c r="F10" s="50"/>
+      <c r="G10" s="78"/>
+      <c r="H10" s="28" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I10" s="64"/>
-      <c r="J10" s="65"/>
-      <c r="K10" s="66"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="13"/>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="8"/>
-      <c r="R10" s="8"/>
-      <c r="S10" s="8"/>
-      <c r="T10" s="8"/>
-      <c r="U10" s="8"/>
-      <c r="V10" s="8"/>
-      <c r="W10" s="8"/>
-      <c r="X10" s="8"/>
-      <c r="Y10" s="8"/>
+      <c r="I10" s="51"/>
+      <c r="J10" s="52"/>
+      <c r="K10" s="53"/>
+      <c r="L10" s="131"/>
+      <c r="M10" s="135"/>
+      <c r="N10" s="131"/>
+      <c r="O10" s="136"/>
+      <c r="P10" s="136"/>
+      <c r="Q10" s="131"/>
+      <c r="R10" s="131"/>
+      <c r="S10" s="131"/>
+      <c r="T10" s="131"/>
+      <c r="U10" s="131"/>
+      <c r="V10" s="131"/>
+      <c r="W10" s="131"/>
+      <c r="X10" s="131"/>
+      <c r="Y10" s="134"/>
       <c r="Z10" s="8"/>
       <c r="AC10" s="1"/>
     </row>
     <row r="11" spans="1:30" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A11" s="47">
+      <c r="A11" s="39" t="str">
         <f>IFERROR(IF((K5&gt;K11)+(K12&gt;K17),IF((K5-K11)&gt;(K12-K17),IF(SUM(F3:F9)&lt;SUM(C3:C9),IF((K5-K11)*5&lt;1,1,IF((K5-K11)*5&gt;3,3,(K5-K11)*5)),IF((K5-K11)*5&lt;1,-1,IF((K5-K11)*5&gt;3,-3,-(K5-K11)*5))),IF(SUM(F12:F15)&lt;SUM(C12:C15),IF((K12-K17)*5&lt;1,-1,IF((K12-K17)*5&gt;3,-3,-(K12-K17)*5)),IF((K12-K17)*5&lt;1,1,IF((K12-K17)*5&gt;3,3,(K12-K17)*5)))),"А"),"А")</f>
-        <v>3</v>
-      </c>
-      <c r="B11" s="20">
+        <v>А</v>
+      </c>
+      <c r="B11" s="12">
         <v>94</v>
       </c>
-      <c r="C11" s="53">
-        <v>34.78</v>
-      </c>
-      <c r="D11" s="123" t="str">
-        <f ca="1">IFERROR(IF((B11-$E$26*($E$2*94/($B$28-$B$30)))&gt;94,((B11-$E$26*($E$2*94/($B$28-$B$30)))-94)/(2.4-(2.4*$E$26*($E$11+$E$13)/$B$30))*($B$30+$E$11*$E$26)*($D$2-($E$27/($A$1*1000)))+(((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))*($D$2-($E$27/($A$1*1000))))*10,(((B11-$E$26*($E$2*94/($B$28-$B$30)))/(9.4-((9.4/($B$28-$B$30))*($E$2+$E$10)*$E$26)))*($B$28-$B$30+($E$26*E9))*(($D$2-($E$27/($A$1*1000)))-((((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))*($D$2-($E$27/($A$1*1000))))/$A$4))))," ")</f>
+      <c r="C11" s="166" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="107" t="str">
+        <f>IFERROR(IF((B11-$E$26*($E$2*94/($B$28-$B$30)))&gt;94,((B11-$E$26*($E$2*94/($B$28-$B$30)))-94)/(2.4-(2.4*$E$26*($E$11+$E$13)/$B$30))*($B$30+$E$11*$E$26)*($D$2-($E$27/($A$1*1000)))+(((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))*($D$2-($E$27/($A$1*1000))))*10,(((B11-$E$26*($E$2*94/($B$28-$B$30)))/(9.4-((9.4/($B$28-$B$30))*($E$2+$E$10)*$E$26)))*($B$28-$B$30+($E$26*E9))*(($D$2-($E$27/($A$1*1000)))-((((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))*($D$2-($E$27/($A$1*1000))))/$A$4))))," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E11" s="116">
+      <c r="E11" s="100">
         <f>K9</f>
         <v>0</v>
       </c>
-      <c r="F11" s="58">
+      <c r="F11" s="46" t="str">
         <f>IF(C11=" "," ",C11)</f>
-        <v>34.78</v>
-      </c>
-      <c r="G11" s="92" t="str">
-        <f ca="1">IFERROR(C11-D11," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H11" s="38">
+      <c r="G11" s="76" t="str">
+        <f>IFERROR(C11-D11," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="H11" s="30" t="e">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="I11" s="30">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I11" s="22">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="J11" s="39">
+      <c r="J11" s="31" t="str">
         <f>IF(F11=" "," ",IF(B1=7,(IF(($C$10&gt;(((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))*($D$2-($E$27/($A$1*1000))))*10),(94-((2.4*($C$10-((((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))*($D$2-($E$27/($A$1*1000))))*10)))/($D$30*($D$2-($E$27/($A$1*1000)))))),(94-(9.4*($C$10-((((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))*($D$2-($E$27/($A$1*1000))))*10)))/(($D$28-$D$30)*(($D$2-($E$27/($A$1*1000)))-((((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))*($D$2-($E$27/($A$1*1000))))/$A$4)))))),0))</f>
-        <v>0</v>
-      </c>
-      <c r="K11" s="80">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K11" s="67">
         <v>0.4</v>
       </c>
-      <c r="L11" s="8"/>
-      <c r="M11" s="10">
+      <c r="L11" s="131"/>
+      <c r="M11" s="132" t="e">
         <f>IF((C11&gt;100)*(B1="№")+(B1="Т"),D11+AD15,IF(B11=AC11,C11+AD11,IF(B11=AC12,C11+AD12,IF(B11=AC14,C11+AD14,IF(B11=AC15,C11+AD15,IF(B11=AC17,C11+AD17,IF(B11=AC18,C11+AD18,IF(B11=AC19,C11+AD19,"ошибка"))))))))</f>
-        <v>8.18</v>
-      </c>
-      <c r="N11" s="8"/>
-      <c r="O11" s="11"/>
-      <c r="P11" s="11"/>
-      <c r="Q11" s="8"/>
-      <c r="R11" s="8"/>
-      <c r="S11" s="8"/>
-      <c r="T11" s="8"/>
-      <c r="U11" s="8"/>
-      <c r="V11" s="8"/>
-      <c r="W11" s="8"/>
-      <c r="X11" s="8"/>
-      <c r="Y11" s="8"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N11" s="131"/>
+      <c r="O11" s="133"/>
+      <c r="P11" s="133"/>
+      <c r="Q11" s="131"/>
+      <c r="R11" s="131"/>
+      <c r="S11" s="131"/>
+      <c r="T11" s="131"/>
+      <c r="U11" s="131"/>
+      <c r="V11" s="131"/>
+      <c r="W11" s="131"/>
+      <c r="X11" s="131"/>
+      <c r="Y11" s="134"/>
       <c r="Z11" s="8"/>
       <c r="AC11" s="2">
         <v>91</v>
@@ -4435,62 +4592,62 @@
       </c>
     </row>
     <row r="12" spans="1:30" ht="15" customHeight="1">
-      <c r="A12" s="151" t="str">
-        <f ca="1">IF((A7=" ")+(A18=" ")," ",ABS(A7-A18))</f>
+      <c r="A12" s="161" t="str">
+        <f>IF((A7=" ")+(A18=" ")," ",ABS(A7-A18))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="B12" s="18">
+      <c r="B12" s="10">
         <v>108</v>
       </c>
-      <c r="C12" s="55">
-        <v>40.14</v>
-      </c>
-      <c r="D12" s="124" t="e">
+      <c r="C12" s="171" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="108" t="e">
         <f ca="1">((B12-$E$26*($E$2*94/($B$28-$B$30)))-94)/(2.4-(2.4*$E$26*($E$11+$E$13)/$B$30))*($B$30+$E$11*$E$26)*($D$2-($E$27/($A$1*1000)))+(((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))*($D$2-($E$27/($A$1*1000))))*10</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E12" s="74"/>
-      <c r="F12" s="59">
+      <c r="E12" s="61"/>
+      <c r="F12" s="47" t="e">
         <f t="shared" ref="F12:F15" si="8">(B12-$B$11)/($B$17-$B$11)*($C$17-$C$11)+$C$11</f>
-        <v>40.044583333333335</v>
-      </c>
-      <c r="G12" s="93" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G12" s="77" t="e">
         <f t="shared" ca="1" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H12" s="36">
+      <c r="H12" s="28" t="e">
         <f t="shared" si="6"/>
-        <v>2.3827608811012348E-3</v>
-      </c>
-      <c r="I12" s="161">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I12" s="153" t="e">
         <f>SUM(H12,H14,H15)/5</f>
-        <v>1.3720364152971093E-3</v>
-      </c>
-      <c r="J12" s="40">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J12" s="32" t="e">
         <f>ABS(C12-F12)</f>
-        <v>9.5416666666665151E-2</v>
-      </c>
-      <c r="K12" s="163">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K12" s="155" t="str">
         <f>IFERROR(IF(MAX(J12:J15)&gt;10,"FAIL",MAX(J12:J15)),"∆АБ=")</f>
-        <v>0.15041666666666487</v>
-      </c>
-      <c r="L12" s="8"/>
-      <c r="M12" s="12">
-        <f>IF((C12&gt;100)*(B1="№")+(B1="Т"),D12+AD20,C12+AD20)</f>
-        <v>7.740000000000002</v>
-      </c>
-      <c r="N12" s="8"/>
-      <c r="O12" s="13"/>
-      <c r="P12" s="13"/>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="8"/>
-      <c r="S12" s="8"/>
-      <c r="T12" s="8"/>
-      <c r="U12" s="8"/>
-      <c r="V12" s="8"/>
-      <c r="W12" s="8"/>
-      <c r="X12" s="8"/>
-      <c r="Y12" s="8"/>
+        <v>∆АБ=</v>
+      </c>
+      <c r="L12" s="131"/>
+      <c r="M12" s="135" t="e">
+        <f ca="1">IF((C12&gt;100)*(B1="№")+(B1="Т"),D12+AD20,C12+AD20)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N12" s="131"/>
+      <c r="O12" s="136"/>
+      <c r="P12" s="136"/>
+      <c r="Q12" s="131"/>
+      <c r="R12" s="131"/>
+      <c r="S12" s="131"/>
+      <c r="T12" s="131"/>
+      <c r="U12" s="131"/>
+      <c r="V12" s="131"/>
+      <c r="W12" s="131"/>
+      <c r="X12" s="131"/>
+      <c r="Y12" s="134"/>
       <c r="Z12" s="8"/>
       <c r="AC12" s="2">
         <v>92</v>
@@ -4501,98 +4658,98 @@
       </c>
     </row>
     <row r="13" spans="1:30" ht="15" hidden="1" customHeight="1">
-      <c r="A13" s="151"/>
-      <c r="B13" s="67"/>
-      <c r="C13" s="62"/>
-      <c r="D13" s="94" t="e">
+      <c r="A13" s="161"/>
+      <c r="B13" s="54"/>
+      <c r="C13" s="170"/>
+      <c r="D13" s="78" t="e">
         <f ca="1">((((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))*($D$2-($E$27/($A$1*1000))))+$D$30*($D$2-($E$27/($A$1*1000))))*10</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E13" s="73">
+      <c r="E13" s="60">
         <f>K18</f>
         <v>0</v>
       </c>
-      <c r="F13" s="63"/>
-      <c r="G13" s="94"/>
-      <c r="H13" s="36" t="e">
+      <c r="F13" s="50"/>
+      <c r="G13" s="78"/>
+      <c r="H13" s="28" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I13" s="161"/>
-      <c r="J13" s="68">
+      <c r="I13" s="153"/>
+      <c r="J13" s="55">
         <f>ABS(C13-F13)</f>
         <v>0</v>
       </c>
-      <c r="K13" s="162"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="13"/>
-      <c r="P13" s="13"/>
-      <c r="Q13" s="8"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="8"/>
-      <c r="T13" s="8"/>
-      <c r="U13" s="8"/>
-      <c r="V13" s="8"/>
-      <c r="W13" s="8"/>
-      <c r="X13" s="8"/>
-      <c r="Y13" s="8"/>
+      <c r="K13" s="154"/>
+      <c r="L13" s="131"/>
+      <c r="M13" s="135"/>
+      <c r="N13" s="131"/>
+      <c r="O13" s="136"/>
+      <c r="P13" s="136"/>
+      <c r="Q13" s="131"/>
+      <c r="R13" s="131"/>
+      <c r="S13" s="131"/>
+      <c r="T13" s="131"/>
+      <c r="U13" s="131"/>
+      <c r="V13" s="131"/>
+      <c r="W13" s="131"/>
+      <c r="X13" s="131"/>
+      <c r="Y13" s="134"/>
       <c r="Z13" s="8"/>
       <c r="AC13" s="2"/>
       <c r="AD13" s="4"/>
     </row>
     <row r="14" spans="1:30" ht="15" customHeight="1">
-      <c r="A14" s="151"/>
-      <c r="B14" s="19">
+      <c r="A14" s="161"/>
+      <c r="B14" s="11">
         <v>120</v>
       </c>
-      <c r="C14" s="56">
-        <v>44.62</v>
-      </c>
-      <c r="D14" s="91" t="e">
-        <f ca="1">IF((B14-$E$26*($E$2*94/($B$28-$B$30)))&gt;118,((B14-$E$26*($E$2*94/($B$28-$B$30)))-118)/(2.4-(2.4*$E$26*($E$14+$E$16)/$B$31))*($B$31+E14*$E$26)*($D$2-($E$27/($A$1*1000)))+((((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))*($D$2-($E$27/($A$1*1000))))+$D$30*($D$2-($E$27/($A$1*1000))))*10,((B14-$E$26*($E$2*94/($B$28-$B$30)))-94)/(2.4-(2.4*$E$26*($E$11+$E$13)/$B$30))*($B$30+$E$12*$E$26)*($D$2-($E$27/($A$1*1000)))+(((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))*($D$2-($E$27/($A$1*1000))))*10)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E14" s="118">
+      <c r="C14" s="172" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="75" t="e">
+        <f>IF((B14-$E$26*($E$2*94/($B$28-$B$30)))&gt;118,((B14-$E$26*($E$2*94/($B$28-$B$30)))-118)/(2.4-(2.4*$E$26*($E$14+$E$16)/$B$31))*($B$31+E14*$E$26)*($D$2-($E$27/($A$1*1000)))+((((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))*($D$2-($E$27/($A$1*1000))))+$D$30*($D$2-($E$27/($A$1*1000))))*10,((B14-$E$26*($E$2*94/($B$28-$B$30)))-94)/(2.4-(2.4*$E$26*($E$11+$E$13)/$B$30))*($B$30+$E$12*$E$26)*($D$2-($E$27/($A$1*1000)))+(((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))*($D$2-($E$27/($A$1*1000))))*10)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E14" s="102">
         <f>K19</f>
         <v>0</v>
       </c>
-      <c r="F14" s="60">
+      <c r="F14" s="48" t="e">
         <f t="shared" si="8"/>
-        <v>44.557083333333331</v>
-      </c>
-      <c r="G14" s="91" t="e">
-        <f t="shared" ca="1" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H14" s="37">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G14" s="75" t="e">
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H14" s="29" t="e">
         <f t="shared" si="6"/>
-        <v>1.41204634504427E-3</v>
-      </c>
-      <c r="I14" s="161"/>
-      <c r="J14" s="77">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I14" s="153"/>
+      <c r="J14" s="64" t="e">
         <f>IF(B14=118,IF(C14&gt;D14,(118-2.4*(($C$14-$D$14)/($D$2-($E$27/($A$1*1000))))/$D$31),(118-2.4*(($C$14-$D$14)/($D$2-($E$27/($A$1*1000))))/$D$31)),ABS(C14-F14))</f>
-        <v>6.2916666666666288E-2</v>
-      </c>
-      <c r="K14" s="162"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="12">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K14" s="154"/>
+      <c r="L14" s="137"/>
+      <c r="M14" s="135" t="e">
         <f>IF((C14&gt;100)*(B1="№")+(B1="Т"),D14+AD21,C14+AD21)</f>
-        <v>7.2199999999999989</v>
-      </c>
-      <c r="N14" s="8"/>
-      <c r="O14" s="13"/>
-      <c r="P14" s="13"/>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="14"/>
-      <c r="S14" s="8"/>
-      <c r="T14" s="8"/>
-      <c r="U14" s="8"/>
-      <c r="V14" s="8"/>
-      <c r="W14" s="8"/>
-      <c r="X14" s="8"/>
-      <c r="Y14" s="8"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N14" s="131"/>
+      <c r="O14" s="136"/>
+      <c r="P14" s="136"/>
+      <c r="Q14" s="138"/>
+      <c r="R14" s="137"/>
+      <c r="S14" s="131"/>
+      <c r="T14" s="131"/>
+      <c r="U14" s="131"/>
+      <c r="V14" s="131"/>
+      <c r="W14" s="131"/>
+      <c r="X14" s="131"/>
+      <c r="Y14" s="134"/>
       <c r="Z14" s="8"/>
       <c r="AC14" s="2">
         <v>93</v>
@@ -4603,53 +4760,53 @@
       </c>
     </row>
     <row r="15" spans="1:30" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A15" s="151"/>
-      <c r="B15" s="18">
+      <c r="A15" s="161"/>
+      <c r="B15" s="10">
         <v>132</v>
       </c>
-      <c r="C15" s="55">
-        <v>49.22</v>
-      </c>
-      <c r="D15" s="125" t="e">
+      <c r="C15" s="171" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="109" t="e">
         <f ca="1">((B15-$E$26*($E$2*94/($B$28-$B$30)))-118)/(2.4-(2.4*$E$26*($E$14+$E$16)/$B$31))*($B$31+E14*$E$26)*($D$2-($E$27/($A$1*1000)))+((((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))*($D$2-($E$27/($A$1*1000))))+$D$30*($D$2-($E$27/($A$1*1000))))*10</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E15" s="71"/>
-      <c r="F15" s="59">
+      <c r="E15" s="58"/>
+      <c r="F15" s="47" t="e">
         <f t="shared" si="8"/>
-        <v>49.069583333333334</v>
-      </c>
-      <c r="G15" s="93" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G15" s="77" t="e">
         <f t="shared" ca="1" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H15" s="36">
+      <c r="H15" s="28" t="e">
         <f t="shared" si="6"/>
-        <v>3.0653748503400415E-3</v>
-      </c>
-      <c r="I15" s="161"/>
-      <c r="J15" s="40">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I15" s="153"/>
+      <c r="J15" s="32" t="e">
         <f>ABS(C15-F15)</f>
-        <v>0.15041666666666487</v>
-      </c>
-      <c r="K15" s="162"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="12">
-        <f>IF((C15&gt;100)*(B1="№")+(B1="Т"),D15+AD22,C15+AD22)</f>
-        <v>6.82</v>
-      </c>
-      <c r="N15" s="8"/>
-      <c r="O15" s="13"/>
-      <c r="P15" s="13"/>
-      <c r="Q15" s="8"/>
-      <c r="R15" s="8"/>
-      <c r="S15" s="8"/>
-      <c r="T15" s="8"/>
-      <c r="U15" s="8"/>
-      <c r="V15" s="8"/>
-      <c r="W15" s="8"/>
-      <c r="X15" s="8"/>
-      <c r="Y15" s="8"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K15" s="154"/>
+      <c r="L15" s="131"/>
+      <c r="M15" s="135" t="e">
+        <f ca="1">IF((C15&gt;100)*(B1="№")+(B1="Т"),D15+AD22,C15+AD22)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N15" s="131"/>
+      <c r="O15" s="136"/>
+      <c r="P15" s="136"/>
+      <c r="Q15" s="131"/>
+      <c r="R15" s="131"/>
+      <c r="S15" s="131"/>
+      <c r="T15" s="131"/>
+      <c r="U15" s="131"/>
+      <c r="V15" s="131"/>
+      <c r="W15" s="131"/>
+      <c r="X15" s="131"/>
+      <c r="Y15" s="134"/>
       <c r="Z15" s="8"/>
       <c r="AC15" s="2">
         <v>94</v>
@@ -4660,105 +4817,105 @@
       </c>
     </row>
     <row r="16" spans="1:30" ht="15.75" hidden="1" customHeight="1" thickBot="1">
-      <c r="A16" s="49"/>
-      <c r="B16" s="67"/>
-      <c r="C16" s="62">
+      <c r="A16" s="127"/>
+      <c r="B16" s="54"/>
+      <c r="C16" s="170" t="str">
         <f>IF($B$17=142,$C$17,$C$16)</f>
-        <v>52.83</v>
-      </c>
-      <c r="D16" s="131" t="e">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D16" s="115" t="e">
         <f ca="1">((((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))+$D$30+$D$31)*($D$2-($E$27/($A$1*1000))))*10</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E16" s="73">
+      <c r="E16" s="60">
         <f>K23</f>
         <v>0</v>
       </c>
-      <c r="F16" s="63"/>
-      <c r="G16" s="94"/>
-      <c r="H16" s="36" t="e">
+      <c r="F16" s="50"/>
+      <c r="G16" s="78"/>
+      <c r="H16" s="28" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I16" s="64"/>
-      <c r="J16" s="65"/>
-      <c r="K16" s="48"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="13"/>
-      <c r="P16" s="13"/>
-      <c r="Q16" s="8"/>
-      <c r="R16" s="8"/>
-      <c r="S16" s="8"/>
-      <c r="T16" s="8"/>
-      <c r="U16" s="8"/>
-      <c r="V16" s="8"/>
-      <c r="W16" s="8"/>
-      <c r="X16" s="8"/>
-      <c r="Y16" s="8"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="52"/>
+      <c r="K16" s="40"/>
+      <c r="L16" s="131"/>
+      <c r="M16" s="135"/>
+      <c r="N16" s="131"/>
+      <c r="O16" s="136"/>
+      <c r="P16" s="136"/>
+      <c r="Q16" s="131"/>
+      <c r="R16" s="131"/>
+      <c r="S16" s="131"/>
+      <c r="T16" s="131"/>
+      <c r="U16" s="131"/>
+      <c r="V16" s="131"/>
+      <c r="W16" s="131"/>
+      <c r="X16" s="131"/>
+      <c r="Y16" s="134"/>
       <c r="Z16" s="8"/>
       <c r="AC16" s="2"/>
       <c r="AD16" s="4"/>
     </row>
     <row r="17" spans="1:30" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A17" s="47">
+      <c r="A17" s="39" t="str">
         <f>IFERROR(IF((K12&gt;K17)+(K20&gt;K25),IF((K12-K17)&gt;(K20-K25),IF(SUM(F12:F15)&lt;SUM(C12:C15),IF((K12-K17)*5&lt;1,-1,IF((K12-K17)*5&gt;3,-3,-(K12-K17)*5)),IF((K12-K17)*5&lt;1,1,IF((K12-K17)*5&gt;3,3,(K12-K17)*5))),IF(SUM(F18:F24)&lt;SUM(C18:C24),IF((K20-K25)*5&lt;1,1,IF((K20-K25)*5+1&gt;3,3,(K20-K25)*5+1)),IF((K20-K25)*5&lt;1,-1,IF((K20-K25)*5+1&gt;3,-3,-(K20-K25)*5-1)))),"Б"),"Б")</f>
-        <v>-3</v>
-      </c>
-      <c r="B17" s="29">
+        <v>Б</v>
+      </c>
+      <c r="B17" s="21">
         <v>142</v>
       </c>
-      <c r="C17" s="53">
-        <v>52.83</v>
-      </c>
-      <c r="D17" s="123" t="str">
-        <f ca="1">IFERROR(IF((B17-$E$26*($E$2*94/($B$28-$B$30)))&gt;142,((B17-$E$26*($E$2*94/($B$28-$B$30)))-142)/(9.4-(9.4*$E$26*($E$17+$E$25)/($B$29-$B$31)))*($B$29-$B$31+E17*$E$26)*(($D$2-($E$27/($A$1*1000)))-((((($D$29-$D$31)*$A$21)/($D$29-$D$31+$A$21))*($D$2-($E$27/($A$1*1000))))/$A$21))+((((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))+$D$30+$D$31)*($D$2-($E$27/($A$1*1000))))*10,((B17-$E$26*($E$2*94/($B$28-$B$30)))-118)/(2.4-(2.4*$E$26*($E$14+$E$16)/$B$31))*($B$31+E15*$E$26)*($D$2-($E$27/($A$1*1000)))+((((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))*($D$2-($E$27/($A$1*1000))))+$D$30*($D$2-($E$27/($A$1*1000))))*10)," ")</f>
+      <c r="C17" s="166" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="107" t="str">
+        <f>IFERROR(IF((B17-$E$26*($E$2*94/($B$28-$B$30)))&gt;142,((B17-$E$26*($E$2*94/($B$28-$B$30)))-142)/(9.4-(9.4*$E$26*($E$17+$E$25)/($B$29-$B$31)))*($B$29-$B$31+E17*$E$26)*(($D$2-($E$27/($A$1*1000)))-((((($D$29-$D$31)*$A$21)/($D$29-$D$31+$A$21))*($D$2-($E$27/($A$1*1000))))/$A$21))+((((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))+$D$30+$D$31)*($D$2-($E$27/($A$1*1000))))*10,((B17-$E$26*($E$2*94/($B$28-$B$30)))-118)/(2.4-(2.4*$E$26*($E$14+$E$16)/$B$31))*($B$31+E15*$E$26)*($D$2-($E$27/($A$1*1000)))+((((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))*($D$2-($E$27/($A$1*1000))))+$D$30*($D$2-($E$27/($A$1*1000))))*10)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E17" s="116">
+      <c r="E17" s="100">
         <f>K24</f>
         <v>0</v>
       </c>
-      <c r="F17" s="58">
+      <c r="F17" s="46" t="str">
         <f>IF(C17=" "," ",C17)</f>
-        <v>52.83</v>
-      </c>
-      <c r="G17" s="92" t="str">
-        <f ca="1">IFERROR(C17-D17," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H17" s="38">
+      <c r="G17" s="76" t="str">
+        <f>IFERROR(C17-D17," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="H17" s="30" t="e">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="I17" s="30">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I17" s="22">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="J17" s="39">
+      <c r="J17" s="31" t="str">
         <f>IF(F17=" "," ",IF(B1=7,IF(($C$16&gt;(((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))+$D$30+$D$31)*($D$2-($E$27/($A$1*1000)))*10),(142-(9.4*($C$16-(((((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))+$D$30+$D$31)*($D$2-($E$27/($A$1*1000))))*10))/(($D$29-$D$31)*(($D$2-($E$27/($A$1*1000)))-((((($D$29-$D$31)*$A$21)/($D$29-$D$31+$A$21))*($D$2-($E$27/($A$1*1000))))/$A$21))))),(142-(2.4*($C$16-(((((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))+$D$30+$D$31)*($D$2-($E$27/($A$1*1000))))*10))/($D$31*($D$2-($E$27/($A$1*1000))))))),0))</f>
-        <v>0</v>
-      </c>
-      <c r="K17" s="80">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K17" s="67">
         <v>0.5</v>
       </c>
-      <c r="L17" s="8"/>
-      <c r="M17" s="16">
+      <c r="L17" s="131"/>
+      <c r="M17" s="139" t="e">
         <f>IF((C17&gt;100)*(B1="№")+(B1="Т"),D17+AD26,IF(B17=AC23,C17+AD23,IF(B17=AC24,C17+AD24,IF(B17=AC25,C17+AD25,IF(B17=AC26,C17+AD26,IF(B17=AC27,C17+AD27,IF(B17=AC32,C17+AD32,IF(B17=AC33,C17+AD33,"ошибка"))))))))</f>
-        <v>6.2299999999999969</v>
-      </c>
-      <c r="N17" s="8"/>
-      <c r="O17" s="11"/>
-      <c r="P17" s="11"/>
-      <c r="Q17" s="8"/>
-      <c r="R17" s="8"/>
-      <c r="S17" s="8"/>
-      <c r="T17" s="8"/>
-      <c r="U17" s="8"/>
-      <c r="V17" s="8"/>
-      <c r="W17" s="8"/>
-      <c r="X17" s="8"/>
-      <c r="Y17" s="8"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N17" s="131"/>
+      <c r="O17" s="133"/>
+      <c r="P17" s="133"/>
+      <c r="Q17" s="131"/>
+      <c r="R17" s="131"/>
+      <c r="S17" s="131"/>
+      <c r="T17" s="131"/>
+      <c r="U17" s="131"/>
+      <c r="V17" s="131"/>
+      <c r="W17" s="131"/>
+      <c r="X17" s="131"/>
+      <c r="Y17" s="134"/>
       <c r="Z17" s="8"/>
       <c r="AC17" s="2">
         <v>95</v>
@@ -4769,59 +4926,59 @@
       </c>
     </row>
     <row r="18" spans="1:30" ht="15" customHeight="1">
-      <c r="A18" s="150" t="str">
-        <f ca="1">IF((C27=" ")+(B30=" "),IF((C4&gt;200)*(C4&lt;400),C4,IF(C4&gt;2000," ",A18)),(((B29-B31)*A21/(B29-B31+A21)+B31)*(A1*1000+(B28-B30)*A4/(B28-B30+A4)+B30))/(((B29-B31)*A21/((B29-B31)+A21)+B31)+A1*1000+(B28-B30)*A4/(B28-B30+A4)+B30))</f>
+      <c r="A18" s="160" t="str">
+        <f>IF((C27=" ")+(B30=" "),IF((C4&gt;200)*(C4&lt;400),C4,IF(C4&gt;2000," ",A18)),(((B29-B31)*A21/(B29-B31+A21)+B31)*(A1*1000+(B28-B30)*A4/(B28-B30+A4)+B30))/(((B29-B31)*A21/((B29-B31)+A21)+B31)+A1*1000+(B28-B30)*A4/(B28-B30+A4)+B30))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="B18" s="32">
+      <c r="B18" s="24">
         <v>156</v>
       </c>
-      <c r="C18" s="55">
-        <v>57.75</v>
-      </c>
-      <c r="D18" s="95" t="e">
+      <c r="C18" s="171" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="79" t="e">
         <f t="shared" ref="D18:D24" ca="1" si="9">((B18-$E$26*($E$2*94/($B$28-$B$30)))-142)/(9.4-(9.4*$E$26*($E$17+$E$25)/($B$29-$B$31)))*($B$29-$B$31+E17*$E$26)*(($D$2-($E$27/($A$1*1000)))-((((($D$29-$D$31)*$A$21)/($D$29-$D$31+$A$21))*($D$2-($E$27/($A$1*1000))))/$A$21))+((((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))+$D$30+$D$31)*($D$2-($E$27/($A$1*1000))))*10</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E18" s="75"/>
-      <c r="F18" s="59">
+      <c r="E18" s="62"/>
+      <c r="F18" s="47" t="e">
         <f t="shared" ref="F18:F24" si="10">(B18-$B$17)/($B$25-$B$17)*($C$25-$C$17)+$C$17</f>
-        <v>57.065744680851061</v>
-      </c>
-      <c r="G18" s="93" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G18" s="77" t="e">
         <f t="shared" ca="1" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H18" s="36">
+      <c r="H18" s="28" t="e">
         <f t="shared" si="6"/>
-        <v>1.1990649083364138E-2</v>
-      </c>
-      <c r="I18" s="161">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I18" s="153" t="e">
         <f>SUM(H17:H25)/9</f>
-        <v>1.2270336334577112E-2</v>
-      </c>
-      <c r="J18" s="40">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J18" s="32" t="e">
         <f t="shared" ref="J18:J24" si="11">ABS(C18-F18)</f>
-        <v>0.68425531914893867</v>
-      </c>
-      <c r="K18" s="44"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="12">
-        <f>IF((C18&gt;100)*(B1="№")+(B1="Т"),D18+AD34,C18+AD34)</f>
-        <v>5.3500000000000014</v>
-      </c>
-      <c r="N18" s="8"/>
-      <c r="O18" s="13"/>
-      <c r="P18" s="13"/>
-      <c r="Q18" s="8"/>
-      <c r="R18" s="8"/>
-      <c r="S18" s="8"/>
-      <c r="T18" s="8"/>
-      <c r="U18" s="8"/>
-      <c r="V18" s="8"/>
-      <c r="W18" s="8"/>
-      <c r="X18" s="8"/>
-      <c r="Y18" s="8"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K18" s="36"/>
+      <c r="L18" s="131"/>
+      <c r="M18" s="135" t="e">
+        <f ca="1">IF((C18&gt;100)*(B1="№")+(B1="Т"),D18+AD34,C18+AD34)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N18" s="131"/>
+      <c r="O18" s="136"/>
+      <c r="P18" s="136"/>
+      <c r="Q18" s="131"/>
+      <c r="R18" s="131"/>
+      <c r="S18" s="131"/>
+      <c r="T18" s="131"/>
+      <c r="U18" s="131"/>
+      <c r="V18" s="131"/>
+      <c r="W18" s="131"/>
+      <c r="X18" s="131"/>
+      <c r="Y18" s="134"/>
       <c r="Z18" s="8"/>
       <c r="AC18" s="3">
         <v>96</v>
@@ -4832,53 +4989,53 @@
       </c>
     </row>
     <row r="19" spans="1:30" ht="15" customHeight="1">
-      <c r="A19" s="150"/>
-      <c r="B19" s="33">
+      <c r="A19" s="160"/>
+      <c r="B19" s="25">
         <v>168</v>
       </c>
-      <c r="C19" s="56">
-        <v>61.91</v>
-      </c>
-      <c r="D19" s="133" t="e">
+      <c r="C19" s="172" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="117" t="e">
         <f t="shared" ca="1" si="9"/>
         <v>#VALUE!</v>
       </c>
-      <c r="E19" s="76"/>
-      <c r="F19" s="60">
+      <c r="E19" s="63"/>
+      <c r="F19" s="48" t="e">
         <f t="shared" si="10"/>
-        <v>60.696382978723406</v>
-      </c>
-      <c r="G19" s="91" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G19" s="75" t="e">
         <f t="shared" ca="1" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H19" s="37">
+      <c r="H19" s="29" t="e">
         <f t="shared" si="6"/>
-        <v>1.9994882095396252E-2</v>
-      </c>
-      <c r="I19" s="161"/>
-      <c r="J19" s="77">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I19" s="153"/>
+      <c r="J19" s="64" t="e">
         <f t="shared" si="11"/>
-        <v>1.2136170212765904</v>
-      </c>
-      <c r="K19" s="44"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="12">
-        <f>IF((C19&gt;100)*(B1="№")+(B1="Т"),D19+AD35,C19+AD35)</f>
-        <v>4.509999999999998</v>
-      </c>
-      <c r="N19" s="8"/>
-      <c r="O19" s="13"/>
-      <c r="P19" s="13"/>
-      <c r="Q19" s="8"/>
-      <c r="R19" s="8"/>
-      <c r="S19" s="8"/>
-      <c r="T19" s="8"/>
-      <c r="U19" s="8"/>
-      <c r="V19" s="8"/>
-      <c r="W19" s="8"/>
-      <c r="X19" s="8"/>
-      <c r="Y19" s="8"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K19" s="36"/>
+      <c r="L19" s="131"/>
+      <c r="M19" s="135" t="e">
+        <f ca="1">IF((C19&gt;100)*(B1="№")+(B1="Т"),D19+AD35,C19+AD35)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N19" s="131"/>
+      <c r="O19" s="136"/>
+      <c r="P19" s="136"/>
+      <c r="Q19" s="131"/>
+      <c r="R19" s="131"/>
+      <c r="S19" s="131"/>
+      <c r="T19" s="131"/>
+      <c r="U19" s="131"/>
+      <c r="V19" s="131"/>
+      <c r="W19" s="131"/>
+      <c r="X19" s="131"/>
+      <c r="Y19" s="134"/>
       <c r="Z19" s="8"/>
       <c r="AC19" s="2">
         <v>97</v>
@@ -4889,56 +5046,56 @@
       </c>
     </row>
     <row r="20" spans="1:30" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A20" s="150"/>
-      <c r="B20" s="34">
+      <c r="A20" s="160"/>
+      <c r="B20" s="26">
         <v>180</v>
       </c>
-      <c r="C20" s="55">
-        <v>65.84</v>
-      </c>
-      <c r="D20" s="95" t="e">
+      <c r="C20" s="171" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="79" t="e">
         <f t="shared" ca="1" si="9"/>
         <v>#VALUE!</v>
       </c>
-      <c r="E20" s="75"/>
-      <c r="F20" s="59">
+      <c r="E20" s="62"/>
+      <c r="F20" s="47" t="e">
         <f t="shared" si="10"/>
-        <v>64.327021276595744</v>
-      </c>
-      <c r="G20" s="93" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G20" s="77" t="e">
         <f t="shared" ca="1" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H20" s="36">
+      <c r="H20" s="28" t="e">
         <f t="shared" si="6"/>
-        <v>2.3520111663474931E-2</v>
-      </c>
-      <c r="I20" s="161"/>
-      <c r="J20" s="40">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I20" s="153"/>
+      <c r="J20" s="32" t="e">
         <f t="shared" si="11"/>
-        <v>1.5129787234042595</v>
-      </c>
-      <c r="K20" s="162">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K20" s="154" t="str">
         <f>IFERROR(IF(MAX(J18:J24)&gt;10,"FAIL",MAX(J18:J24)),"∆БВ=")</f>
-        <v>1.5129787234042595</v>
-      </c>
-      <c r="L20" s="8"/>
-      <c r="M20" s="12">
-        <f>IF((C20&gt;100)*(B1="№")+(B1="Т"),D20+AD36,C20+AD36)</f>
-        <v>3.4400000000000048</v>
-      </c>
-      <c r="N20" s="8"/>
-      <c r="O20" s="13"/>
-      <c r="P20" s="13"/>
-      <c r="Q20" s="8"/>
-      <c r="R20" s="8"/>
-      <c r="S20" s="8"/>
-      <c r="T20" s="8"/>
-      <c r="U20" s="8"/>
-      <c r="V20" s="8"/>
-      <c r="W20" s="8"/>
-      <c r="X20" s="8"/>
-      <c r="Y20" s="8"/>
+        <v>∆БВ=</v>
+      </c>
+      <c r="L20" s="131"/>
+      <c r="M20" s="135" t="e">
+        <f ca="1">IF((C20&gt;100)*(B1="№")+(B1="Т"),D20+AD36,C20+AD36)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N20" s="131"/>
+      <c r="O20" s="136"/>
+      <c r="P20" s="136"/>
+      <c r="Q20" s="131"/>
+      <c r="R20" s="131"/>
+      <c r="S20" s="131"/>
+      <c r="T20" s="131"/>
+      <c r="U20" s="131"/>
+      <c r="V20" s="131"/>
+      <c r="W20" s="131"/>
+      <c r="X20" s="131"/>
+      <c r="Y20" s="134"/>
       <c r="Z20" s="8"/>
       <c r="AC20" s="1">
         <v>108</v>
@@ -4949,56 +5106,56 @@
       </c>
     </row>
     <row r="21" spans="1:30" ht="15" customHeight="1">
-      <c r="A21" s="147" t="str">
-        <f ca="1">IF(B30=" ",IF(C6&gt;2000," ",IF((C6&gt;200)*(C6&lt;400),C6,A21)),326.8)</f>
+      <c r="A21" s="157" t="str">
+        <f>IF(B30=" ",IF(C6&gt;2000," ",IF((C6&gt;200)*(C6&lt;400),C6,A21)),326.8)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="B21" s="33">
+      <c r="B21" s="25">
         <v>192</v>
       </c>
-      <c r="C21" s="56">
-        <v>67.05</v>
-      </c>
-      <c r="D21" s="133" t="e">
+      <c r="C21" s="172" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="117" t="e">
         <f t="shared" ca="1" si="9"/>
         <v>#VALUE!</v>
       </c>
-      <c r="E21" s="76"/>
-      <c r="F21" s="60">
+      <c r="E21" s="63"/>
+      <c r="F21" s="48" t="e">
         <f t="shared" si="10"/>
-        <v>67.957659574468082</v>
-      </c>
-      <c r="G21" s="91" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G21" s="75" t="e">
         <f t="shared" ca="1" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H21" s="37">
+      <c r="H21" s="29" t="e">
         <f t="shared" si="6"/>
-        <v>1.3356251232776345E-2</v>
-      </c>
-      <c r="I21" s="161"/>
-      <c r="J21" s="77">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I21" s="153"/>
+      <c r="J21" s="64" t="e">
         <f t="shared" si="11"/>
-        <v>0.90765957446808443</v>
-      </c>
-      <c r="K21" s="162"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="12">
-        <f>IF((C21&gt;100)*(B1="№")+(B1="Т"),D21+AD37,C21+AD37)</f>
-        <v>-0.35000000000000853</v>
-      </c>
-      <c r="N21" s="8"/>
-      <c r="O21" s="13"/>
-      <c r="P21" s="13"/>
-      <c r="Q21" s="15"/>
-      <c r="R21" s="14"/>
-      <c r="S21" s="8"/>
-      <c r="T21" s="8"/>
-      <c r="U21" s="8"/>
-      <c r="V21" s="8"/>
-      <c r="W21" s="8"/>
-      <c r="X21" s="8"/>
-      <c r="Y21" s="8"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K21" s="154"/>
+      <c r="L21" s="137"/>
+      <c r="M21" s="135" t="e">
+        <f ca="1">IF((C21&gt;100)*(B1="№")+(B1="Т"),D21+AD37,C21+AD37)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N21" s="131"/>
+      <c r="O21" s="136"/>
+      <c r="P21" s="136"/>
+      <c r="Q21" s="138"/>
+      <c r="R21" s="137"/>
+      <c r="S21" s="131"/>
+      <c r="T21" s="131"/>
+      <c r="U21" s="131"/>
+      <c r="V21" s="131"/>
+      <c r="W21" s="131"/>
+      <c r="X21" s="131"/>
+      <c r="Y21" s="134"/>
       <c r="Z21" s="8"/>
       <c r="AC21" s="1">
         <v>120</v>
@@ -5009,53 +5166,53 @@
       </c>
     </row>
     <row r="22" spans="1:30" ht="15" customHeight="1">
-      <c r="A22" s="148"/>
-      <c r="B22" s="34">
+      <c r="A22" s="158"/>
+      <c r="B22" s="26">
         <v>204</v>
       </c>
-      <c r="C22" s="55">
-        <v>70.11</v>
-      </c>
-      <c r="D22" s="95" t="e">
+      <c r="C22" s="171" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="79" t="e">
         <f t="shared" ca="1" si="9"/>
         <v>#VALUE!</v>
       </c>
-      <c r="E22" s="75"/>
-      <c r="F22" s="59">
+      <c r="E22" s="62"/>
+      <c r="F22" s="47" t="e">
         <f t="shared" si="10"/>
-        <v>71.588297872340419</v>
-      </c>
-      <c r="G22" s="93" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G22" s="77" t="e">
         <f t="shared" ca="1" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H22" s="36">
+      <c r="H22" s="28" t="e">
         <f t="shared" si="6"/>
-        <v>2.0649993312825923E-2</v>
-      </c>
-      <c r="I22" s="161"/>
-      <c r="J22" s="40">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I22" s="153"/>
+      <c r="J22" s="32" t="e">
         <f t="shared" si="11"/>
-        <v>1.4782978723404199</v>
-      </c>
-      <c r="K22" s="162"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="12">
-        <f>IF((C22&gt;100)*(B1="№")+(B1="Т"),D22+AD38,C22+AD38)</f>
-        <v>-2.2900000000000063</v>
-      </c>
-      <c r="N22" s="8"/>
-      <c r="O22" s="13"/>
-      <c r="P22" s="13"/>
-      <c r="Q22" s="8"/>
-      <c r="R22" s="8"/>
-      <c r="S22" s="8"/>
-      <c r="T22" s="8"/>
-      <c r="U22" s="8"/>
-      <c r="V22" s="8"/>
-      <c r="W22" s="8"/>
-      <c r="X22" s="8"/>
-      <c r="Y22" s="8"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K22" s="154"/>
+      <c r="L22" s="131"/>
+      <c r="M22" s="135" t="e">
+        <f ca="1">IF((C22&gt;100)*(B1="№")+(B1="Т"),D22+AD38,C22+AD38)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N22" s="131"/>
+      <c r="O22" s="136"/>
+      <c r="P22" s="136"/>
+      <c r="Q22" s="131"/>
+      <c r="R22" s="131"/>
+      <c r="S22" s="131"/>
+      <c r="T22" s="131"/>
+      <c r="U22" s="131"/>
+      <c r="V22" s="131"/>
+      <c r="W22" s="131"/>
+      <c r="X22" s="131"/>
+      <c r="Y22" s="134"/>
       <c r="Z22" s="8"/>
       <c r="AC22" s="1">
         <v>132</v>
@@ -5066,53 +5223,53 @@
       </c>
     </row>
     <row r="23" spans="1:30" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A23" s="149"/>
-      <c r="B23" s="33">
+      <c r="A23" s="159"/>
+      <c r="B23" s="25">
         <v>216</v>
       </c>
-      <c r="C23" s="56">
-        <v>74.16</v>
-      </c>
-      <c r="D23" s="133" t="e">
+      <c r="C23" s="172" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="117" t="e">
         <f t="shared" ca="1" si="9"/>
         <v>#VALUE!</v>
       </c>
-      <c r="E23" s="76"/>
-      <c r="F23" s="60">
+      <c r="E23" s="63"/>
+      <c r="F23" s="48" t="e">
         <f t="shared" si="10"/>
-        <v>75.218936170212771</v>
-      </c>
-      <c r="G23" s="91" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G23" s="75" t="e">
         <f t="shared" ca="1" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H23" s="37">
+      <c r="H23" s="29" t="e">
         <f t="shared" si="6"/>
-        <v>1.4078053002724078E-2</v>
-      </c>
-      <c r="I23" s="161"/>
-      <c r="J23" s="77">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I23" s="153"/>
+      <c r="J23" s="64" t="e">
         <f t="shared" si="11"/>
-        <v>1.0589361702127746</v>
-      </c>
-      <c r="K23" s="44"/>
-      <c r="L23" s="8"/>
-      <c r="M23" s="12">
-        <f>IF((C23&gt;100)*(B1="№")+(B1="Т"),D23+AD39,C23+AD39)</f>
-        <v>-3.2400000000000091</v>
-      </c>
-      <c r="N23" s="8"/>
-      <c r="O23" s="13"/>
-      <c r="P23" s="13"/>
-      <c r="Q23" s="8"/>
-      <c r="R23" s="8"/>
-      <c r="S23" s="8"/>
-      <c r="T23" s="8"/>
-      <c r="U23" s="8"/>
-      <c r="V23" s="8"/>
-      <c r="W23" s="8"/>
-      <c r="X23" s="8"/>
-      <c r="Y23" s="8"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K23" s="36"/>
+      <c r="L23" s="131"/>
+      <c r="M23" s="135" t="e">
+        <f ca="1">IF((C23&gt;100)*(B1="№")+(B1="Т"),D23+AD39,C23+AD39)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N23" s="131"/>
+      <c r="O23" s="136"/>
+      <c r="P23" s="136"/>
+      <c r="Q23" s="131"/>
+      <c r="R23" s="131"/>
+      <c r="S23" s="131"/>
+      <c r="T23" s="131"/>
+      <c r="U23" s="131"/>
+      <c r="V23" s="131"/>
+      <c r="W23" s="131"/>
+      <c r="X23" s="131"/>
+      <c r="Y23" s="134"/>
       <c r="Z23" s="8"/>
       <c r="AC23" s="2">
         <v>139</v>
@@ -5123,55 +5280,55 @@
       </c>
     </row>
     <row r="24" spans="1:30" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A24" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="B24" s="35">
+      <c r="A24" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="27">
         <v>228</v>
       </c>
-      <c r="C24" s="55">
-        <v>78.31</v>
-      </c>
-      <c r="D24" s="95" t="e">
+      <c r="C24" s="171" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="79" t="e">
         <f t="shared" ca="1" si="9"/>
         <v>#VALUE!</v>
       </c>
-      <c r="E24" s="75"/>
-      <c r="F24" s="59">
+      <c r="E24" s="62"/>
+      <c r="F24" s="47" t="e">
         <f t="shared" si="10"/>
-        <v>78.849574468085109</v>
-      </c>
-      <c r="G24" s="93" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G24" s="77" t="e">
         <f t="shared" ca="1" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="H24" s="36">
+      <c r="H24" s="28" t="e">
         <f t="shared" si="6"/>
-        <v>6.8430866206323415E-3</v>
-      </c>
-      <c r="I24" s="161"/>
-      <c r="J24" s="40">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I24" s="153"/>
+      <c r="J24" s="32" t="e">
         <f t="shared" si="11"/>
-        <v>0.53957446808510667</v>
-      </c>
-      <c r="K24" s="45"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="12">
-        <f>IF((C24&gt;100)*(B1="№")+(B1="Т"),D24+AD40,C24+AD40)</f>
-        <v>-4.0900000000000034</v>
-      </c>
-      <c r="N24" s="8"/>
-      <c r="O24" s="13"/>
-      <c r="P24" s="13"/>
-      <c r="Q24" s="8"/>
-      <c r="R24" s="8"/>
-      <c r="S24" s="8"/>
-      <c r="T24" s="8"/>
-      <c r="U24" s="8"/>
-      <c r="V24" s="8"/>
-      <c r="W24" s="8"/>
-      <c r="X24" s="8"/>
-      <c r="Y24" s="8"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K24" s="37"/>
+      <c r="L24" s="131"/>
+      <c r="M24" s="135" t="e">
+        <f ca="1">IF((C24&gt;100)*(B1="№")+(B1="Т"),D24+AD40,C24+AD40)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N24" s="131"/>
+      <c r="O24" s="136"/>
+      <c r="P24" s="136"/>
+      <c r="Q24" s="131"/>
+      <c r="R24" s="131"/>
+      <c r="S24" s="131"/>
+      <c r="T24" s="131"/>
+      <c r="U24" s="131"/>
+      <c r="V24" s="131"/>
+      <c r="W24" s="131"/>
+      <c r="X24" s="131"/>
+      <c r="Y24" s="134"/>
       <c r="Z24" s="8"/>
       <c r="AC24" s="2">
         <v>140</v>
@@ -5182,63 +5339,63 @@
       </c>
     </row>
     <row r="25" spans="1:30" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A25" s="47">
+      <c r="A25" s="39" t="str">
         <f>IFERROR(IF(K20&gt;K25,IF(SUM(F18:F24)&lt;SUM(C18:C24),IF(C25&gt;99.5,IF((K20-K25)*5&lt;1,-1,IF((K20-K25)*5&gt;4,-4,-(K20-K25)*5)),IF((K20-K25)*5&lt;1,1,IF((K20-K25)*5&gt;4,4,(K20-K25)*5))),IF(C25&gt;99.5,IF((K20-K25)*5&lt;1,1,IF((K20-K25)*5&gt;4,4,(K20-K25)*5)),IF((K20-K25)*5&lt;1,-1,IF((K20-K25)*5&gt;4,-4,-(K20-K25)*5)))),"В"),"В")</f>
-        <v>-4</v>
-      </c>
-      <c r="B25" s="29">
+        <v>В</v>
+      </c>
+      <c r="B25" s="21">
         <v>236</v>
       </c>
-      <c r="C25" s="53">
-        <v>81.27</v>
-      </c>
-      <c r="D25" s="132" t="str">
+      <c r="C25" s="166" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="116" t="str">
         <f ca="1">IFERROR(((B25-$E$26*($E$2*94/($B$28-$B$30)))-142)/(9.4-(9.4*$E$26*($E$17+$E$25)/($B$29-$B$31)))*($B$29-$B$31+E24*$E$26)*(($D$2-($E$27/($A$1*1000)))-((((($D$29-$D$31)*$A$21)/($D$29-$D$31+$A$21))*($D$2-($E$27/($A$1*1000))))/$A$21))+((((($D$28-$D$30)*$A$4)/($D$28-$D$30+$A$4))+$D$30+$D$31)*($D$2-($E$27/($A$1*1000))))*10," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E25" s="117">
+      <c r="E25" s="101">
         <f>K4</f>
         <v>0</v>
       </c>
-      <c r="F25" s="58">
+      <c r="F25" s="46" t="str">
         <f>IF(C25=" "," ",C25)</f>
-        <v>81.27</v>
-      </c>
-      <c r="G25" s="92" t="str">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G25" s="76" t="str">
         <f ca="1">IFERROR(C25-D25," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H25" s="38">
+      <c r="H25" s="30" t="e">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="I25" s="30">
+        <v>#VALUE!</v>
+      </c>
+      <c r="I25" s="22">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="J25" s="142">
+      <c r="J25" s="124" t="str">
         <f>IF(F25=" "," ",IF(B1=7,236-(9.4*(($C$24-$D$24)/(($D$2-($E$27/($A$1*1000)))-((((($D$29-$D$31)*$A$21)/($D$29-$D$31+$A$21))*($D$2-($E$27/($A$1*1000))))/$A$21)))/($D$29-$D$31)),0))</f>
-        <v>0</v>
-      </c>
-      <c r="K25" s="80">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="K25" s="67">
         <v>0.4</v>
       </c>
-      <c r="L25" s="8"/>
-      <c r="M25" s="10">
-        <f>IF((C25&gt;110)*(B1="№")+(B1="Т"),D25+AD45,IF(B25=AC41,C25+AD41,IF(B25=AC42,C25+AD42,IF(B25=AC43,C25+AD43,IF(B25=AC44,C25+AD44,IF(B25=AC45,C25+AD45,IF(B25=AC46,C25+AD46,IF(B25=AC47,C25+AD47,IF(B25=AC48,C25+AD48,IF(B25=AC49,C25+AD49,"ошибка"))))))))))</f>
-        <v>-4.5299999999999869</v>
-      </c>
-      <c r="N25" s="8"/>
-      <c r="O25" s="11"/>
-      <c r="P25" s="11"/>
-      <c r="Q25" s="8"/>
-      <c r="R25" s="8"/>
-      <c r="S25" s="8"/>
-      <c r="T25" s="8"/>
-      <c r="U25" s="8"/>
-      <c r="V25" s="8"/>
-      <c r="W25" s="8"/>
-      <c r="X25" s="8"/>
-      <c r="Y25" s="8"/>
+      <c r="L25" s="131"/>
+      <c r="M25" s="132" t="e">
+        <f ca="1">IF((C25&gt;110)*(B1="№")+(B1="Т"),D25+AD45,IF(B25=AC41,C25+AD41,IF(B25=AC42,C25+AD42,IF(B25=AC43,C25+AD43,IF(B25=AC44,C25+AD44,IF(B25=AC45,C25+AD45,IF(B25=AC46,C25+AD46,IF(B25=AC47,C25+AD47,IF(B25=AC48,C25+AD48,IF(B25=AC49,C25+AD49,"ошибка"))))))))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N25" s="131"/>
+      <c r="O25" s="133"/>
+      <c r="P25" s="133"/>
+      <c r="Q25" s="131"/>
+      <c r="R25" s="131"/>
+      <c r="S25" s="131"/>
+      <c r="T25" s="131"/>
+      <c r="U25" s="131"/>
+      <c r="V25" s="131"/>
+      <c r="W25" s="131"/>
+      <c r="X25" s="131"/>
+      <c r="Y25" s="134"/>
       <c r="Z25" s="8"/>
       <c r="AC25" s="2">
         <v>141</v>
@@ -5249,45 +5406,45 @@
       </c>
     </row>
     <row r="26" spans="1:30" ht="15.75" thickBot="1">
-      <c r="A26" s="122" t="str">
-        <f ca="1">IF(C9&gt;5000," ",IF((C9&lt;5),C9,A26))</f>
+      <c r="A26" s="106" t="str">
+        <f>IF(C9&gt;5000," ",IF((C9&lt;5),C9,A26))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="B26" s="52" t="e">
-        <f ca="1">IF(B27&lt;600,"Ползун",B28/B30)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C26" s="51" t="e">
-        <f ca="1">IF(B27&lt;600,"Общее",B29/B31)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D26" s="96" t="str">
-        <f ca="1">IFERROR(D28+D29," ")</f>
+      <c r="B26" s="43" t="e">
+        <f>IF(B27&lt;600,"Ползун",B28/B30)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C26" s="42" t="e">
+        <f>IF(B27&lt;600,"Общее",B29/B31)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D26" s="80" t="str">
+        <f>IFERROR(D28+D29," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E26" s="84">
+      <c r="E26" s="71">
         <v>2</v>
       </c>
-      <c r="F26" s="107"/>
-      <c r="G26" s="108"/>
-      <c r="H26" s="108"/>
-      <c r="I26" s="108"/>
-      <c r="J26" s="108"/>
-      <c r="K26" s="109"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="17"/>
-      <c r="N26" s="8"/>
-      <c r="O26" s="8"/>
-      <c r="P26" s="8"/>
-      <c r="Q26" s="8"/>
-      <c r="R26" s="8"/>
-      <c r="S26" s="8"/>
-      <c r="T26" s="8"/>
-      <c r="U26" s="8"/>
-      <c r="V26" s="8"/>
-      <c r="W26" s="8"/>
-      <c r="X26" s="8"/>
-      <c r="Y26" s="8"/>
+      <c r="F26" s="91"/>
+      <c r="G26" s="92"/>
+      <c r="H26" s="92"/>
+      <c r="I26" s="92"/>
+      <c r="J26" s="92"/>
+      <c r="K26" s="93"/>
+      <c r="L26" s="131"/>
+      <c r="M26" s="140"/>
+      <c r="N26" s="131"/>
+      <c r="O26" s="131"/>
+      <c r="P26" s="131"/>
+      <c r="Q26" s="131"/>
+      <c r="R26" s="131"/>
+      <c r="S26" s="131"/>
+      <c r="T26" s="131"/>
+      <c r="U26" s="131"/>
+      <c r="V26" s="131"/>
+      <c r="W26" s="131"/>
+      <c r="X26" s="131"/>
+      <c r="Y26" s="134"/>
       <c r="Z26" s="8"/>
       <c r="AC26" s="2">
         <v>142</v>
@@ -5298,44 +5455,44 @@
       </c>
     </row>
     <row r="27" spans="1:30" ht="15.75" thickBot="1">
-      <c r="A27" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="79" t="str">
-        <f ca="1">IF(B28=" ",IF((C5&gt;200)*(C5&lt;2000),C5,IF(C5&gt;2000," ",B27)),B28+B29)</f>
+      <c r="A27" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="66" t="str">
+        <f>IF(B28=" ",IF((C5&gt;200)*(C5&lt;2000),C5,IF(C5&gt;2000," ",B27)),B28+B29)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C27" s="85" t="str">
-        <f ca="1">(IF(B30=" ",IF((C2&gt;400)*(C2&lt;2000),C2,IF(C2&gt;2000," ",C27)),((B28-B30)*A4/((B28-B30)+A4)+B30+B31+(B29-B31)*A21/((B29-B31)+A21))*A1*1000/(((B28-B30)*A4/((B28-B30)+A4)+B30+B31+(B29-B31)*A21/((B29-B31)+A21))+A1*1000)))</f>
+      <c r="C27" s="72" t="str">
+        <f>(IF(B30=" ",IF((C2&gt;400)*(C2&lt;2000),C2,IF(C2&gt;2000," ",C27)),((B28-B30)*A4/((B28-B30)+A4)+B30+B31+(B29-B31)*A21/((B29-B31)+A21))*A1*1000/(((B28-B30)*A4/((B28-B30)+A4)+B30+B31+(B29-B31)*A21/((B29-B31)+A21))+A1*1000)))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D27" s="105" t="str">
+      <c r="D27" s="89" t="str">
         <f ca="1">IFERROR(((D28-D30)*A4/((D28-D30)+A4)+D30+D31+(D29-D31)*A21/((D29-D31)+A21))*A1*1000/(((D28-D30)*A4/((D28-D30)+A4)+D30+D31+(D29-D31)*A21/((D29-D31)+A21))+A1*1000)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E27" s="119">
+      <c r="E27" s="103">
         <v>10</v>
       </c>
-      <c r="F27" s="110"/>
-      <c r="G27" s="111"/>
-      <c r="H27" s="111"/>
-      <c r="I27" s="111"/>
-      <c r="J27" s="111"/>
-      <c r="K27" s="112"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="9"/>
-      <c r="N27" s="8"/>
-      <c r="O27" s="8"/>
-      <c r="P27" s="8"/>
-      <c r="Q27" s="8"/>
-      <c r="R27" s="8"/>
-      <c r="S27" s="8"/>
-      <c r="T27" s="8"/>
-      <c r="U27" s="8"/>
-      <c r="V27" s="8"/>
-      <c r="W27" s="8"/>
-      <c r="X27" s="8"/>
-      <c r="Y27" s="8"/>
+      <c r="F27" s="94"/>
+      <c r="G27" s="95"/>
+      <c r="H27" s="95"/>
+      <c r="I27" s="95"/>
+      <c r="J27" s="95"/>
+      <c r="K27" s="96"/>
+      <c r="L27" s="131"/>
+      <c r="M27" s="141"/>
+      <c r="N27" s="131"/>
+      <c r="O27" s="131"/>
+      <c r="P27" s="131"/>
+      <c r="Q27" s="131"/>
+      <c r="R27" s="131"/>
+      <c r="S27" s="131"/>
+      <c r="T27" s="131"/>
+      <c r="U27" s="131"/>
+      <c r="V27" s="131"/>
+      <c r="W27" s="131"/>
+      <c r="X27" s="131"/>
+      <c r="Y27" s="134"/>
       <c r="Z27" s="8"/>
       <c r="AC27" s="2">
         <v>143</v>
@@ -5346,197 +5503,197 @@
       </c>
     </row>
     <row r="28" spans="1:30">
-      <c r="A28" s="42" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28" s="97" t="str">
-        <f ca="1">IF(C3&gt;2000," ",IF((C3&gt;400)*(C3&lt;1500),C3,B28))</f>
+      <c r="A28" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="81" t="str">
+        <f>IF(C3&gt;2000," ",IF((C3&gt;400)*(C3&lt;1500),C3,B28))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C28" s="158" t="str">
-        <f ca="1">IF(NOT(B1="R"),IF(B28=" "," ",ABS(B28-B29)),ABS(D28-D29))</f>
+      <c r="C28" s="150" t="str">
+        <f>IF(NOT(B1="R"),IF(B28=" "," ",ABS(B28-B29)),ABS(D28-D29))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D28" s="98" t="str">
-        <f ca="1">IFERROR(IF(A7=" ",(SQRT(POWER(2*A4-(C27*A1*1000*0.8)/(A1*1000-C27),2)+(1.28*C27*A1*1000*A4)/(A1*1000-C27))+(C27*A1*1000*0.8)/(A1*1000-C27)-2*A4)/0.64,IFERROR(B28+E26*SUM(E2:E13),(-(A4-(1-1/E30)*((-(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-SQRT(((-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))*(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-4*(((A1*1000)*C27/((A1*1000)-C27))+(A1*1000))*A7)))/2))+SQRT(((A4-(1-1/E30)*((-(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-SQRT(((-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))*(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-4*(((A1*1000)*C27/((A1*1000)-C27))+(A1*1000))*A7)))/2))*(A4-(1-1/E30)*((-(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-SQRT(((-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))*(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-4*(((A1*1000)*C27/((A1*1000)-C27))+(A1*1000))*A7)))/2))+4*((E30-1)/(E30*E30))*A4*((-(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-SQRT(((-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))*(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-4*(((A1*1000)*C27/((A1*1000)-C27))+(A1*1000))*A7)))/2))))/(2*((E30-1)/(E30*E30)))))," ")</f>
+      <c r="D28" s="82" t="str">
+        <f>IFERROR(IF(A7=" ",(SQRT(POWER(2*A4-(C27*A1*1000*0.8)/(A1*1000-C27),2)+(1.28*C27*A1*1000*A4)/(A1*1000-C27))+(C27*A1*1000*0.8)/(A1*1000-C27)-2*A4)/0.64,IFERROR(B28+E26*SUM(E2:E13),(-(A4-(1-1/E30)*((-(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-SQRT(((-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))*(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-4*(((A1*1000)*C27/((A1*1000)-C27))+(A1*1000))*A7)))/2))+SQRT(((A4-(1-1/E30)*((-(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-SQRT(((-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))*(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-4*(((A1*1000)*C27/((A1*1000)-C27))+(A1*1000))*A7)))/2))*(A4-(1-1/E30)*((-(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-SQRT(((-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))*(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-4*(((A1*1000)*C27/((A1*1000)-C27))+(A1*1000))*A7)))/2))+4*((E30-1)/(E30*E30))*A4*((-(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-SQRT(((-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))*(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-4*(((A1*1000)*C27/((A1*1000)-C27))+(A1*1000))*A7)))/2))))/(2*((E30-1)/(E30*E30)))))," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E28" s="98" t="str">
-        <f ca="1">IFERROR(ABS(D28-D29)," ")</f>
+      <c r="E28" s="82" t="str">
+        <f>IFERROR(ABS(D28-D29)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F28" s="110"/>
-      <c r="G28" s="111"/>
-      <c r="H28" s="111"/>
-      <c r="I28" s="111"/>
-      <c r="J28" s="111"/>
-      <c r="K28" s="112"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="9"/>
-      <c r="N28" s="8"/>
-      <c r="O28" s="8"/>
-      <c r="P28" s="8"/>
-      <c r="Q28" s="8"/>
-      <c r="R28" s="8"/>
-      <c r="S28" s="8"/>
-      <c r="T28" s="8"/>
-      <c r="U28" s="8"/>
-      <c r="V28" s="8"/>
-      <c r="W28" s="8"/>
-      <c r="X28" s="8"/>
-      <c r="Y28" s="8"/>
+      <c r="F28" s="94"/>
+      <c r="G28" s="95"/>
+      <c r="H28" s="95"/>
+      <c r="I28" s="95"/>
+      <c r="J28" s="95"/>
+      <c r="K28" s="96"/>
+      <c r="L28" s="131"/>
+      <c r="M28" s="141"/>
+      <c r="N28" s="131"/>
+      <c r="O28" s="131"/>
+      <c r="P28" s="131"/>
+      <c r="Q28" s="131"/>
+      <c r="R28" s="131"/>
+      <c r="S28" s="131"/>
+      <c r="T28" s="131"/>
+      <c r="U28" s="131"/>
+      <c r="V28" s="131"/>
+      <c r="W28" s="131"/>
+      <c r="X28" s="131"/>
+      <c r="Y28" s="134"/>
       <c r="Z28" s="8"/>
       <c r="AC28" s="2"/>
     </row>
     <row r="29" spans="1:30" ht="15.75" thickBot="1">
-      <c r="A29" s="99" t="s">
-        <v>8</v>
-      </c>
-      <c r="B29" s="100" t="str">
-        <f ca="1">IF(C4&gt;2000," ",IF((C4&gt;400)*(C4&lt;1500),C4,B29))</f>
+      <c r="A29" s="83" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="84" t="str">
+        <f>IF(C4&gt;2000," ",IF((C4&gt;400)*(C4&lt;1500),C4,B29))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C29" s="159"/>
-      <c r="D29" s="101" t="str">
-        <f ca="1">IFERROR(IF(A18=" ",(SQRT(POWER(2*A4-(C27*A1*1000*0.8)/(A1*1000-C27),2)+(1.28*C27*A1*1000*A4)/(A1*1000-C27))+(C27*A1*1000*0.8)/(A1*1000-C27)-2*A4)/0.64,IFERROR(B29+E26*SUM(E14:E25),(-(A21-(1-1/E31)*((-(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-SQRT(((-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))*(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-4*(((A1*1000)*C27/((A1*1000)-C27))+(A1*1000))*A18)))/2))+SQRT(((A21-(1-1/E31)*((-(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-SQRT(((-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))*(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-4*(((A1*1000)*C27/((A1*1000)-C27))+(A1*1000))*A18)))/2))*(A21-(1-1/E31)*((-(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-SQRT(((-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))*(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-4*(((A1*1000)*C27/((A1*1000)-C27))+(A1*1000))*A18)))/2))+4*((E31-1)/(E31*E31))*A21*((-(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-SQRT(((-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))*(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-4*(((A1*1000)*C27/((A1*1000)-C27))+(A1*1000))*A18)))/2))))/(2*((E31-1)/(E31*E31)))))," ")</f>
+      <c r="C29" s="151"/>
+      <c r="D29" s="85" t="str">
+        <f>IFERROR(IF(A18=" ",(SQRT(POWER(2*A4-(C27*A1*1000*0.8)/(A1*1000-C27),2)+(1.28*C27*A1*1000*A4)/(A1*1000-C27))+(C27*A1*1000*0.8)/(A1*1000-C27)-2*A4)/0.64,IFERROR(B29+E26*SUM(E14:E25),(-(A21-(1-1/E31)*((-(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-SQRT(((-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))*(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-4*(((A1*1000)*C27/((A1*1000)-C27))+(A1*1000))*A18)))/2))+SQRT(((A21-(1-1/E31)*((-(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-SQRT(((-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))*(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-4*(((A1*1000)*C27/((A1*1000)-C27))+(A1*1000))*A18)))/2))*(A21-(1-1/E31)*((-(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-SQRT(((-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))*(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-4*(((A1*1000)*C27/((A1*1000)-C27))+(A1*1000))*A18)))/2))+4*((E31-1)/(E31*E31))*A21*((-(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-SQRT(((-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))*(-((A1*1000)*C27/((A1*1000)-C27))-(A1*1000))-4*(((A1*1000)*C27/((A1*1000)-C27))+(A1*1000))*A18)))/2))))/(2*((E31-1)/(E31*E31)))))," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E29" s="101" t="str">
+      <c r="E29" s="85" t="str">
         <f ca="1">IFERROR(ABS(D30-D31)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F29" s="110"/>
-      <c r="G29" s="111"/>
-      <c r="H29" s="111"/>
-      <c r="I29" s="111"/>
-      <c r="J29" s="111"/>
-      <c r="K29" s="112"/>
-      <c r="L29" s="8"/>
-      <c r="M29" s="9"/>
-      <c r="N29" s="8"/>
-      <c r="O29" s="8"/>
-      <c r="P29" s="8"/>
-      <c r="Q29" s="8"/>
-      <c r="R29" s="8"/>
-      <c r="S29" s="8"/>
-      <c r="T29" s="8"/>
-      <c r="U29" s="8"/>
-      <c r="V29" s="8"/>
-      <c r="W29" s="8"/>
-      <c r="X29" s="8"/>
-      <c r="Y29" s="8"/>
+      <c r="F29" s="94"/>
+      <c r="G29" s="95"/>
+      <c r="H29" s="95"/>
+      <c r="I29" s="95"/>
+      <c r="J29" s="95"/>
+      <c r="K29" s="96"/>
+      <c r="L29" s="131"/>
+      <c r="M29" s="141"/>
+      <c r="N29" s="131"/>
+      <c r="O29" s="131"/>
+      <c r="P29" s="131"/>
+      <c r="Q29" s="131"/>
+      <c r="R29" s="131"/>
+      <c r="S29" s="131"/>
+      <c r="T29" s="131"/>
+      <c r="U29" s="131"/>
+      <c r="V29" s="131"/>
+      <c r="W29" s="131"/>
+      <c r="X29" s="131"/>
+      <c r="Y29" s="134"/>
       <c r="Z29" s="8"/>
       <c r="AC29" s="2"/>
     </row>
     <row r="30" spans="1:30">
-      <c r="A30" s="102" t="s">
-        <v>10</v>
-      </c>
-      <c r="B30" s="103" t="str">
-        <f ca="1">IF(C5&gt;400," ",IF((C5&gt;100)*(C5&lt;250),C5,B30))</f>
+      <c r="A30" s="86" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" s="87" t="str">
+        <f>IF(C5&gt;400," ",IF((C5&gt;100)*(C5&lt;250),C5,B30))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C30" s="160" t="str">
-        <f ca="1">IF(NOT(B1="R"),IF(B30=" "," ",ABS(B30-B31)),ABS(D30-D31))</f>
+      <c r="C30" s="152" t="str">
+        <f>IF(NOT(B1="R"),IF(B30=" "," ",ABS(B30-B31)),ABS(D30-D31))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D30" s="140" t="str">
+      <c r="D30" s="122" t="str">
         <f ca="1">IFERROR(IFERROR(IF(NOT(B1="R"),B30+E26*SUM(E11:E13),IF(A7=" ",D28/5,D28/E30)),D28/E30)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E30" s="121" t="str">
+      <c r="E30" s="105" t="str">
         <f ca="1">IFERROR(IFERROR((((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))+(0.5*((A1*1000+(A1*1000*C27/(A1*1000-C27))-((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))*A4/((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))+A4)))-((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))*A4/((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))+A4))-SQRT((POWER((((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))*A4/((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))+A4))-(A1*1000+(A1*1000*C27/(A1*1000-C27))-((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))*A4/((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))+A4)))),2)-4*(A7*((A1*1000*C27/(A1*1000-C27))+(A1*1000))-(((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))*A4/((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))+A4))*(A1*1000+(A1*1000*C27/(A1*1000-C27))-((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))*A4/((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))+A4))))))))))/(0.5*((A1*1000+(A1*1000*C27/(A1*1000-C27))-((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))*A4/((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))+A4)))-((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))*A4/((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))+A4))-SQRT((POWER((((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))*A4/((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))+A4))-(A1*1000+(A1*1000*C27/(A1*1000-C27))-((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))*A4/((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))+A4)))),2)-4*(A7*((A1*1000*C27/(A1*1000-C27))+(A1*1000))-(((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))*A4/((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))+A4))*(A1*1000+(A1*1000*C27/(A1*1000-C27))-((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))*A4/((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))+A4)))))))))),IF(B31=" ",IF(A7=" ",D28/D30,4.92),D28/D30))," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F30" s="110"/>
-      <c r="G30" s="111"/>
-      <c r="H30" s="111"/>
-      <c r="I30" s="111"/>
-      <c r="J30" s="111"/>
-      <c r="K30" s="112"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="9"/>
-      <c r="N30" s="8"/>
-      <c r="O30" s="8"/>
-      <c r="P30" s="8"/>
-      <c r="Q30" s="8"/>
-      <c r="R30" s="8"/>
-      <c r="S30" s="8"/>
-      <c r="T30" s="8"/>
-      <c r="U30" s="8"/>
-      <c r="V30" s="8"/>
-      <c r="W30" s="8"/>
-      <c r="X30" s="8"/>
-      <c r="Y30" s="8"/>
+      <c r="F30" s="94"/>
+      <c r="G30" s="95"/>
+      <c r="H30" s="95"/>
+      <c r="I30" s="95"/>
+      <c r="J30" s="95"/>
+      <c r="K30" s="96"/>
+      <c r="L30" s="131"/>
+      <c r="M30" s="141"/>
+      <c r="N30" s="131"/>
+      <c r="O30" s="131"/>
+      <c r="P30" s="131"/>
+      <c r="Q30" s="131"/>
+      <c r="R30" s="131"/>
+      <c r="S30" s="131"/>
+      <c r="T30" s="131"/>
+      <c r="U30" s="131"/>
+      <c r="V30" s="131"/>
+      <c r="W30" s="131"/>
+      <c r="X30" s="131"/>
+      <c r="Y30" s="134"/>
       <c r="Z30" s="8"/>
       <c r="AC30" s="2"/>
     </row>
     <row r="31" spans="1:30" ht="15.75" thickBot="1">
-      <c r="A31" s="99" t="s">
-        <v>9</v>
-      </c>
-      <c r="B31" s="104" t="str">
-        <f ca="1">IF(C6&gt;400," ",IF((C6&gt;100)*(C6&lt;250),C6,B31))</f>
+      <c r="A31" s="83" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" s="88" t="str">
+        <f>IF(C6&gt;400," ",IF((C6&gt;100)*(C6&lt;250),C6,B31))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C31" s="159"/>
-      <c r="D31" s="120" t="str">
+      <c r="C31" s="151"/>
+      <c r="D31" s="104" t="str">
         <f ca="1">IFERROR(IFERROR(IF(NOT(B1="R"),B31+E26*SUM(E14:E16),IF(A18=" ",D29/5,D29/E31)),D29/E31)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E31" s="120" t="str">
+      <c r="E31" s="104" t="str">
         <f ca="1">IFERROR(IFERROR((((0.1*(C25-C17)/(((E27/C27)-(E27/(A1*1000)))-0.1*(C25-C17)/A21))+((A1*1000*C27/(A1*1000-C27))-((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))*A4/((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))+A4))-((0.1*(C25-C17)/(((E27/C27)-(E27/(A1*1000)))-0.1*(C25-C17)/A21))*A21/((0.1*(C25-C17)/(((E27/C27)-(E27/(A1*1000)))-0.1*(C25-C17)/A21))+A21))-(0.5*((A1*1000+(A1*1000*C27/(A1*1000-C27))-((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))*A4/((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))+A4)))-((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))*A4/((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))+A4))-SQRT((POWER((((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))*A4/((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))+A4))-(A1*1000+(A1*1000*C27/(A1*1000-C27))-((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))*A4/((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))+A4)))),2)-4*(A7*((A1*1000*C27/(A1*1000-C27))+(A1*1000))-(((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))*A4/((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))+A4))*(A1*1000+(A1*1000*C27/(A1*1000-C27))-((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))*A4/((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))+A4)))))))))))/((A1*1000*C27/(A1*1000-C27))-((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))*A4/((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))+A4))-((0.1*(C25-C17)/(((E27/C27)-(E27/(A1*1000)))-0.1*(C25-C17)/A21))*A21/((0.1*(C25-C17)/(((E27/C27)-(E27/(A1*1000)))-0.1*(C25-C17)/A21))+A21))-(0.5*((A1*1000+(A1*1000*C27/(A1*1000-C27))-((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))*A4/((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))+A4)))-((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))*A4/((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))+A4))-SQRT((POWER((((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))*A4/((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))+A4))-(A1*1000+(A1*1000*C27/(A1*1000-C27))-((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))*A4/((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))+A4)))),2)-4*(A7*((A1*1000*C27/(A1*1000-C27))+(A1*1000))-(((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))*A4/((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))+A4))*(A1*1000+(A1*1000*C27/(A1*1000-C27))-((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))*A4/((0.1*C11/(((E27/C27)-(E27/(A1*1000)))-(0.1*C11/A4)))+A4))))))))))),IF(B31=" ",IF(A18=" ",D29/D31,4.92),D29/D31))," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F31" s="113"/>
-      <c r="G31" s="114"/>
-      <c r="H31" s="114"/>
-      <c r="I31" s="114"/>
-      <c r="J31" s="114"/>
-      <c r="K31" s="115"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="9"/>
-      <c r="N31" s="8"/>
-      <c r="O31" s="8"/>
-      <c r="P31" s="8"/>
-      <c r="Q31" s="8"/>
-      <c r="R31" s="8"/>
-      <c r="S31" s="8"/>
-      <c r="T31" s="8"/>
-      <c r="U31" s="8"/>
-      <c r="V31" s="8"/>
-      <c r="W31" s="8"/>
-      <c r="X31" s="8"/>
-      <c r="Y31" s="8"/>
+      <c r="F31" s="97"/>
+      <c r="G31" s="98"/>
+      <c r="H31" s="98"/>
+      <c r="I31" s="98"/>
+      <c r="J31" s="98"/>
+      <c r="K31" s="99"/>
+      <c r="L31" s="131"/>
+      <c r="M31" s="141"/>
+      <c r="N31" s="131"/>
+      <c r="O31" s="131"/>
+      <c r="P31" s="131"/>
+      <c r="Q31" s="131"/>
+      <c r="R31" s="131"/>
+      <c r="S31" s="131"/>
+      <c r="T31" s="131"/>
+      <c r="U31" s="131"/>
+      <c r="V31" s="131"/>
+      <c r="W31" s="131"/>
+      <c r="X31" s="131"/>
+      <c r="Y31" s="134"/>
       <c r="Z31" s="8"/>
       <c r="AC31" s="2"/>
     </row>
-    <row r="32" spans="1:30">
-      <c r="A32" s="126"/>
-      <c r="B32" s="126"/>
-      <c r="C32" s="134"/>
-      <c r="D32" s="134"/>
-      <c r="E32" s="134"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="135"/>
-      <c r="L32" s="8"/>
-      <c r="M32" s="9"/>
-      <c r="N32" s="8"/>
-      <c r="O32" s="8"/>
-      <c r="P32" s="8"/>
-      <c r="Q32" s="8"/>
-      <c r="R32" s="8"/>
-      <c r="S32" s="8"/>
-      <c r="T32" s="8"/>
-      <c r="U32" s="8"/>
-      <c r="V32" s="8"/>
-      <c r="W32" s="8"/>
-      <c r="X32" s="8"/>
-      <c r="Y32" s="8"/>
+    <row r="32" spans="1:30" ht="15.75" thickBot="1">
+      <c r="A32" s="145"/>
+      <c r="B32" s="146"/>
+      <c r="C32" s="146"/>
+      <c r="D32" s="146"/>
+      <c r="E32" s="146"/>
+      <c r="F32" s="146"/>
+      <c r="G32" s="146"/>
+      <c r="H32" s="146"/>
+      <c r="I32" s="146"/>
+      <c r="J32" s="146"/>
+      <c r="K32" s="147"/>
+      <c r="L32" s="142"/>
+      <c r="M32" s="143"/>
+      <c r="N32" s="142"/>
+      <c r="O32" s="142"/>
+      <c r="P32" s="142"/>
+      <c r="Q32" s="142"/>
+      <c r="R32" s="142"/>
+      <c r="S32" s="142"/>
+      <c r="T32" s="142"/>
+      <c r="U32" s="142"/>
+      <c r="V32" s="142"/>
+      <c r="W32" s="142"/>
+      <c r="X32" s="142"/>
+      <c r="Y32" s="144"/>
       <c r="Z32" s="8"/>
       <c r="AC32" s="3">
         <v>144</v>
@@ -5547,19 +5704,23 @@
       </c>
     </row>
     <row r="33" spans="1:30">
-      <c r="A33" s="126"/>
-      <c r="B33" s="145"/>
-      <c r="C33" s="145"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="146"/>
-      <c r="G33" s="136"/>
-      <c r="H33" s="136"/>
-      <c r="I33" s="136"/>
-      <c r="J33" s="136"/>
-      <c r="K33" s="137"/>
-      <c r="L33" s="22"/>
-      <c r="M33" s="22" t="s">
+      <c r="A33" s="110"/>
+      <c r="B33" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="118"/>
+      <c r="G33" s="118"/>
+      <c r="H33" s="118"/>
+      <c r="I33" s="118"/>
+      <c r="J33" s="118"/>
+      <c r="K33" s="119"/>
+      <c r="L33" s="14"/>
+      <c r="M33" s="14" t="s">
         <v>1</v>
       </c>
       <c r="N33" s="9"/>
@@ -5584,23 +5745,23 @@
       </c>
     </row>
     <row r="34" spans="1:30">
-      <c r="A34" s="126"/>
-      <c r="B34" s="22">
+      <c r="A34" s="110"/>
+      <c r="B34" s="14">
         <v>0</v>
       </c>
-      <c r="C34" s="22">
+      <c r="C34" s="14">
         <v>232</v>
       </c>
-      <c r="D34" s="22"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="136"/>
-      <c r="G34" s="136"/>
-      <c r="H34" s="136"/>
-      <c r="I34" s="136"/>
-      <c r="J34" s="136"/>
-      <c r="K34" s="137"/>
-      <c r="L34" s="22"/>
-      <c r="M34" s="22">
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="118"/>
+      <c r="G34" s="118"/>
+      <c r="H34" s="118"/>
+      <c r="I34" s="118"/>
+      <c r="J34" s="118"/>
+      <c r="K34" s="119"/>
+      <c r="L34" s="14"/>
+      <c r="M34" s="14">
         <v>240</v>
       </c>
       <c r="N34" s="9"/>
@@ -5625,23 +5786,23 @@
       </c>
     </row>
     <row r="35" spans="1:30">
-      <c r="A35" s="138"/>
-      <c r="B35" s="22">
+      <c r="A35" s="120"/>
+      <c r="B35" s="14">
         <v>25</v>
       </c>
-      <c r="C35" s="22">
+      <c r="C35" s="14">
         <v>232</v>
       </c>
-      <c r="D35" s="22"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="136"/>
-      <c r="G35" s="136"/>
-      <c r="H35" s="136"/>
-      <c r="I35" s="136"/>
-      <c r="J35" s="136"/>
-      <c r="K35" s="137"/>
-      <c r="L35" s="22"/>
-      <c r="M35" s="22">
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="118"/>
+      <c r="G35" s="118"/>
+      <c r="H35" s="118"/>
+      <c r="I35" s="118"/>
+      <c r="J35" s="118"/>
+      <c r="K35" s="119"/>
+      <c r="L35" s="14"/>
+      <c r="M35" s="14">
         <v>240</v>
       </c>
       <c r="N35" s="9"/>
@@ -5666,21 +5827,21 @@
       </c>
     </row>
     <row r="36" spans="1:30">
-      <c r="A36" s="138"/>
-      <c r="B36" s="22"/>
-      <c r="C36" s="23">
+      <c r="A36" s="120"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="15">
         <v>139</v>
       </c>
-      <c r="D36" s="23"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
-      <c r="G36" s="23"/>
-      <c r="H36" s="23"/>
-      <c r="I36" s="23"/>
-      <c r="J36" s="23"/>
-      <c r="K36" s="139"/>
-      <c r="L36" s="23"/>
-      <c r="M36" s="23">
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="15"/>
+      <c r="K36" s="121"/>
+      <c r="L36" s="15"/>
+      <c r="M36" s="15">
         <v>145</v>
       </c>
       <c r="N36" s="9"/>
@@ -5705,21 +5866,21 @@
       </c>
     </row>
     <row r="37" spans="1:30">
-      <c r="A37" s="138"/>
-      <c r="B37" s="22"/>
-      <c r="C37" s="23">
+      <c r="A37" s="120"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="15">
         <v>139</v>
       </c>
-      <c r="D37" s="23"/>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
-      <c r="G37" s="23"/>
-      <c r="H37" s="23"/>
-      <c r="I37" s="23"/>
-      <c r="J37" s="23"/>
-      <c r="K37" s="139"/>
-      <c r="L37" s="23"/>
-      <c r="M37" s="23">
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15"/>
+      <c r="K37" s="121"/>
+      <c r="L37" s="15"/>
+      <c r="M37" s="15">
         <v>145</v>
       </c>
       <c r="N37" s="9"/>
@@ -5744,21 +5905,21 @@
       </c>
     </row>
     <row r="38" spans="1:30">
-      <c r="A38" s="138"/>
-      <c r="B38" s="22"/>
-      <c r="C38" s="23">
+      <c r="A38" s="120"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="15">
         <v>91</v>
       </c>
-      <c r="D38" s="23"/>
-      <c r="E38" s="23"/>
-      <c r="F38" s="23"/>
-      <c r="G38" s="23"/>
-      <c r="H38" s="23"/>
-      <c r="I38" s="23"/>
-      <c r="J38" s="23"/>
-      <c r="K38" s="139"/>
-      <c r="L38" s="23"/>
-      <c r="M38" s="23">
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="15"/>
+      <c r="J38" s="15"/>
+      <c r="K38" s="121"/>
+      <c r="L38" s="15"/>
+      <c r="M38" s="15">
         <v>97</v>
       </c>
       <c r="N38" s="9"/>
@@ -5783,21 +5944,21 @@
       </c>
     </row>
     <row r="39" spans="1:30">
-      <c r="A39" s="138"/>
-      <c r="B39" s="22"/>
-      <c r="C39" s="23">
+      <c r="A39" s="120"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="15">
         <v>91</v>
       </c>
-      <c r="D39" s="23"/>
-      <c r="E39" s="23"/>
-      <c r="F39" s="23"/>
-      <c r="G39" s="23"/>
-      <c r="H39" s="23"/>
-      <c r="I39" s="23"/>
-      <c r="J39" s="23"/>
-      <c r="K39" s="139"/>
-      <c r="L39" s="23"/>
-      <c r="M39" s="23">
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="15"/>
+      <c r="I39" s="15"/>
+      <c r="J39" s="15"/>
+      <c r="K39" s="121"/>
+      <c r="L39" s="15"/>
+      <c r="M39" s="15">
         <v>97</v>
       </c>
       <c r="N39" s="9"/>
@@ -5830,7 +5991,7 @@
       <c r="H40" s="6"/>
       <c r="I40" s="6"/>
       <c r="J40" s="6"/>
-      <c r="K40" s="24"/>
+      <c r="K40" s="16"/>
       <c r="L40" s="6"/>
       <c r="N40" s="6"/>
       <c r="AC40" s="1">
@@ -5842,17 +6003,17 @@
       </c>
     </row>
     <row r="41" spans="1:30">
-      <c r="A41" s="127"/>
-      <c r="B41" s="141"/>
-      <c r="C41" s="127"/>
-      <c r="D41" s="127"/>
-      <c r="E41" s="127"/>
-      <c r="F41" s="127"/>
-      <c r="G41" s="127"/>
-      <c r="H41" s="127"/>
-      <c r="I41" s="127"/>
-      <c r="J41" s="127"/>
-      <c r="K41" s="128"/>
+      <c r="A41" s="111"/>
+      <c r="B41" s="123"/>
+      <c r="C41" s="111"/>
+      <c r="D41" s="111"/>
+      <c r="E41" s="111"/>
+      <c r="F41" s="111"/>
+      <c r="G41" s="111"/>
+      <c r="H41" s="111"/>
+      <c r="I41" s="111"/>
+      <c r="J41" s="111"/>
+      <c r="K41" s="112"/>
       <c r="L41" s="5"/>
       <c r="M41" s="5" t="s">
         <v>2</v>
@@ -5867,17 +6028,17 @@
       </c>
     </row>
     <row r="42" spans="1:30">
-      <c r="A42" s="127"/>
-      <c r="B42" s="141"/>
-      <c r="C42" s="129"/>
-      <c r="D42" s="129"/>
-      <c r="E42" s="129"/>
-      <c r="F42" s="129"/>
-      <c r="G42" s="129"/>
-      <c r="H42" s="129"/>
-      <c r="I42" s="129"/>
-      <c r="J42" s="129"/>
-      <c r="K42" s="128"/>
+      <c r="A42" s="111"/>
+      <c r="B42" s="123"/>
+      <c r="C42" s="113"/>
+      <c r="D42" s="113"/>
+      <c r="E42" s="113"/>
+      <c r="F42" s="113"/>
+      <c r="G42" s="113"/>
+      <c r="H42" s="113"/>
+      <c r="I42" s="113"/>
+      <c r="J42" s="113"/>
+      <c r="K42" s="112"/>
       <c r="L42" s="7"/>
       <c r="M42" s="5">
         <f>B2</f>
@@ -5893,10 +6054,10 @@
       </c>
     </row>
     <row r="43" spans="1:30">
-      <c r="B43" s="130"/>
-      <c r="C43" s="7">
+      <c r="B43" s="114"/>
+      <c r="C43" s="7" t="e">
         <f>M11</f>
-        <v>8.18</v>
+        <v>#VALUE!</v>
       </c>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
@@ -5905,7 +6066,7 @@
       <c r="H43" s="7"/>
       <c r="I43" s="7"/>
       <c r="J43" s="7"/>
-      <c r="K43" s="25"/>
+      <c r="K43" s="17"/>
       <c r="L43" s="7"/>
       <c r="M43" s="5">
         <f>B11</f>
@@ -5930,7 +6091,7 @@
       <c r="H44" s="6"/>
       <c r="I44" s="6"/>
       <c r="J44" s="6"/>
-      <c r="K44" s="24"/>
+      <c r="K44" s="16"/>
       <c r="L44" s="6"/>
       <c r="N44" s="6"/>
       <c r="AC44" s="2">
@@ -5950,7 +6111,7 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
-      <c r="K45" s="26"/>
+      <c r="K45" s="18"/>
       <c r="L45" s="1"/>
       <c r="M45" s="5"/>
       <c r="AC45" s="2">
@@ -5970,7 +6131,7 @@
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
-      <c r="K46" s="26"/>
+      <c r="K46" s="18"/>
       <c r="L46" s="1"/>
       <c r="M46" s="5"/>
       <c r="AC46" s="2">
@@ -6009,7 +6170,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
+    <mergeCell ref="A32:K32"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="C28:C29"/>
     <mergeCell ref="C30:C31"/>
@@ -6027,484 +6189,564 @@
     <mergeCell ref="A7:A9"/>
   </mergeCells>
   <conditionalFormatting sqref="I3:I10">
-    <cfRule type="cellIs" dxfId="117" priority="460" operator="lessThan">
+    <cfRule type="cellIs" dxfId="133" priority="476" operator="lessThan">
       <formula>$I$11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12:I16">
-    <cfRule type="cellIs" dxfId="116" priority="459" operator="lessThan">
+    <cfRule type="cellIs" dxfId="132" priority="475" operator="lessThan">
       <formula>$I$17</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I18:I24">
-    <cfRule type="cellIs" dxfId="115" priority="458" operator="lessThan">
+    <cfRule type="cellIs" dxfId="131" priority="474" operator="lessThan">
       <formula>$I$25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18:I24">
-    <cfRule type="cellIs" dxfId="114" priority="457" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="130" priority="473" operator="greaterThan">
       <formula>$I$25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:I16">
-    <cfRule type="cellIs" dxfId="113" priority="456" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="129" priority="472" operator="greaterThan">
       <formula>$I$17</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:I10 H4:H25">
-    <cfRule type="cellIs" dxfId="112" priority="455" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="128" priority="471" operator="greaterThan">
       <formula>$I$11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F11 H2:H11">
-    <cfRule type="expression" dxfId="111" priority="411">
+    <cfRule type="expression" dxfId="127" priority="427">
       <formula>NOT($C$11=" ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12:F17 H12:H17">
-    <cfRule type="expression" dxfId="110" priority="410">
+    <cfRule type="expression" dxfId="126" priority="426">
       <formula>NOT($C$17=" ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18:F25 H18:H25">
-    <cfRule type="expression" dxfId="109" priority="409">
+    <cfRule type="expression" dxfId="125" priority="425">
       <formula>NOT($C$25=" ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:A23">
-    <cfRule type="expression" dxfId="108" priority="392">
+    <cfRule type="expression" dxfId="124" priority="408">
       <formula>($A$18=" ")*($A$21=" ")*($B$1="№")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24">
-    <cfRule type="expression" dxfId="107" priority="391">
+    <cfRule type="expression" dxfId="123" priority="407">
       <formula>($A$18=" ")*($A$21=" ")*($B$1="№")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="expression" dxfId="106" priority="390">
+    <cfRule type="expression" dxfId="122" priority="406">
       <formula>($A$7=" ")*($A$4=" ")*($B$1="№")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:A6">
-    <cfRule type="expression" dxfId="105" priority="389">
+    <cfRule type="expression" dxfId="121" priority="405">
       <formula>($A$7=" ")*($A$4=" ")*($B$1="№")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="cellIs" dxfId="104" priority="368" operator="between">
+    <cfRule type="cellIs" dxfId="120" priority="384" operator="between">
       <formula>1350</formula>
       <formula>2000</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="103" priority="369" operator="between">
+    <cfRule type="cellIs" dxfId="119" priority="385" operator="between">
       <formula>562</formula>
       <formula>950</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="370" operator="lessThan">
+    <cfRule type="cellIs" dxfId="118" priority="386" operator="lessThan">
       <formula>458</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="794">
+    <cfRule type="expression" dxfId="117" priority="810">
       <formula>(($B$27=" ")+($B$26="Ползун")*(($B$27&gt;458)*($B$27&lt;562))+(($B$27&gt;950)*($B$27&lt;1350)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26:C26">
-    <cfRule type="expression" dxfId="100" priority="378">
+    <cfRule type="expression" dxfId="116" priority="394">
       <formula>($B$27=" ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:A16">
-    <cfRule type="expression" dxfId="99" priority="374">
+    <cfRule type="expression" dxfId="115" priority="390">
       <formula>($A$12=" ")</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="375" operator="lessThan">
+    <cfRule type="cellIs" dxfId="114" priority="391" operator="lessThan">
       <formula>8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="376" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="113" priority="392" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:C31">
-    <cfRule type="expression" dxfId="96" priority="373">
+    <cfRule type="expression" dxfId="112" priority="389">
       <formula>($B$28=" ")*($B$29=" ")*($B$30=" ")*($B$31=" ")*($B$1="№")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26:E27">
-    <cfRule type="expression" dxfId="95" priority="361">
+    <cfRule type="expression" dxfId="111" priority="377">
       <formula>($C$27=" ")*($B$1="№")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="expression" dxfId="94" priority="413">
+    <cfRule type="expression" dxfId="110" priority="429">
       <formula>(($B$28=" ")+($B$29=" "))*(($D$28=" ")+($D$29=" "))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="448" operator="lessThan">
+    <cfRule type="cellIs" dxfId="109" priority="464" operator="lessThan">
       <formula>7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="450" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="108" priority="466" operator="greaterThan">
       <formula>7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30">
-    <cfRule type="expression" dxfId="91" priority="412">
+    <cfRule type="expression" dxfId="107" priority="428">
       <formula>(($B$30=" ")+($B$31=" "))*(($D$30=" ")+($D$31=" "))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="447" operator="lessThan">
+    <cfRule type="cellIs" dxfId="106" priority="463" operator="lessThan">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="449" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="105" priority="465" operator="greaterThan">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="expression" dxfId="88" priority="383">
+    <cfRule type="expression" dxfId="104" priority="399">
       <formula>($C$27=" ")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="87" priority="207">
+    <cfRule type="expression" dxfId="103" priority="223">
       <formula>(C27&gt;585)*(C27&lt;590)+(C27&gt;530)*(C27&lt;535)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D25">
-    <cfRule type="expression" dxfId="86" priority="357">
+    <cfRule type="expression" dxfId="102" priority="373">
       <formula>NOT($B$30=" ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18:H25">
-    <cfRule type="expression" dxfId="85" priority="354">
+    <cfRule type="expression" dxfId="101" priority="370">
       <formula>"не($C$22="" "")"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27">
-    <cfRule type="expression" dxfId="84" priority="275">
+    <cfRule type="expression" dxfId="100" priority="291">
       <formula>NOT($D$27=" ")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="83" priority="385">
+    <cfRule type="expression" dxfId="99" priority="401">
       <formula>$D$27=" "</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12:J17">
-    <cfRule type="expression" dxfId="82" priority="554">
+    <cfRule type="expression" dxfId="98" priority="570">
       <formula>NOT($C$17=" ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J18:J25">
-    <cfRule type="expression" dxfId="81" priority="557">
+    <cfRule type="expression" dxfId="97" priority="573">
       <formula>NOT($C$25=" ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J11">
-    <cfRule type="expression" dxfId="80" priority="560">
+    <cfRule type="expression" dxfId="96" priority="576">
       <formula>NOT($C$11=" ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K10">
-    <cfRule type="expression" dxfId="79" priority="342">
+    <cfRule type="expression" dxfId="95" priority="358">
       <formula>$K$5="∆ОА="</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="343">
+    <cfRule type="expression" dxfId="94" priority="359">
       <formula>$K$5&lt;$K$11</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="77" priority="344">
+    <cfRule type="expression" dxfId="93" priority="360">
       <formula>$K$5&gt;$K$11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12:K16">
-    <cfRule type="expression" dxfId="76" priority="334">
+    <cfRule type="expression" dxfId="92" priority="350">
       <formula>($K$12&lt;2000)+($K$12="FAIL")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="339">
+    <cfRule type="expression" dxfId="91" priority="355">
       <formula>$K$12="∆АБ="</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="340" operator="lessThan">
+    <cfRule type="cellIs" dxfId="90" priority="356" operator="lessThan">
       <formula>$K$17</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="341" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="89" priority="357" operator="greaterThan">
       <formula>$K$17</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18:K24">
-    <cfRule type="expression" dxfId="72" priority="336">
+    <cfRule type="expression" dxfId="88" priority="352">
       <formula>$K$20="∆БВ="</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="71" priority="337">
+    <cfRule type="expression" dxfId="87" priority="353">
       <formula>$K$20&lt;$K$25</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="338">
+    <cfRule type="expression" dxfId="86" priority="354">
       <formula>$K$20&gt;$K$25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5:K7">
-    <cfRule type="expression" dxfId="69" priority="335">
+    <cfRule type="expression" dxfId="85" priority="351">
       <formula>($K$5&lt;2000)+($K$5="FAIL")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20:K22">
-    <cfRule type="expression" dxfId="68" priority="333">
+    <cfRule type="expression" dxfId="84" priority="349">
       <formula>($K$20&lt;2000)+($K$20="FAIL")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26">
-    <cfRule type="cellIs" dxfId="67" priority="363" operator="lessThan">
+    <cfRule type="cellIs" dxfId="83" priority="379" operator="lessThan">
       <formula>950</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="364" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="82" priority="380" operator="greaterThan">
       <formula>1350</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="65" priority="27">
+    <cfRule type="expression" dxfId="81" priority="43">
       <formula>($D$26=" ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:D27">
-    <cfRule type="cellIs" dxfId="64" priority="619" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="80" priority="635" operator="greaterThan">
       <formula>590</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="679" operator="lessThan">
+    <cfRule type="cellIs" dxfId="79" priority="695" operator="lessThan">
       <formula>530</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F17:K17 F25:K25 F11:K11 A11:D11 A25:D25 A17:D17 A2:D2 F2:K2 E2 E11 E17 E25">
-    <cfRule type="expression" dxfId="62" priority="236">
+    <cfRule type="expression" dxfId="78" priority="252">
       <formula>($K$5&lt;$K$11)*($K$12&lt;$K$17)*($K$20&lt;$K$25)*($B$11=94)*($B$17=142)*($B$25=236)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J9">
-    <cfRule type="cellIs" dxfId="61" priority="325" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="77" priority="341" operator="greaterThan">
       <formula>$K$11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12:J15">
-    <cfRule type="cellIs" dxfId="60" priority="324" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="76" priority="340" operator="greaterThan">
       <formula>$K$17</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J18:J24">
-    <cfRule type="cellIs" dxfId="59" priority="323" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="75" priority="339" operator="greaterThan">
       <formula>$K$25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F26:K31">
-    <cfRule type="expression" dxfId="58" priority="629">
+    <cfRule type="expression" dxfId="74" priority="645">
       <formula>($K$5&lt;$K$11)*($K$12&lt;$K$17)*($K$20&lt;$K$25)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28:E31">
-    <cfRule type="expression" dxfId="57" priority="260">
+    <cfRule type="expression" dxfId="73" priority="276">
       <formula>($B$1="№")*($B$28=" ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28:D29 E28">
-    <cfRule type="expression" dxfId="56" priority="261">
+    <cfRule type="expression" dxfId="72" priority="277">
       <formula>ABS($D$28-$D$29)&gt;7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30:D31 E29">
-    <cfRule type="expression" dxfId="55" priority="262">
+    <cfRule type="expression" dxfId="71" priority="278">
       <formula>ABS($D$30-$D$31)&gt;5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A27:E27">
-    <cfRule type="expression" dxfId="54" priority="384">
+    <cfRule type="expression" dxfId="70" priority="400">
       <formula>($K$5&lt;$K$11)*($K$12&lt;$K$17)*($K$20&lt;$K$25)*($B$11=94)*($B$17=142)*($B$25=236)*($C$27&lt;590)*($C$27&gt;530)*(($B$27&lt;1350)*($B$27&gt;950)+($B$27&lt;562)*($B$27&gt;458)+($B$27=" "))*(($C$28&lt;7)+($C$28=" "))*(($C$30&lt;5)+($C$30=" "))*(($A$12&lt;8)+($A$12=" "))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11">
-    <cfRule type="expression" dxfId="53" priority="795">
+    <cfRule type="expression" dxfId="69" priority="811">
       <formula>$A$11="А"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="796">
+    <cfRule type="expression" dxfId="68" priority="812">
       <formula>($K$5&gt;$K$11)+($K$12&gt;$K$17)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17">
-    <cfRule type="expression" dxfId="51" priority="797">
+    <cfRule type="expression" dxfId="67" priority="813">
       <formula>$A$17="Б"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="798">
+    <cfRule type="expression" dxfId="66" priority="814">
       <formula>($K$12&gt;$K$17)+($K$20&gt;$K$25)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="expression" dxfId="49" priority="799">
+    <cfRule type="expression" dxfId="65" priority="815">
       <formula>$A$25="В"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="800">
+    <cfRule type="expression" dxfId="64" priority="816">
       <formula>$K$20&gt;$K$25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="expression" dxfId="47" priority="804">
+    <cfRule type="expression" dxfId="63" priority="820">
       <formula>($J$2&lt;$K$2)*($J$11&lt;$K$11)*($J$15&lt;$K$15)*($B$10=94)*($B$14=142)*($B$22=236)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G11">
-    <cfRule type="expression" dxfId="46" priority="267">
+    <cfRule type="expression" dxfId="62" priority="283">
       <formula>NOT($B$28=" ")*NOT($C$11=" ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12:G17">
-    <cfRule type="expression" dxfId="45" priority="241">
+    <cfRule type="expression" dxfId="61" priority="257">
       <formula>NOT($B$28=" ")*NOT($C$17=" ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G18:G25">
-    <cfRule type="expression" dxfId="44" priority="240">
+    <cfRule type="expression" dxfId="60" priority="256">
       <formula>NOT($B$28=" ")*NOT($C$25=" ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="expression" dxfId="43" priority="234">
+    <cfRule type="expression" dxfId="59" priority="250">
       <formula>($K$5&lt;$K$11)*($K$12&lt;$K$17)*($K$20&lt;$K$25)*($B$11=94)*($B$17=142)*($B$25=236)*($E$2=0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="230">
+    <cfRule type="expression" dxfId="58" priority="246">
       <formula>NOT($E$2=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="expression" dxfId="41" priority="233">
+    <cfRule type="expression" dxfId="57" priority="249">
       <formula>($K$5&lt;$K$11)*($K$12&lt;$K$17)*($K$20&lt;$K$25)*($B$11=94)*($B$17=142)*($B$25=236)*($E$11=0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="221">
+    <cfRule type="expression" dxfId="56" priority="237">
       <formula>NOT($E$11=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17">
-    <cfRule type="expression" dxfId="39" priority="232">
+    <cfRule type="expression" dxfId="55" priority="248">
       <formula>($K$5&lt;$K$11)*($K$12&lt;$K$17)*($K$20&lt;$K$25)*($B$11=94)*($B$17=142)*($B$25=236)*($E$17=0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="217">
+    <cfRule type="expression" dxfId="54" priority="233">
       <formula>NOT($E$17=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25">
-    <cfRule type="expression" dxfId="37" priority="231">
+    <cfRule type="expression" dxfId="53" priority="247">
       <formula>($K$5&lt;$K$11)*($K$12&lt;$K$17)*($K$20&lt;$K$25)*($B$11=94)*($B$17=142)*($B$25=236)*($E$25=0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="209">
+    <cfRule type="expression" dxfId="52" priority="225">
       <formula>NOT($E$25=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="expression" dxfId="35" priority="229">
+    <cfRule type="expression" dxfId="51" priority="245">
       <formula>NOT($E$3=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="expression" dxfId="34" priority="228">
+    <cfRule type="expression" dxfId="50" priority="244">
       <formula>NOT($E$4=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="expression" dxfId="33" priority="227">
+    <cfRule type="expression" dxfId="49" priority="243">
       <formula>NOT($E$5=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="expression" dxfId="32" priority="226">
+    <cfRule type="expression" dxfId="48" priority="242">
       <formula>NOT($E$6=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="expression" dxfId="31" priority="225">
+    <cfRule type="expression" dxfId="47" priority="241">
       <formula>NOT($E$7=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="expression" dxfId="30" priority="224">
+    <cfRule type="expression" dxfId="46" priority="240">
       <formula>NOT($E$8=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="expression" dxfId="29" priority="222">
+    <cfRule type="expression" dxfId="45" priority="238">
       <formula>NOT($E$9=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="expression" dxfId="28" priority="220">
+    <cfRule type="expression" dxfId="44" priority="236">
       <formula>NOT($E$12=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="expression" dxfId="27" priority="219">
+    <cfRule type="expression" dxfId="43" priority="235">
       <formula>NOT($E$14=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="expression" dxfId="26" priority="218">
+    <cfRule type="expression" dxfId="42" priority="234">
       <formula>NOT($E$15=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18">
-    <cfRule type="expression" dxfId="25" priority="216">
+    <cfRule type="expression" dxfId="41" priority="232">
       <formula>NOT($E$18=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19">
-    <cfRule type="expression" dxfId="24" priority="215">
+    <cfRule type="expression" dxfId="40" priority="231">
       <formula>NOT($E$19=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20">
-    <cfRule type="expression" dxfId="23" priority="214">
+    <cfRule type="expression" dxfId="39" priority="230">
       <formula>NOT($E$20=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="expression" dxfId="22" priority="213">
+    <cfRule type="expression" dxfId="38" priority="229">
       <formula>NOT($E$21=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="expression" dxfId="21" priority="212">
+    <cfRule type="expression" dxfId="37" priority="228">
       <formula>NOT($E$22=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="expression" dxfId="20" priority="211">
+    <cfRule type="expression" dxfId="36" priority="227">
       <formula>NOT($E$23=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="expression" dxfId="19" priority="210">
+    <cfRule type="expression" dxfId="35" priority="226">
       <formula>NOT($E$24=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26 D26">
-    <cfRule type="expression" dxfId="18" priority="208">
+    <cfRule type="expression" dxfId="34" priority="224">
       <formula>($B$1="R")+NOT($D$27=" ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="expression" dxfId="17" priority="205">
+    <cfRule type="expression" dxfId="33" priority="221">
       <formula>NOT($A$1=" ")+(C27&gt;585)*(C27&lt;590)+(C27&gt;530)*(C27&lt;535)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26">
-    <cfRule type="expression" dxfId="16" priority="204">
+    <cfRule type="expression" dxfId="32" priority="220">
       <formula>(NOT($A$26=" "))*($A$26&gt;1.2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30">
-    <cfRule type="expression" dxfId="15" priority="349">
+    <cfRule type="expression" dxfId="31" priority="365">
       <formula>($B$1="R")*NOT($A$7=" ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
+    <cfRule type="expression" dxfId="30" priority="31">
+      <formula>($C$6&gt;2000)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7">
+    <cfRule type="expression" dxfId="29" priority="30">
+      <formula>($C$7&gt;2000)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="expression" dxfId="28" priority="29">
+      <formula>($C$8&gt;2000)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31">
+    <cfRule type="expression" dxfId="27" priority="28">
+      <formula>($B$1="R")*NOT($A$18=" ")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7">
+    <cfRule type="expression" dxfId="26" priority="27">
+      <formula>"(($H$2&lt;0.4)*($H$11&lt;0.6)*($H$15&lt;0.4))"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2">
+    <cfRule type="expression" dxfId="25" priority="26">
+      <formula>($K$5&lt;$K$11)*($K$12&lt;$K$17)*($K$20&lt;$K$25)*($B$11=94)*($B$17=142)*($B$25=236)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2">
+    <cfRule type="expression" dxfId="24" priority="25">
+      <formula>($J$2&lt;$K$2)*($J$11&lt;$K$11)*($J$15&lt;$K$15)*($B$10=94)*($B$14=142)*($B$22=236)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7">
+    <cfRule type="expression" dxfId="23" priority="24">
+      <formula>"(($H$2&lt;0.4)*($H$11&lt;0.6)*($H$15&lt;0.4))"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7">
+    <cfRule type="expression" dxfId="22" priority="23">
+      <formula>"(($H$2&lt;0.4)*($H$11&lt;0.6)*($H$15&lt;0.4))"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7">
+    <cfRule type="expression" dxfId="21" priority="22">
+      <formula>"(($H$2&lt;0.4)*($H$11&lt;0.6)*($H$15&lt;0.4))"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2">
+    <cfRule type="expression" dxfId="20" priority="21">
+      <formula>($K$2&lt;$L$2)*($K$11&lt;$L$11)*($K$15&lt;$L$15)*($B$10=94)*($B$14=142)*($B$22=236)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7">
+    <cfRule type="expression" dxfId="19" priority="20">
+      <formula>"(($H$2&lt;0.4)*($H$11&lt;0.6)*($H$15&lt;0.4))"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7">
+    <cfRule type="expression" dxfId="18" priority="19">
+      <formula>"(($H$2&lt;0.4)*($H$11&lt;0.6)*($H$15&lt;0.4))"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7">
+    <cfRule type="expression" dxfId="17" priority="18">
+      <formula>"(($H$2&lt;0.4)*($H$11&lt;0.6)*($H$15&lt;0.4))"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2">
+    <cfRule type="expression" dxfId="16" priority="17">
+      <formula>($K$2&lt;$L$2)*($K$11&lt;$L$11)*($K$15&lt;$L$15)*($B$10=94)*($B$14=142)*($B$22=236)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11 C25 C17 C2">
+    <cfRule type="expression" dxfId="15" priority="16">
+      <formula>($K$5&lt;$K$11)*($K$12&lt;$K$17)*($K$20&lt;$K$25)*($B$11=94)*($B$17=142)*($B$25=236)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2">
     <cfRule type="expression" dxfId="14" priority="15">
+      <formula>($J$2&lt;$K$2)*($J$11&lt;$K$11)*($J$15&lt;$K$15)*($B$10=94)*($B$14=142)*($B$22=236)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6">
+    <cfRule type="expression" dxfId="13" priority="14">
       <formula>($C$6&gt;2000)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="expression" dxfId="13" priority="14">
+    <cfRule type="expression" dxfId="12" priority="13">
       <formula>($C$7&gt;2000)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="expression" dxfId="12" priority="13">
+    <cfRule type="expression" dxfId="11" priority="12">
       <formula>($C$8&gt;2000)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E31">
-    <cfRule type="expression" dxfId="11" priority="12">
-      <formula>($B$1="R")*NOT($A$18=" ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">

</xml_diff>